<commit_message>
Improve indication and interventions
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/full_1.xlsx
+++ b/tests/integration_test_files/full_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B30078-298C-2444-A574-D583D93B717B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865802FE-BEE0-2649-A169-8C326FC9F7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8720" yWindow="500" windowWidth="56760" windowHeight="20140" activeTab="12" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="23320" yWindow="2420" windowWidth="56760" windowHeight="20140" activeTab="10" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -242,12 +242,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>IND</t>
-  </si>
-  <si>
-    <t>INT</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -497,13 +491,7 @@
     <t>Something else</t>
   </si>
   <si>
-    <t>Bad stuff</t>
-  </si>
-  <si>
     <t>IC Event Description Number 2</t>
-  </si>
-  <si>
-    <t>Really really bad shit</t>
   </si>
   <si>
     <t>Clinical Study Sponsor</t>
@@ -1906,6 +1894,18 @@
   </si>
   <si>
     <t>objectiveName</t>
+  </si>
+  <si>
+    <t>Something else bad</t>
+  </si>
+  <si>
+    <t>Something  Else</t>
+  </si>
+  <si>
+    <t>Indication</t>
+  </si>
+  <si>
+    <t>Intervention</t>
   </si>
 </sst>
 </file>
@@ -1989,7 +1989,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2016,10 +2016,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2076,6 +2072,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2403,21 +2402,21 @@
     <col min="2" max="2" width="27.5" customWidth="1"/>
     <col min="3" max="3" width="29.6640625" customWidth="1"/>
     <col min="4" max="4" width="18.1640625" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" style="25" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" style="25" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" style="23" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" style="23" customWidth="1"/>
     <col min="7" max="7" width="47.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>461</v>
+      <c r="A1" s="16" t="s">
+        <v>457</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="16" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -2425,15 +2424,15 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="11" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="16" t="s">
         <v>28</v>
       </c>
       <c r="B4" s="10" t="s">
@@ -2441,7 +2440,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="16" t="s">
         <v>29</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -2449,167 +2448,167 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="B6" s="10" t="s">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="16" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="B7" s="10" t="s">
+      <c r="B9" s="10" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="16" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="s">
+      <c r="B10" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B11" s="10" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="18" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B12" s="10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="18" t="s">
-        <v>127</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="18" t="s">
-        <v>128</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="18" t="s">
-        <v>533</v>
-      </c>
-      <c r="B16" s="18" t="s">
-        <v>461</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>534</v>
-      </c>
-      <c r="E16" s="21" t="s">
+      <c r="A16" s="16" t="s">
+        <v>529</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>457</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>530</v>
+      </c>
+      <c r="E16" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="F16" s="21" t="s">
-        <v>535</v>
-      </c>
-      <c r="G16" s="18" t="s">
-        <v>547</v>
+      <c r="F16" s="19" t="s">
+        <v>531</v>
+      </c>
+      <c r="G16" s="16" t="s">
+        <v>543</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="C17" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="D17" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="E17" t="s">
-        <v>544</v>
-      </c>
-      <c r="F17" s="26">
+        <v>540</v>
+      </c>
+      <c r="F17" s="24">
         <v>44927</v>
       </c>
       <c r="G17" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
+        <v>537</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>533</v>
+      </c>
+      <c r="C18" t="s">
+        <v>538</v>
+      </c>
+      <c r="D18" t="s">
+        <v>539</v>
+      </c>
+      <c r="E18" t="s">
         <v>541</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>537</v>
-      </c>
-      <c r="C18" t="s">
-        <v>542</v>
-      </c>
-      <c r="D18" t="s">
-        <v>543</v>
-      </c>
-      <c r="E18" t="s">
-        <v>545</v>
-      </c>
-      <c r="F18" s="26">
+      <c r="F18" s="24">
         <v>44927</v>
       </c>
       <c r="G18" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
+        <v>537</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>533</v>
+      </c>
+      <c r="C19" t="s">
+        <v>538</v>
+      </c>
+      <c r="D19" t="s">
+        <v>539</v>
+      </c>
+      <c r="E19" t="s">
         <v>541</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>537</v>
-      </c>
-      <c r="C19" t="s">
-        <v>542</v>
-      </c>
-      <c r="D19" t="s">
-        <v>543</v>
-      </c>
-      <c r="E19" t="s">
-        <v>545</v>
-      </c>
-      <c r="F19" s="26">
+      <c r="F19" s="24">
         <v>44958</v>
       </c>
       <c r="G19" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
   </sheetData>
@@ -2635,17 +2634,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
-        <v>256</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>257</v>
-      </c>
-      <c r="C1" s="17" t="s">
-        <v>258</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>259</v>
+      <c r="A1" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>254</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2653,7 +2652,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2661,13 +2660,13 @@
         <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D3" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -2683,84 +2682,86 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E548DFC1-EB0E-374B-95D2-A04104B745FB}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="50.33203125" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="5" t="s">
+      <c r="A1" s="19" t="s">
+        <v>457</v>
+      </c>
+      <c r="B1" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>65</v>
+      <c r="C1" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>606</v>
       </c>
       <c r="C2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>606</v>
       </c>
       <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="D3" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>607</v>
       </c>
       <c r="C4" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>70</v>
+      <c r="D4" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>607</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2786,85 +2787,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
-        <v>461</v>
-      </c>
-      <c r="B1" s="21" t="s">
+      <c r="A1" s="19" t="s">
+        <v>457</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>77</v>
+      <c r="E1" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>75</v>
       </c>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="B2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="C2">
         <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" t="s">
         <v>76</v>
-      </c>
-      <c r="F2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="B3" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="C3">
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="B4" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="C4">
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2876,8 +2877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B908C5D6-C6A1-4043-A49A-69C599CFBAE9}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2896,117 +2897,117 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
-        <v>607</v>
-      </c>
-      <c r="B1" s="21" t="s">
+      <c r="A1" s="19" t="s">
+        <v>603</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>593</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>596</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>592</v>
+      </c>
+      <c r="G1" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="H1" s="19" t="s">
+        <v>594</v>
+      </c>
+      <c r="I1" s="19" t="s">
         <v>597</v>
       </c>
-      <c r="D1" s="21" t="s">
-        <v>600</v>
-      </c>
-      <c r="E1" s="21" t="s">
+      <c r="J1" s="19" t="s">
+        <v>595</v>
+      </c>
+      <c r="K1" s="19" t="s">
         <v>85</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>596</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="H1" s="21" t="s">
-        <v>598</v>
-      </c>
-      <c r="I1" s="21" t="s">
-        <v>601</v>
-      </c>
-      <c r="J1" s="21" t="s">
-        <v>599</v>
-      </c>
-      <c r="K1" s="21" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>601</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>605</v>
-      </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14" t="s">
+      <c r="G2" s="12" t="s">
+        <v>598</v>
+      </c>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="J2" s="10"/>
+      <c r="K2" s="12" t="s">
         <v>89</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>602</v>
-      </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="J2" s="10"/>
-      <c r="K2" s="14" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>602</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>606</v>
-      </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14" t="s">
+      <c r="G3" s="12" t="s">
+        <v>599</v>
+      </c>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>603</v>
-      </c>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14" t="s">
+      <c r="J3" s="10"/>
+      <c r="K3" s="12" t="s">
         <v>94</v>
-      </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="14" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>604</v>
-      </c>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14" t="s">
-        <v>95</v>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>600</v>
+      </c>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12" t="s">
+        <v>93</v>
       </c>
       <c r="J4" s="10"/>
-      <c r="K4" s="14" t="s">
-        <v>96</v>
+      <c r="K4" s="12" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -3285,105 +3286,121 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6.83203125" customWidth="1"/>
     <col min="2" max="2" width="22.5" customWidth="1"/>
-    <col min="3" max="4" width="23" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="28.1640625" customWidth="1"/>
-    <col min="6" max="7" width="17" customWidth="1"/>
-    <col min="8" max="8" width="61.83203125" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="8" max="8" width="35.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="31" t="s">
+        <v>457</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="C1" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>115</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="F1" s="12" t="s">
+      <c r="G2" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="10"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="G1" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B2" t="s">
-        <v>116</v>
-      </c>
-      <c r="C2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E2" t="s">
-        <v>118</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="D5" s="10" t="s">
+        <v>605</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="G2" t="s">
-        <v>105</v>
-      </c>
-      <c r="H2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>145</v>
-      </c>
-      <c r="B5" t="s">
-        <v>146</v>
-      </c>
-      <c r="C5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D5" t="s">
-        <v>147</v>
-      </c>
-      <c r="E5" t="s">
-        <v>148</v>
-      </c>
-      <c r="F5" t="s">
-        <v>101</v>
-      </c>
-      <c r="G5" t="s">
-        <v>106</v>
-      </c>
-      <c r="H5" t="s">
-        <v>149</v>
+      <c r="G5" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>604</v>
       </c>
     </row>
   </sheetData>
@@ -3412,65 +3429,65 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="C1" s="16" t="s">
-        <v>229</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>230</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="G1" s="16" t="s">
-        <v>164</v>
+        <v>95</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C2" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="D2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" t="s">
+        <v>228</v>
+      </c>
+      <c r="D3" t="s">
+        <v>230</v>
+      </c>
+      <c r="E3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="C3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D3" t="s">
-        <v>234</v>
-      </c>
-      <c r="E3" t="s">
-        <v>169</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>170</v>
-      </c>
       <c r="G3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -3502,138 +3519,138 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="21" t="s">
+      <c r="A1" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>171</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="F1" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="G1" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="H1" s="19" t="s">
         <v>175</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>176</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>177</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>178</v>
-      </c>
-      <c r="H1" s="21" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>186</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>185</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>186</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>185</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -3659,105 +3676,105 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>203</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>178</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>179</v>
+      <c r="A1" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>174</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>219</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>220</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -3783,1231 +3800,1231 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
-        <v>501</v>
-      </c>
-      <c r="B1" s="24" t="s">
-        <v>461</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>263</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>264</v>
+      <c r="A1" s="22" t="s">
+        <v>497</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>457</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>259</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="33" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="23"/>
+      <c r="B2" s="21"/>
       <c r="C2" s="9" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="113" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="13" t="s">
-        <v>529</v>
+      <c r="A10" s="11" t="s">
+        <v>525</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>395</v>
-      </c>
-      <c r="B13" s="23"/>
+        <v>391</v>
+      </c>
+      <c r="B13" s="21"/>
       <c r="C13" s="9" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>405</v>
-      </c>
-      <c r="B14" s="23"/>
+        <v>401</v>
+      </c>
+      <c r="B14" s="21"/>
       <c r="C14" s="9" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>406</v>
-      </c>
-      <c r="B15" s="23"/>
+        <v>402</v>
+      </c>
+      <c r="B15" s="21"/>
       <c r="C15" s="9" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>407</v>
-      </c>
-      <c r="B16" s="23"/>
+        <v>403</v>
+      </c>
+      <c r="B16" s="21"/>
       <c r="C16" s="9" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>408</v>
-      </c>
-      <c r="B17" s="23"/>
+        <v>404</v>
+      </c>
+      <c r="B17" s="21"/>
       <c r="C17" s="9" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>484</v>
-      </c>
-      <c r="B18" s="23"/>
+        <v>480</v>
+      </c>
+      <c r="B18" s="21"/>
       <c r="C18" s="9" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>485</v>
-      </c>
-      <c r="B19" s="23"/>
+        <v>481</v>
+      </c>
+      <c r="B19" s="21"/>
       <c r="C19" s="9" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>462</v>
-      </c>
-      <c r="B20" s="23"/>
+        <v>458</v>
+      </c>
+      <c r="B20" s="21"/>
       <c r="C20" s="9" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
-        <v>486</v>
-      </c>
-      <c r="B21" s="23"/>
+        <v>482</v>
+      </c>
+      <c r="B21" s="21"/>
       <c r="C21" s="9" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>487</v>
-      </c>
-      <c r="B22" s="23"/>
+        <v>483</v>
+      </c>
+      <c r="B22" s="21"/>
       <c r="C22" s="9" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>488</v>
-      </c>
-      <c r="B23" s="23"/>
+        <v>484</v>
+      </c>
+      <c r="B23" s="21"/>
       <c r="C23" s="9" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>489</v>
-      </c>
-      <c r="B24" s="23"/>
+        <v>485</v>
+      </c>
+      <c r="B24" s="21"/>
       <c r="C24" s="9" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>490</v>
-      </c>
-      <c r="B25" s="23"/>
+        <v>486</v>
+      </c>
+      <c r="B25" s="21"/>
       <c r="C25" s="9" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>451</v>
-      </c>
-      <c r="B26" s="23"/>
+        <v>447</v>
+      </c>
+      <c r="B26" s="21"/>
       <c r="C26" s="9" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
-        <v>452</v>
-      </c>
-      <c r="B27" s="23"/>
+        <v>448</v>
+      </c>
+      <c r="B27" s="21"/>
       <c r="C27" s="9" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
-        <v>453</v>
-      </c>
-      <c r="B28" s="23"/>
+        <v>449</v>
+      </c>
+      <c r="B28" s="21"/>
       <c r="C28" s="9" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
-        <v>454</v>
-      </c>
-      <c r="B29" s="23"/>
+        <v>450</v>
+      </c>
+      <c r="B29" s="21"/>
       <c r="C29" s="9" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
-        <v>491</v>
-      </c>
-      <c r="B30" s="23"/>
+        <v>487</v>
+      </c>
+      <c r="B30" s="21"/>
       <c r="C30" s="9" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
-        <v>463</v>
-      </c>
-      <c r="B31" s="23"/>
+        <v>459</v>
+      </c>
+      <c r="B31" s="21"/>
       <c r="C31" s="9" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
-        <v>492</v>
-      </c>
-      <c r="B32" s="23"/>
+        <v>488</v>
+      </c>
+      <c r="B32" s="21"/>
       <c r="C32" s="9" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
-        <v>493</v>
-      </c>
-      <c r="B33" s="23"/>
+        <v>489</v>
+      </c>
+      <c r="B33" s="21"/>
       <c r="C33" s="9" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
-        <v>494</v>
-      </c>
-      <c r="B34" s="23"/>
+        <v>490</v>
+      </c>
+      <c r="B34" s="21"/>
       <c r="C34" s="9" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
-        <v>409</v>
-      </c>
-      <c r="B35" s="23"/>
+        <v>405</v>
+      </c>
+      <c r="B35" s="21"/>
       <c r="C35" s="9" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
-        <v>495</v>
-      </c>
-      <c r="B36" s="23"/>
+        <v>491</v>
+      </c>
+      <c r="B36" s="21"/>
       <c r="C36" s="9" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
-        <v>496</v>
-      </c>
-      <c r="B37" s="23"/>
+        <v>492</v>
+      </c>
+      <c r="B37" s="21"/>
       <c r="C37" s="9" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
-        <v>410</v>
-      </c>
-      <c r="B38" s="23"/>
+        <v>406</v>
+      </c>
+      <c r="B38" s="21"/>
       <c r="C38" s="9" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
-        <v>411</v>
-      </c>
-      <c r="B39" s="23"/>
+        <v>407</v>
+      </c>
+      <c r="B39" s="21"/>
       <c r="C39" s="9" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
-        <v>412</v>
-      </c>
-      <c r="B40" s="23"/>
+        <v>408</v>
+      </c>
+      <c r="B40" s="21"/>
       <c r="C40" s="9" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
-        <v>497</v>
-      </c>
-      <c r="B41" s="23"/>
+        <v>493</v>
+      </c>
+      <c r="B41" s="21"/>
       <c r="C41" s="9" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
-        <v>413</v>
-      </c>
-      <c r="B42" s="23"/>
+        <v>409</v>
+      </c>
+      <c r="B42" s="21"/>
       <c r="C42" s="9" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
-        <v>414</v>
-      </c>
-      <c r="B43" s="23"/>
+        <v>410</v>
+      </c>
+      <c r="B43" s="21"/>
       <c r="C43" s="9" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
-        <v>415</v>
-      </c>
-      <c r="B44" s="23"/>
+        <v>411</v>
+      </c>
+      <c r="B44" s="21"/>
       <c r="C44" s="9" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
-        <v>498</v>
-      </c>
-      <c r="B45" s="23"/>
+        <v>494</v>
+      </c>
+      <c r="B45" s="21"/>
       <c r="C45" s="9" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
-        <v>499</v>
-      </c>
-      <c r="B46" s="23"/>
+        <v>495</v>
+      </c>
+      <c r="B46" s="21"/>
       <c r="C46" s="9" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
-        <v>416</v>
-      </c>
-      <c r="B47" s="23"/>
+        <v>412</v>
+      </c>
+      <c r="B47" s="21"/>
       <c r="C47" s="9" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
-        <v>417</v>
-      </c>
-      <c r="B48" s="23"/>
+        <v>413</v>
+      </c>
+      <c r="B48" s="21"/>
       <c r="C48" s="9" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
-        <v>418</v>
-      </c>
-      <c r="B49" s="23"/>
+        <v>414</v>
+      </c>
+      <c r="B49" s="21"/>
       <c r="C49" s="9" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
-        <v>419</v>
-      </c>
-      <c r="B50" s="23"/>
+        <v>415</v>
+      </c>
+      <c r="B50" s="21"/>
       <c r="C50" s="9" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="10" t="s">
-        <v>464</v>
-      </c>
-      <c r="B51" s="23"/>
+        <v>460</v>
+      </c>
+      <c r="B51" s="21"/>
       <c r="C51" s="9" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
-        <v>500</v>
-      </c>
-      <c r="B52" s="23"/>
+        <v>496</v>
+      </c>
+      <c r="B52" s="21"/>
       <c r="C52" s="9" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="10" t="s">
-        <v>420</v>
-      </c>
-      <c r="B53" s="23"/>
+        <v>416</v>
+      </c>
+      <c r="B53" s="21"/>
       <c r="C53" s="9" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
-        <v>421</v>
-      </c>
-      <c r="B54" s="23"/>
+        <v>417</v>
+      </c>
+      <c r="B54" s="21"/>
       <c r="C54" s="9" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
-        <v>422</v>
-      </c>
-      <c r="B55" s="23"/>
+        <v>418</v>
+      </c>
+      <c r="B55" s="21"/>
       <c r="C55" s="9" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
-        <v>502</v>
-      </c>
-      <c r="B56" s="23"/>
+        <v>498</v>
+      </c>
+      <c r="B56" s="21"/>
       <c r="C56" s="9" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
-        <v>503</v>
-      </c>
-      <c r="B57" s="23"/>
+        <v>499</v>
+      </c>
+      <c r="B57" s="21"/>
       <c r="C57" s="9" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
-        <v>504</v>
-      </c>
-      <c r="B58" s="23"/>
+        <v>500</v>
+      </c>
+      <c r="B58" s="21"/>
       <c r="C58" s="9" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
-        <v>465</v>
-      </c>
-      <c r="B59" s="23"/>
+        <v>461</v>
+      </c>
+      <c r="B59" s="21"/>
       <c r="C59" s="9" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="10" t="s">
-        <v>505</v>
-      </c>
-      <c r="B60" s="23"/>
+        <v>501</v>
+      </c>
+      <c r="B60" s="21"/>
       <c r="C60" s="9" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="10" t="s">
-        <v>506</v>
-      </c>
-      <c r="B61" s="23"/>
+        <v>502</v>
+      </c>
+      <c r="B61" s="21"/>
       <c r="C61" s="9" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="10" t="s">
-        <v>507</v>
-      </c>
-      <c r="B62" s="23"/>
+        <v>503</v>
+      </c>
+      <c r="B62" s="21"/>
       <c r="C62" s="9" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="10" t="s">
-        <v>455</v>
-      </c>
-      <c r="B63" s="23"/>
+        <v>451</v>
+      </c>
+      <c r="B63" s="21"/>
       <c r="C63" s="9" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="10" t="s">
-        <v>423</v>
-      </c>
-      <c r="B64" s="23"/>
+        <v>419</v>
+      </c>
+      <c r="B64" s="21"/>
       <c r="C64" s="9" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="10" t="s">
-        <v>424</v>
-      </c>
-      <c r="B65" s="23"/>
+        <v>420</v>
+      </c>
+      <c r="B65" s="21"/>
       <c r="C65" s="9" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="10" t="s">
-        <v>425</v>
-      </c>
-      <c r="B66" s="23"/>
+        <v>421</v>
+      </c>
+      <c r="B66" s="21"/>
       <c r="C66" s="9" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="10" t="s">
-        <v>426</v>
-      </c>
-      <c r="B67" s="23"/>
+        <v>422</v>
+      </c>
+      <c r="B67" s="21"/>
       <c r="C67" s="9" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="10" t="s">
-        <v>508</v>
-      </c>
-      <c r="B68" s="23"/>
+        <v>504</v>
+      </c>
+      <c r="B68" s="21"/>
       <c r="C68" s="9" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="10" t="s">
-        <v>456</v>
-      </c>
-      <c r="B69" s="23"/>
+        <v>452</v>
+      </c>
+      <c r="B69" s="21"/>
       <c r="C69" s="9" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A70" s="10" t="s">
-        <v>427</v>
-      </c>
-      <c r="B70" s="23"/>
+        <v>423</v>
+      </c>
+      <c r="B70" s="21"/>
       <c r="C70" s="9" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="10" t="s">
-        <v>428</v>
-      </c>
-      <c r="B71" s="23"/>
+        <v>424</v>
+      </c>
+      <c r="B71" s="21"/>
       <c r="C71" s="9" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="10" t="s">
-        <v>429</v>
-      </c>
-      <c r="B72" s="23"/>
+        <v>425</v>
+      </c>
+      <c r="B72" s="21"/>
       <c r="C72" s="9" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="10" t="s">
-        <v>430</v>
-      </c>
-      <c r="B73" s="23"/>
+        <v>426</v>
+      </c>
+      <c r="B73" s="21"/>
       <c r="C73" s="9" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="10" t="s">
-        <v>431</v>
-      </c>
-      <c r="B74" s="23"/>
+        <v>427</v>
+      </c>
+      <c r="B74" s="21"/>
       <c r="C74" s="9" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="10" t="s">
-        <v>432</v>
-      </c>
-      <c r="B75" s="23"/>
+        <v>428</v>
+      </c>
+      <c r="B75" s="21"/>
       <c r="C75" s="9" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="10" t="s">
-        <v>433</v>
-      </c>
-      <c r="B76" s="23"/>
+        <v>429</v>
+      </c>
+      <c r="B76" s="21"/>
       <c r="C76" s="9" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="10" t="s">
-        <v>434</v>
-      </c>
-      <c r="B77" s="23"/>
+        <v>430</v>
+      </c>
+      <c r="B77" s="21"/>
       <c r="C77" s="9" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A78" s="10" t="s">
-        <v>435</v>
-      </c>
-      <c r="B78" s="23"/>
+        <v>431</v>
+      </c>
+      <c r="B78" s="21"/>
       <c r="C78" s="9" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="10" t="s">
-        <v>509</v>
-      </c>
-      <c r="B79" s="23"/>
+        <v>505</v>
+      </c>
+      <c r="B79" s="21"/>
       <c r="C79" s="9" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="10" t="s">
-        <v>436</v>
-      </c>
-      <c r="B80" s="23"/>
+        <v>432</v>
+      </c>
+      <c r="B80" s="21"/>
       <c r="C80" s="9" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="10" t="s">
-        <v>437</v>
-      </c>
-      <c r="B81" s="23"/>
+        <v>433</v>
+      </c>
+      <c r="B81" s="21"/>
       <c r="C81" s="9" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A82" s="10" t="s">
-        <v>510</v>
-      </c>
-      <c r="B82" s="23"/>
+        <v>506</v>
+      </c>
+      <c r="B82" s="21"/>
       <c r="C82" s="9" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="10" t="s">
-        <v>438</v>
-      </c>
-      <c r="B83" s="23"/>
+        <v>434</v>
+      </c>
+      <c r="B83" s="21"/>
       <c r="C83" s="9" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="10" t="s">
-        <v>439</v>
-      </c>
-      <c r="B84" s="23"/>
+        <v>435</v>
+      </c>
+      <c r="B84" s="21"/>
       <c r="C84" s="9" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A85" s="10" t="s">
-        <v>440</v>
-      </c>
-      <c r="B85" s="23"/>
+        <v>436</v>
+      </c>
+      <c r="B85" s="21"/>
       <c r="C85" s="9" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="10" t="s">
-        <v>441</v>
-      </c>
-      <c r="B86" s="23"/>
+        <v>437</v>
+      </c>
+      <c r="B86" s="21"/>
       <c r="C86" s="9" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" s="10" t="s">
-        <v>442</v>
-      </c>
-      <c r="B87" s="23"/>
+        <v>438</v>
+      </c>
+      <c r="B87" s="21"/>
       <c r="C87" s="9" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="10" t="s">
-        <v>511</v>
-      </c>
-      <c r="B88" s="23"/>
+        <v>507</v>
+      </c>
+      <c r="B88" s="21"/>
       <c r="C88" s="9" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="10" t="s">
-        <v>512</v>
-      </c>
-      <c r="B89" s="23"/>
+        <v>508</v>
+      </c>
+      <c r="B89" s="21"/>
       <c r="C89" s="9" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="10" t="s">
-        <v>513</v>
-      </c>
-      <c r="B90" s="23"/>
+        <v>509</v>
+      </c>
+      <c r="B90" s="21"/>
       <c r="C90" s="9" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="10" t="s">
-        <v>505</v>
-      </c>
-      <c r="B91" s="23"/>
+        <v>501</v>
+      </c>
+      <c r="B91" s="21"/>
       <c r="C91" s="9" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="10" t="s">
-        <v>457</v>
-      </c>
-      <c r="B92" s="23"/>
+        <v>453</v>
+      </c>
+      <c r="B92" s="21"/>
       <c r="C92" s="9" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="10" t="s">
-        <v>466</v>
-      </c>
-      <c r="B93" s="23"/>
+        <v>462</v>
+      </c>
+      <c r="B93" s="21"/>
       <c r="C93" s="9" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="10" t="s">
-        <v>514</v>
-      </c>
-      <c r="B94" s="23"/>
+        <v>510</v>
+      </c>
+      <c r="B94" s="21"/>
       <c r="C94" s="9" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="10" t="s">
-        <v>515</v>
-      </c>
-      <c r="B95" s="23"/>
+        <v>511</v>
+      </c>
+      <c r="B95" s="21"/>
       <c r="C95" s="9" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="10" t="s">
-        <v>443</v>
-      </c>
-      <c r="B96" s="23"/>
+        <v>439</v>
+      </c>
+      <c r="B96" s="21"/>
       <c r="C96" s="9" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="10" t="s">
-        <v>444</v>
-      </c>
-      <c r="B97" s="23"/>
+        <v>440</v>
+      </c>
+      <c r="B97" s="21"/>
       <c r="C97" s="9" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="10" t="s">
-        <v>445</v>
-      </c>
-      <c r="B98" s="23"/>
+        <v>441</v>
+      </c>
+      <c r="B98" s="21"/>
       <c r="C98" s="9" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="10" t="s">
-        <v>446</v>
-      </c>
-      <c r="B99" s="23"/>
+        <v>442</v>
+      </c>
+      <c r="B99" s="21"/>
       <c r="C99" s="9" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="B100" s="23"/>
+        <v>443</v>
+      </c>
+      <c r="B100" s="21"/>
       <c r="C100" s="9" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="10" t="s">
-        <v>516</v>
-      </c>
-      <c r="B101" s="23"/>
+        <v>512</v>
+      </c>
+      <c r="B101" s="21"/>
       <c r="C101" s="9" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="10" t="s">
-        <v>517</v>
-      </c>
-      <c r="B102" s="23"/>
+        <v>513</v>
+      </c>
+      <c r="B102" s="21"/>
       <c r="C102" s="9" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="10" t="s">
-        <v>518</v>
-      </c>
-      <c r="B103" s="23"/>
+        <v>514</v>
+      </c>
+      <c r="B103" s="21"/>
       <c r="C103" s="9" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="10" t="s">
-        <v>519</v>
-      </c>
-      <c r="B104" s="23"/>
+        <v>515</v>
+      </c>
+      <c r="B104" s="21"/>
       <c r="C104" s="9" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="10" t="s">
-        <v>520</v>
-      </c>
-      <c r="B105" s="23"/>
+        <v>516</v>
+      </c>
+      <c r="B105" s="21"/>
       <c r="C105" s="9" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="10" t="s">
-        <v>521</v>
-      </c>
-      <c r="B106" s="23"/>
+        <v>517</v>
+      </c>
+      <c r="B106" s="21"/>
       <c r="C106" s="9" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="10" t="s">
-        <v>522</v>
-      </c>
-      <c r="B107" s="23"/>
+        <v>518</v>
+      </c>
+      <c r="B107" s="21"/>
       <c r="C107" s="9" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A108" s="10" t="s">
-        <v>467</v>
-      </c>
-      <c r="B108" s="23"/>
+        <v>463</v>
+      </c>
+      <c r="B108" s="21"/>
       <c r="C108" s="9" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="10" t="s">
-        <v>523</v>
-      </c>
-      <c r="B109" s="23"/>
+        <v>519</v>
+      </c>
+      <c r="B109" s="21"/>
       <c r="C109" s="9" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="10" t="s">
-        <v>524</v>
-      </c>
-      <c r="B110" s="23"/>
+        <v>520</v>
+      </c>
+      <c r="B110" s="21"/>
       <c r="C110" s="9" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="10" t="s">
-        <v>525</v>
-      </c>
-      <c r="B111" s="23"/>
+        <v>521</v>
+      </c>
+      <c r="B111" s="21"/>
       <c r="C111" s="9" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="10" t="s">
-        <v>526</v>
-      </c>
-      <c r="B112" s="23"/>
+        <v>522</v>
+      </c>
+      <c r="B112" s="21"/>
       <c r="C112" s="9" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="10" t="s">
-        <v>527</v>
-      </c>
-      <c r="B113" s="23"/>
+        <v>523</v>
+      </c>
+      <c r="B113" s="21"/>
       <c r="C113" s="9" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A114" s="10" t="s">
-        <v>468</v>
-      </c>
-      <c r="B114" s="23"/>
+        <v>464</v>
+      </c>
+      <c r="B114" s="21"/>
       <c r="C114" s="9" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="10" t="s">
-        <v>483</v>
-      </c>
-      <c r="B115" s="23"/>
+        <v>479</v>
+      </c>
+      <c r="B115" s="21"/>
       <c r="C115" s="9" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="10" t="s">
-        <v>482</v>
-      </c>
-      <c r="B116" s="23"/>
+        <v>478</v>
+      </c>
+      <c r="B116" s="21"/>
       <c r="C116" s="9" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="10" t="s">
-        <v>481</v>
-      </c>
-      <c r="B117" s="23"/>
+        <v>477</v>
+      </c>
+      <c r="B117" s="21"/>
       <c r="C117" s="9" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A118" s="10" t="s">
-        <v>469</v>
-      </c>
-      <c r="B118" s="23"/>
+        <v>465</v>
+      </c>
+      <c r="B118" s="21"/>
       <c r="C118" s="9" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="10" t="s">
-        <v>480</v>
-      </c>
-      <c r="B119" s="23"/>
+        <v>476</v>
+      </c>
+      <c r="B119" s="21"/>
       <c r="C119" s="9" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="10" t="s">
-        <v>479</v>
-      </c>
-      <c r="B120" s="23"/>
+        <v>475</v>
+      </c>
+      <c r="B120" s="21"/>
       <c r="C120" s="9" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="10" t="s">
-        <v>478</v>
-      </c>
-      <c r="B121" s="23"/>
+        <v>474</v>
+      </c>
+      <c r="B121" s="21"/>
       <c r="C121" s="9" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="10" t="s">
-        <v>477</v>
-      </c>
-      <c r="B122" s="23"/>
+        <v>473</v>
+      </c>
+      <c r="B122" s="21"/>
       <c r="C122" s="9" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A123" s="10" t="s">
-        <v>470</v>
-      </c>
-      <c r="B123" s="23"/>
+        <v>466</v>
+      </c>
+      <c r="B123" s="21"/>
       <c r="C123" s="9" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="10" t="s">
-        <v>476</v>
-      </c>
-      <c r="B124" s="23"/>
+        <v>472</v>
+      </c>
+      <c r="B124" s="21"/>
       <c r="C124" s="9" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="10" t="s">
-        <v>448</v>
-      </c>
-      <c r="B125" s="23"/>
+        <v>444</v>
+      </c>
+      <c r="B125" s="21"/>
       <c r="C125" s="9" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="10" t="s">
-        <v>449</v>
-      </c>
-      <c r="B126" s="23"/>
+        <v>445</v>
+      </c>
+      <c r="B126" s="21"/>
       <c r="C126" s="9" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="10" t="s">
-        <v>450</v>
-      </c>
-      <c r="B127" s="23"/>
+        <v>446</v>
+      </c>
+      <c r="B127" s="21"/>
       <c r="C127" s="9" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="10" t="s">
-        <v>475</v>
-      </c>
-      <c r="B128" s="23"/>
+        <v>471</v>
+      </c>
+      <c r="B128" s="21"/>
       <c r="C128" s="9" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="10" t="s">
-        <v>474</v>
-      </c>
-      <c r="B129" s="23"/>
+        <v>470</v>
+      </c>
+      <c r="B129" s="21"/>
       <c r="C129" s="9" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="10" t="s">
-        <v>473</v>
-      </c>
-      <c r="B130" s="23"/>
+        <v>469</v>
+      </c>
+      <c r="B130" s="21"/>
       <c r="C130" s="9" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="10" t="s">
-        <v>471</v>
-      </c>
-      <c r="B131" s="23"/>
+        <v>467</v>
+      </c>
+      <c r="B131" s="21"/>
       <c r="C131" s="9" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="10" t="s">
-        <v>472</v>
-      </c>
-      <c r="B132" s="23"/>
+        <v>468</v>
+      </c>
+      <c r="B132" s="21"/>
       <c r="C132" s="9" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="10" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="10" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="10" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="10" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="10" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="10" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
     </row>
   </sheetData>
@@ -5031,18 +5048,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" t="s">
         <v>140</v>
-      </c>
-      <c r="B1" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -5069,23 +5086,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="25" t="s">
+        <v>544</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>545</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>546</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>547</v>
+      </c>
+      <c r="E1" s="16" t="s">
         <v>548</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>549</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>550</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>551</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>552</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>561</v>
+      <c r="F1" s="26" t="s">
+        <v>557</v>
       </c>
       <c r="G1" s="10"/>
     </row>
@@ -5094,17 +5111,17 @@
         <v>4</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="G2" s="10"/>
     </row>
@@ -5112,18 +5129,18 @@
       <c r="A3" s="2">
         <v>3</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="11" t="s">
+        <v>549</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>553</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>170</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>557</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="10" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="G3" s="10"/>
     </row>
@@ -5132,19 +5149,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="G4" s="10"/>
     </row>
@@ -5153,17 +5170,17 @@
         <v>1</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="10" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="G5" s="10"/>
     </row>
@@ -5190,22 +5207,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="18" t="s">
         <v>57</v>
       </c>
     </row>
@@ -5220,7 +5237,7 @@
         <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E2" t="s">
         <v>39</v>
@@ -5240,7 +5257,7 @@
         <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E3" t="s">
         <v>55</v>
@@ -5270,116 +5287,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
-        <v>227</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>226</v>
-      </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
+      <c r="A1" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
-        <v>228</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>225</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
+      <c r="A2" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="30" t="s">
-        <v>152</v>
-      </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
+      <c r="B3" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="31" t="s">
-        <v>172</v>
-      </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
+      <c r="B4" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B7" s="29" t="s">
-        <v>139</v>
-      </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="29" t="s">
-        <v>138</v>
-      </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="B9" s="29" t="s">
-        <v>153</v>
-      </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
+      <c r="A9" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="27"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
+      <c r="A10" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="s">
-        <v>200</v>
+      <c r="A12" s="13" t="s">
+        <v>196</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>43</v>
@@ -5399,16 +5416,16 @@
         <v>41</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -5416,16 +5433,16 @@
         <v>42</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -5473,20 +5490,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>243</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="E1" s="19" t="s">
         <v>246</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>247</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>248</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>249</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -5494,16 +5511,16 @@
         <v>41</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -5514,13 +5531,13 @@
         <v>42</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -5550,66 +5567,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
-        <v>533</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>569</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>461</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>534</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>264</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>570</v>
+      <c r="A1" s="19" t="s">
+        <v>529</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>565</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>457</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>530</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>566</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>577</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>578</v>
+      </c>
+      <c r="C2" t="s">
+        <v>579</v>
+      </c>
+      <c r="D2" t="s">
+        <v>580</v>
+      </c>
+      <c r="F2" t="s">
         <v>581</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>582</v>
-      </c>
-      <c r="C2" t="s">
-        <v>583</v>
-      </c>
-      <c r="D2" t="s">
-        <v>584</v>
-      </c>
-      <c r="F2" t="s">
-        <v>585</v>
-      </c>
       <c r="G2" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="C3" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="D3" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="F3" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="G3" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
     </row>
   </sheetData>
@@ -5621,9 +5638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EB40753-8F7D-3941-9F21-F336F33F75CC}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5635,63 +5650,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
-        <v>461</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>64</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>534</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>571</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>572</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>573</v>
+      <c r="A1" s="19" t="s">
+        <v>457</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>530</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>567</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>568</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>569</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>570</v>
+      </c>
+      <c r="B2" t="s">
+        <v>571</v>
+      </c>
+      <c r="C2" t="s">
+        <v>572</v>
+      </c>
+      <c r="D2" t="s">
+        <v>573</v>
+      </c>
+      <c r="E2" t="s">
         <v>574</v>
       </c>
-      <c r="B2" t="s">
+      <c r="F2" t="s">
         <v>575</v>
       </c>
-      <c r="C2" t="s">
-        <v>576</v>
-      </c>
-      <c r="D2" t="s">
-        <v>577</v>
-      </c>
-      <c r="E2" t="s">
-        <v>578</v>
-      </c>
-      <c r="F2" t="s">
-        <v>579</v>
-      </c>
       <c r="G2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="E3" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="F3" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="G3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -5715,14 +5730,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
-        <v>235</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>236</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>237</v>
+      <c r="A1" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -5730,10 +5745,10 @@
         <v>43</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -5741,10 +5756,10 @@
         <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -5752,10 +5767,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -5763,10 +5778,10 @@
         <v>44</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -5795,13 +5810,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
-        <v>155</v>
+      <c r="A1" s="13" t="s">
+        <v>151</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>156</v>
-      </c>
-      <c r="C1" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -5810,22 +5825,22 @@
       <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="32"/>
+      <c r="G1" s="30"/>
       <c r="H1" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
-        <v>157</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="C2" s="15" t="s">
+      <c r="A2" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -5845,13 +5860,13 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
-        <v>159</v>
+      <c r="A3" s="13" t="s">
+        <v>155</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="C3" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -5873,7 +5888,7 @@
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
       <c r="B4" s="10"/>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="13" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -5895,7 +5910,7 @@
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="13" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -5917,7 +5932,7 @@
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="10"/>
       <c r="B6" s="10"/>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="13" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -5939,30 +5954,30 @@
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
-      <c r="C7" s="15" t="s">
-        <v>197</v>
+      <c r="C7" s="13" t="s">
+        <v>193</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
-      <c r="C8" s="15" t="s">
-        <v>198</v>
+      <c r="C8" s="13" t="s">
+        <v>194</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>15</v>
@@ -5976,14 +5991,14 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="21" t="s">
-        <v>199</v>
+      <c r="C9" s="19" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add in arms and epoch tweaks
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/full_1.xlsx
+++ b/tests/integration_test_files/full_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5140C1CA-31AB-414F-9D2E-15849EDFA559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EF4F622-0713-5248-8600-6631FE3BF2FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23320" yWindow="2400" windowWidth="56760" windowHeight="20140" activeTab="16" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="23320" yWindow="2400" windowWidth="56760" windowHeight="20140" activeTab="5" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -18,9 +18,9 @@
     <sheet name="studyIdentifiers" sheetId="3" r:id="rId3"/>
     <sheet name="studyDesign" sheetId="4" r:id="rId4"/>
     <sheet name="studyDesignArms" sheetId="15" r:id="rId5"/>
-    <sheet name="studyDesignEligibilityCriteria" sheetId="19" r:id="rId6"/>
-    <sheet name="dictionaries" sheetId="23" r:id="rId7"/>
-    <sheet name="studyDesignEpochs" sheetId="14" r:id="rId8"/>
+    <sheet name="studyDesignEpochs" sheetId="14" r:id="rId6"/>
+    <sheet name="studyDesignEligibilityCriteria" sheetId="19" r:id="rId7"/>
+    <sheet name="dictionaries" sheetId="23" r:id="rId8"/>
     <sheet name="mainTimeline" sheetId="1" r:id="rId9"/>
     <sheet name="studyDesignActivities" sheetId="16" r:id="rId10"/>
     <sheet name="studyDesignII" sheetId="6" r:id="rId11"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="602">
   <si>
     <t>Epoch</t>
   </si>
@@ -746,15 +746,6 @@
     <t>Test Nine</t>
   </si>
   <si>
-    <t>studyEpochName</t>
-  </si>
-  <si>
-    <t>studyEpochDescription</t>
-  </si>
-  <si>
-    <t>studyEpochType</t>
-  </si>
-  <si>
     <t>Screening Epoch</t>
   </si>
   <si>
@@ -777,21 +768,6 @@
   </si>
   <si>
     <t>FOLLOW-UP</t>
-  </si>
-  <si>
-    <t>studyArmName</t>
-  </si>
-  <si>
-    <t>studyArmDescription</t>
-  </si>
-  <si>
-    <t>studyArmType</t>
-  </si>
-  <si>
-    <t>studyArmDataOriginDescription</t>
-  </si>
-  <si>
-    <t>studyArmDataOriginType</t>
   </si>
   <si>
     <t>Active Substance</t>
@@ -1906,6 +1882,12 @@
   </si>
   <si>
     <t>Label</t>
+  </si>
+  <si>
+    <t>dataOriginDescription</t>
+  </si>
+  <si>
+    <t>dataOriginType</t>
   </si>
 </sst>
 </file>
@@ -2409,10 +2391,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>541</v>
+        <v>533</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2521,94 +2503,94 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>62</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="E16" s="19" t="s">
         <v>61</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>542</v>
+        <v>534</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
+        <v>523</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>524</v>
+      </c>
+      <c r="C17" t="s">
+        <v>525</v>
+      </c>
+      <c r="D17" t="s">
+        <v>526</v>
+      </c>
+      <c r="E17" t="s">
         <v>531</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>532</v>
-      </c>
-      <c r="C17" t="s">
-        <v>533</v>
-      </c>
-      <c r="D17" t="s">
-        <v>534</v>
-      </c>
-      <c r="E17" t="s">
-        <v>539</v>
       </c>
       <c r="F17" s="24">
         <v>44927</v>
       </c>
       <c r="G17" t="s">
-        <v>563</v>
+        <v>555</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
       <c r="B18" s="10" t="s">
+        <v>524</v>
+      </c>
+      <c r="C18" t="s">
+        <v>529</v>
+      </c>
+      <c r="D18" t="s">
+        <v>530</v>
+      </c>
+      <c r="E18" t="s">
         <v>532</v>
-      </c>
-      <c r="C18" t="s">
-        <v>537</v>
-      </c>
-      <c r="D18" t="s">
-        <v>538</v>
-      </c>
-      <c r="E18" t="s">
-        <v>540</v>
       </c>
       <c r="F18" s="24">
         <v>44927</v>
       </c>
       <c r="G18" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>536</v>
+        <v>528</v>
       </c>
       <c r="B19" s="10" t="s">
+        <v>524</v>
+      </c>
+      <c r="C19" t="s">
+        <v>529</v>
+      </c>
+      <c r="D19" t="s">
+        <v>530</v>
+      </c>
+      <c r="E19" t="s">
         <v>532</v>
-      </c>
-      <c r="C19" t="s">
-        <v>537</v>
-      </c>
-      <c r="D19" t="s">
-        <v>538</v>
-      </c>
-      <c r="E19" t="s">
-        <v>540</v>
       </c>
       <c r="F19" s="24">
         <v>44958</v>
       </c>
       <c r="G19" t="s">
-        <v>586</v>
+        <v>578</v>
       </c>
     </row>
   </sheetData>
@@ -2635,16 +2617,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2652,7 +2634,7 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2660,13 +2642,13 @@
         <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>166</v>
       </c>
       <c r="D3" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -2696,7 +2678,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>61</v>
@@ -2713,7 +2695,7 @@
         <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>605</v>
+        <v>597</v>
       </c>
       <c r="C2" t="s">
         <v>64</v>
@@ -2727,7 +2709,7 @@
         <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>605</v>
+        <v>597</v>
       </c>
       <c r="C3" t="s">
         <v>64</v>
@@ -2741,7 +2723,7 @@
         <v>97</v>
       </c>
       <c r="B4" t="s">
-        <v>606</v>
+        <v>598</v>
       </c>
       <c r="C4" t="s">
         <v>66</v>
@@ -2755,7 +2737,7 @@
         <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>606</v>
+        <v>598</v>
       </c>
       <c r="C5" t="s">
         <v>66</v>
@@ -2788,7 +2770,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>70</v>
@@ -2810,10 +2792,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>574</v>
+        <v>566</v>
       </c>
       <c r="B2" t="s">
-        <v>583</v>
+        <v>575</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -2830,10 +2812,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>581</v>
+        <v>573</v>
       </c>
       <c r="B3" t="s">
-        <v>584</v>
+        <v>576</v>
       </c>
       <c r="C3">
         <v>20</v>
@@ -2850,10 +2832,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>582</v>
+        <v>574</v>
       </c>
       <c r="B4" t="s">
-        <v>585</v>
+        <v>577</v>
       </c>
       <c r="C4">
         <v>20</v>
@@ -2898,34 +2880,34 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>602</v>
+        <v>594</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>82</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>592</v>
+        <v>584</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>595</v>
+        <v>587</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>83</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>591</v>
+        <v>583</v>
       </c>
       <c r="G1" s="19" t="s">
         <v>84</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>593</v>
+        <v>585</v>
       </c>
       <c r="I1" s="19" t="s">
-        <v>596</v>
+        <v>588</v>
       </c>
       <c r="J1" s="19" t="s">
-        <v>594</v>
+        <v>586</v>
       </c>
       <c r="K1" s="19" t="s">
         <v>85</v>
@@ -2936,7 +2918,7 @@
         <v>101</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>600</v>
+        <v>592</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -2949,7 +2931,7 @@
         <v>103</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>597</v>
+        <v>589</v>
       </c>
       <c r="H2" s="12"/>
       <c r="I2" s="12" t="s">
@@ -2965,7 +2947,7 @@
         <v>102</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>601</v>
+        <v>593</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12" t="s">
@@ -2978,7 +2960,7 @@
         <v>104</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>598</v>
+        <v>590</v>
       </c>
       <c r="H3" s="12"/>
       <c r="I3" s="12" t="s">
@@ -2999,7 +2981,7 @@
         <v>105</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>599</v>
+        <v>591</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12" t="s">
@@ -3303,7 +3285,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="31" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="B1" s="31" t="s">
         <v>106</v>
@@ -3388,7 +3370,7 @@
         <v>111</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>604</v>
+        <v>596</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>145</v>
@@ -3400,7 +3382,7 @@
         <v>104</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>603</v>
+        <v>595</v>
       </c>
     </row>
   </sheetData>
@@ -3663,8 +3645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{137D84F3-D0D8-A149-BA12-7DBD407EC782}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3678,13 +3660,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>198</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>607</v>
+        <v>599</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>174</v>
@@ -3802,16 +3784,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>496</v>
+        <v>488</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="33" x14ac:dyDescent="0.2">
@@ -3820,1212 +3802,1212 @@
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="9" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>526</v>
+        <v>518</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="113" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>524</v>
+        <v>516</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>527</v>
+        <v>519</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="B13" s="21"/>
       <c r="C13" s="9" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="B14" s="21"/>
       <c r="C14" s="9" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="B15" s="21"/>
       <c r="C15" s="9" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="B16" s="21"/>
       <c r="C16" s="9" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="B17" s="21"/>
       <c r="C17" s="9" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="B18" s="21"/>
       <c r="C18" s="9" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="B19" s="21"/>
       <c r="C19" s="9" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>457</v>
+        <v>449</v>
       </c>
       <c r="B20" s="21"/>
       <c r="C20" s="9" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="B21" s="21"/>
       <c r="C21" s="9" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="B22" s="21"/>
       <c r="C22" s="9" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
       <c r="B23" s="21"/>
       <c r="C23" s="9" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="B24" s="21"/>
       <c r="C24" s="9" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>454</v>
+        <v>446</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="B25" s="21"/>
       <c r="C25" s="9" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>446</v>
+        <v>438</v>
       </c>
       <c r="B26" s="21"/>
       <c r="C26" s="9" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
-        <v>447</v>
+        <v>439</v>
       </c>
       <c r="B27" s="21"/>
       <c r="C27" s="9" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
-        <v>448</v>
+        <v>440</v>
       </c>
       <c r="B28" s="21"/>
       <c r="C28" s="9" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
-        <v>449</v>
+        <v>441</v>
       </c>
       <c r="B29" s="21"/>
       <c r="C29" s="9" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
       <c r="B30" s="21"/>
       <c r="C30" s="9" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
-        <v>458</v>
+        <v>450</v>
       </c>
       <c r="B31" s="21"/>
       <c r="C31" s="9" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="B32" s="21"/>
       <c r="C32" s="9" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="B33" s="21"/>
       <c r="C33" s="9" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="B34" s="21"/>
       <c r="C34" s="9" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="B35" s="21"/>
       <c r="C35" s="9" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="B36" s="21"/>
       <c r="C36" s="9" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="B37" s="21"/>
       <c r="C37" s="9" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="B38" s="21"/>
       <c r="C38" s="9" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="B39" s="21"/>
       <c r="C39" s="9" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="B40" s="21"/>
       <c r="C40" s="9" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
       <c r="B41" s="21"/>
       <c r="C41" s="9" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="B42" s="21"/>
       <c r="C42" s="9" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="B43" s="21"/>
       <c r="C43" s="9" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="B44" s="21"/>
       <c r="C44" s="9" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>455</v>
+        <v>447</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="B45" s="21"/>
       <c r="C45" s="9" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
       <c r="B46" s="21"/>
       <c r="C46" s="9" t="s">
-        <v>303</v>
+        <v>295</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="B47" s="21"/>
       <c r="C47" s="9" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="B48" s="21"/>
       <c r="C48" s="9" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="B49" s="21"/>
       <c r="C49" s="9" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="B50" s="21"/>
       <c r="C50" s="9" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="10" t="s">
-        <v>459</v>
+        <v>451</v>
       </c>
       <c r="B51" s="21"/>
       <c r="C51" s="9" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
-        <v>495</v>
+        <v>487</v>
       </c>
       <c r="B52" s="21"/>
       <c r="C52" s="9" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="10" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="B53" s="21"/>
       <c r="C53" s="9" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="B54" s="21"/>
       <c r="C54" s="9" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="B55" s="21"/>
       <c r="C55" s="9" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
-        <v>497</v>
+        <v>489</v>
       </c>
       <c r="B56" s="21"/>
       <c r="C56" s="9" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
-        <v>498</v>
+        <v>490</v>
       </c>
       <c r="B57" s="21"/>
       <c r="C57" s="9" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="B58" s="21"/>
       <c r="C58" s="9" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
-        <v>460</v>
+        <v>452</v>
       </c>
       <c r="B59" s="21"/>
       <c r="C59" s="9" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="10" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="B60" s="21"/>
       <c r="C60" s="9" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="10" t="s">
-        <v>501</v>
+        <v>493</v>
       </c>
       <c r="B61" s="21"/>
       <c r="C61" s="9" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="10" t="s">
-        <v>502</v>
+        <v>494</v>
       </c>
       <c r="B62" s="21"/>
       <c r="C62" s="9" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="10" t="s">
-        <v>450</v>
+        <v>442</v>
       </c>
       <c r="B63" s="21"/>
       <c r="C63" s="9" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="10" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="B64" s="21"/>
       <c r="C64" s="9" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="10" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="B65" s="21"/>
       <c r="C65" s="9" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="10" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="B66" s="21"/>
       <c r="C66" s="9" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="10" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="B67" s="21"/>
       <c r="C67" s="9" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="10" t="s">
-        <v>503</v>
+        <v>495</v>
       </c>
       <c r="B68" s="21"/>
       <c r="C68" s="9" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="10" t="s">
-        <v>451</v>
+        <v>443</v>
       </c>
       <c r="B69" s="21"/>
       <c r="C69" s="9" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A70" s="10" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="B70" s="21"/>
       <c r="C70" s="9" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="10" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="B71" s="21"/>
       <c r="C71" s="9" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="10" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="B72" s="21"/>
       <c r="C72" s="9" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="10" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="B73" s="21"/>
       <c r="C73" s="9" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="10" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="B74" s="21"/>
       <c r="C74" s="9" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="10" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="B75" s="21"/>
       <c r="C75" s="9" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="10" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="B76" s="21"/>
       <c r="C76" s="9" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="10" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="B77" s="21"/>
       <c r="C77" s="9" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A78" s="10" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="B78" s="21"/>
       <c r="C78" s="9" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="10" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="B79" s="21"/>
       <c r="C79" s="9" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="10" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="B80" s="21"/>
       <c r="C80" s="9" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="10" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="B81" s="21"/>
       <c r="C81" s="9" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A82" s="10" t="s">
-        <v>505</v>
+        <v>497</v>
       </c>
       <c r="B82" s="21"/>
       <c r="C82" s="9" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="10" t="s">
-        <v>433</v>
+        <v>425</v>
       </c>
       <c r="B83" s="21"/>
       <c r="C83" s="9" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="10" t="s">
-        <v>434</v>
+        <v>426</v>
       </c>
       <c r="B84" s="21"/>
       <c r="C84" s="9" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A85" s="10" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="B85" s="21"/>
       <c r="C85" s="9" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="10" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="B86" s="21"/>
       <c r="C86" s="9" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" s="10" t="s">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="B87" s="21"/>
       <c r="C87" s="9" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="10" t="s">
-        <v>506</v>
+        <v>498</v>
       </c>
       <c r="B88" s="21"/>
       <c r="C88" s="9" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="10" t="s">
-        <v>507</v>
+        <v>499</v>
       </c>
       <c r="B89" s="21"/>
       <c r="C89" s="9" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="10" t="s">
-        <v>508</v>
+        <v>500</v>
       </c>
       <c r="B90" s="21"/>
       <c r="C90" s="9" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="10" t="s">
-        <v>500</v>
+        <v>492</v>
       </c>
       <c r="B91" s="21"/>
       <c r="C91" s="9" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="10" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="B92" s="21"/>
       <c r="C92" s="9" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="10" t="s">
-        <v>461</v>
+        <v>453</v>
       </c>
       <c r="B93" s="21"/>
       <c r="C93" s="9" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="10" t="s">
-        <v>509</v>
+        <v>501</v>
       </c>
       <c r="B94" s="21"/>
       <c r="C94" s="9" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="10" t="s">
-        <v>510</v>
+        <v>502</v>
       </c>
       <c r="B95" s="21"/>
       <c r="C95" s="9" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="10" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="B96" s="21"/>
       <c r="C96" s="9" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="10" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="B97" s="21"/>
       <c r="C97" s="9" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="10" t="s">
-        <v>440</v>
+        <v>432</v>
       </c>
       <c r="B98" s="21"/>
       <c r="C98" s="9" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="10" t="s">
-        <v>441</v>
+        <v>433</v>
       </c>
       <c r="B99" s="21"/>
       <c r="C99" s="9" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="10" t="s">
-        <v>442</v>
+        <v>434</v>
       </c>
       <c r="B100" s="21"/>
       <c r="C100" s="9" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="10" t="s">
-        <v>511</v>
+        <v>503</v>
       </c>
       <c r="B101" s="21"/>
       <c r="C101" s="9" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="10" t="s">
-        <v>512</v>
+        <v>504</v>
       </c>
       <c r="B102" s="21"/>
       <c r="C102" s="9" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="10" t="s">
-        <v>513</v>
+        <v>505</v>
       </c>
       <c r="B103" s="21"/>
       <c r="C103" s="9" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="10" t="s">
-        <v>514</v>
+        <v>506</v>
       </c>
       <c r="B104" s="21"/>
       <c r="C104" s="9" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="10" t="s">
-        <v>515</v>
+        <v>507</v>
       </c>
       <c r="B105" s="21"/>
       <c r="C105" s="9" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="10" t="s">
-        <v>516</v>
+        <v>508</v>
       </c>
       <c r="B106" s="21"/>
       <c r="C106" s="9" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="10" t="s">
-        <v>517</v>
+        <v>509</v>
       </c>
       <c r="B107" s="21"/>
       <c r="C107" s="9" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A108" s="10" t="s">
-        <v>462</v>
+        <v>454</v>
       </c>
       <c r="B108" s="21"/>
       <c r="C108" s="9" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="10" t="s">
-        <v>518</v>
+        <v>510</v>
       </c>
       <c r="B109" s="21"/>
       <c r="C109" s="9" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="10" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
       <c r="B110" s="21"/>
       <c r="C110" s="9" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="10" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="B111" s="21"/>
       <c r="C111" s="9" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="10" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="B112" s="21"/>
       <c r="C112" s="9" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="10" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="B113" s="21"/>
       <c r="C113" s="9" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A114" s="10" t="s">
-        <v>463</v>
+        <v>455</v>
       </c>
       <c r="B114" s="21"/>
       <c r="C114" s="9" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="10" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="B115" s="21"/>
       <c r="C115" s="9" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="10" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
       <c r="B116" s="21"/>
       <c r="C116" s="9" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="10" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
       <c r="B117" s="21"/>
       <c r="C117" s="9" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A118" s="10" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
       <c r="B118" s="21"/>
       <c r="C118" s="9" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="10" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
       <c r="B119" s="21"/>
       <c r="C119" s="9" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="10" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="B120" s="21"/>
       <c r="C120" s="9" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="10" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
       <c r="B121" s="21"/>
       <c r="C121" s="9" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="10" t="s">
-        <v>472</v>
+        <v>464</v>
       </c>
       <c r="B122" s="21"/>
       <c r="C122" s="9" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A123" s="10" t="s">
-        <v>465</v>
+        <v>457</v>
       </c>
       <c r="B123" s="21"/>
       <c r="C123" s="9" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="10" t="s">
-        <v>471</v>
+        <v>463</v>
       </c>
       <c r="B124" s="21"/>
       <c r="C124" s="9" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="10" t="s">
-        <v>443</v>
+        <v>435</v>
       </c>
       <c r="B125" s="21"/>
       <c r="C125" s="9" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="10" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
       <c r="B126" s="21"/>
       <c r="C126" s="9" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="10" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="B127" s="21"/>
       <c r="C127" s="9" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="10" t="s">
-        <v>470</v>
+        <v>462</v>
       </c>
       <c r="B128" s="21"/>
       <c r="C128" s="9" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="10" t="s">
-        <v>469</v>
+        <v>461</v>
       </c>
       <c r="B129" s="21"/>
       <c r="C129" s="9" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="10" t="s">
-        <v>468</v>
+        <v>460</v>
       </c>
       <c r="B130" s="21"/>
       <c r="C130" s="9" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="10" t="s">
-        <v>466</v>
+        <v>458</v>
       </c>
       <c r="B131" s="21"/>
       <c r="C131" s="9" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="10" t="s">
-        <v>467</v>
+        <v>459</v>
       </c>
       <c r="B132" s="21"/>
       <c r="C132" s="9" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="10" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="10" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="10" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="10" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="10" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="10" t="s">
-        <v>523</v>
+        <v>515</v>
       </c>
     </row>
   </sheetData>
@@ -5088,22 +5070,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
-        <v>543</v>
+        <v>535</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>544</v>
+        <v>536</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>545</v>
+        <v>537</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>546</v>
+        <v>538</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
       <c r="G1" s="10"/>
     </row>
@@ -5112,17 +5094,17 @@
         <v>4</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>549</v>
+        <v>541</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>166</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10" t="s">
-        <v>559</v>
+        <v>551</v>
       </c>
       <c r="G2" s="10"/>
     </row>
@@ -5131,17 +5113,17 @@
         <v>3</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>166</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>552</v>
+        <v>544</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="10" t="s">
-        <v>560</v>
+        <v>552</v>
       </c>
       <c r="G3" s="10"/>
     </row>
@@ -5150,19 +5132,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>553</v>
+        <v>545</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>166</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>554</v>
+        <v>546</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>555</v>
+        <v>547</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>561</v>
+        <v>553</v>
       </c>
       <c r="G4" s="10"/>
     </row>
@@ -5171,17 +5153,17 @@
         <v>1</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>557</v>
+        <v>549</v>
       </c>
       <c r="C5" s="10" t="s">
+        <v>542</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>550</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>558</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="10" t="s">
-        <v>562</v>
+        <v>554</v>
       </c>
       <c r="G5" s="10"/>
     </row>
@@ -5477,54 +5459,63 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7FA707-26D8-0546-9A99-D418F7F4E088}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.83203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="24.83203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="23.5" style="3" customWidth="1"/>
-    <col min="4" max="4" width="32.1640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18.1640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="23.5" style="3" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>241</v>
+        <v>448</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>242</v>
+        <v>62</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>243</v>
+        <v>521</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>244</v>
+        <v>61</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>600</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>240</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>42</v>
       </c>
@@ -5532,17 +5523,20 @@
         <v>42</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>250</v>
+        <v>42</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="E4" s="10"/>
+        <v>240</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F4" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5550,6 +5544,97 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E1D5BD-3A57-0140-9167-DAF5A3D4D9EF}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>448</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>521</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED1B92D-F8EC-D24D-81E6-6B85449D22F0}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -5569,65 +5654,65 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>528</v>
+        <v>520</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>564</v>
+        <v>556</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>62</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>565</v>
+        <v>557</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>577</v>
+        <v>569</v>
       </c>
       <c r="C2" t="s">
-        <v>578</v>
+        <v>570</v>
       </c>
       <c r="D2" t="s">
-        <v>579</v>
+        <v>571</v>
       </c>
       <c r="F2" t="s">
-        <v>580</v>
+        <v>572</v>
       </c>
       <c r="G2" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>576</v>
+        <v>568</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>587</v>
+        <v>579</v>
       </c>
       <c r="C3" t="s">
-        <v>588</v>
+        <v>580</v>
       </c>
       <c r="D3" t="s">
-        <v>589</v>
+        <v>581</v>
       </c>
       <c r="F3" t="s">
-        <v>590</v>
+        <v>582</v>
       </c>
       <c r="G3" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
     </row>
   </sheetData>
@@ -5635,7 +5720,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EB40753-8F7D-3941-9F21-F336F33F75CC}">
   <dimension ref="A1:G3"/>
   <sheetViews>
@@ -5652,45 +5737,45 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>456</v>
+        <v>448</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>62</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>566</v>
+        <v>558</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>567</v>
+        <v>559</v>
       </c>
       <c r="F1" s="19" t="s">
         <v>95</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>568</v>
+        <v>560</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>569</v>
+        <v>561</v>
       </c>
       <c r="B2" t="s">
-        <v>570</v>
+        <v>562</v>
       </c>
       <c r="C2" t="s">
-        <v>571</v>
+        <v>563</v>
       </c>
       <c r="D2" t="s">
-        <v>572</v>
+        <v>564</v>
       </c>
       <c r="E2" t="s">
-        <v>573</v>
+        <v>565</v>
       </c>
       <c r="F2" t="s">
-        <v>574</v>
+        <v>566</v>
       </c>
       <c r="G2" t="s">
         <v>72</v>
@@ -5698,91 +5783,16 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>575</v>
+        <v>567</v>
       </c>
       <c r="E3" t="s">
-        <v>573</v>
+        <v>565</v>
       </c>
       <c r="F3" t="s">
-        <v>574</v>
+        <v>566</v>
       </c>
       <c r="G3" t="s">
         <v>81</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E1D5BD-3A57-0140-9167-DAF5A3D4D9EF}">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="18.33203125" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
-        <v>230</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>231</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update timeline, timing and associated definitions
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/full_1.xlsx
+++ b/tests/integration_test_files/full_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9382BC-4AAF-D44C-9C44-670EE6AA7360}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25508B10-AEEC-CE4E-9091-9B098BF16D0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11840" yWindow="6980" windowWidth="56760" windowHeight="20140" activeTab="14" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="29260" yWindow="5760" windowWidth="47180" windowHeight="20040" firstSheet="5" activeTab="10" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -22,16 +22,17 @@
     <sheet name="studyDesignEligibilityCriteria" sheetId="19" r:id="rId7"/>
     <sheet name="dictionaries" sheetId="23" r:id="rId8"/>
     <sheet name="mainTimeline" sheetId="1" r:id="rId9"/>
-    <sheet name="studyDesignActivities" sheetId="16" r:id="rId10"/>
-    <sheet name="studyDesignII" sheetId="6" r:id="rId11"/>
-    <sheet name="studyDesignPopulations" sheetId="7" r:id="rId12"/>
-    <sheet name="studyDesignOE" sheetId="8" r:id="rId13"/>
-    <sheet name="studyDesignEstimands" sheetId="9" r:id="rId14"/>
-    <sheet name="studyDesignProcedures" sheetId="11" r:id="rId15"/>
-    <sheet name="studyDesignEncounters" sheetId="12" r:id="rId16"/>
-    <sheet name="studyDesignElements" sheetId="13" r:id="rId17"/>
-    <sheet name="studyDesignContent" sheetId="17" r:id="rId18"/>
-    <sheet name="configuration" sheetId="10" r:id="rId19"/>
+    <sheet name="studyDesignTiming" sheetId="25" r:id="rId10"/>
+    <sheet name="studyDesignActivities" sheetId="16" r:id="rId11"/>
+    <sheet name="studyDesignII" sheetId="6" r:id="rId12"/>
+    <sheet name="studyDesignPopulations" sheetId="7" r:id="rId13"/>
+    <sheet name="studyDesignOE" sheetId="8" r:id="rId14"/>
+    <sheet name="studyDesignEstimands" sheetId="9" r:id="rId15"/>
+    <sheet name="studyDesignProcedures" sheetId="11" r:id="rId16"/>
+    <sheet name="studyDesignEncounters" sheetId="12" r:id="rId17"/>
+    <sheet name="studyDesignElements" sheetId="13" r:id="rId18"/>
+    <sheet name="studyDesignContent" sheetId="17" r:id="rId19"/>
+    <sheet name="configuration" sheetId="10" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,10 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="595">
-  <si>
-    <t>Epoch</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="640">
   <si>
     <t>Screening</t>
   </si>
@@ -65,15 +63,6 @@
     <t>Treatment</t>
   </si>
   <si>
-    <t>Cycle</t>
-  </si>
-  <si>
-    <t>Cycle End Rule</t>
-  </si>
-  <si>
-    <t>A:</t>
-  </si>
-  <si>
     <t>X</t>
   </si>
   <si>
@@ -83,57 +72,18 @@
     <t>Child Activity</t>
   </si>
   <si>
-    <t>N: 0..2 Days</t>
-  </si>
-  <si>
     <t>Demographics</t>
   </si>
   <si>
     <t>Baseline</t>
   </si>
   <si>
-    <t>0..1 Hours</t>
-  </si>
-  <si>
     <t>15 min</t>
   </si>
   <si>
-    <t>P: +24 Hours</t>
-  </si>
-  <si>
-    <t>0..4 Hours</t>
-  </si>
-  <si>
-    <t>N: Pre Dose</t>
-  </si>
-  <si>
-    <t>Day 24</t>
-  </si>
-  <si>
-    <t>Day 35</t>
-  </si>
-  <si>
-    <t>P: +7 Days</t>
-  </si>
-  <si>
-    <t>-3..3 Days</t>
-  </si>
-  <si>
-    <t>First Cycle Start</t>
-  </si>
-  <si>
-    <t>Cycle Period</t>
-  </si>
-  <si>
-    <t>Timing</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>Something Else</t>
-  </si>
-  <si>
     <t>studyTitle</t>
   </si>
   <si>
@@ -575,9 +525,6 @@
     <t>2 week visit</t>
   </si>
   <si>
-    <t>5 week visit</t>
-  </si>
-  <si>
     <t>Visit</t>
   </si>
   <si>
@@ -614,12 +561,6 @@
     <t>E5</t>
   </si>
   <si>
-    <t>Encounter xref</t>
-  </si>
-  <si>
-    <t>Window</t>
-  </si>
-  <si>
     <t>BC/Procedure/Timeline</t>
   </si>
   <si>
@@ -753,9 +694,6 @@
   </si>
   <si>
     <t>Basic Demog</t>
-  </si>
-  <si>
-    <t>Something weird</t>
   </si>
   <si>
     <t>sectionTitle</t>
@@ -1867,6 +1805,204 @@
   </si>
   <si>
     <t>Only do this if this 'condition' is true</t>
+  </si>
+  <si>
+    <t>SCREEN</t>
+  </si>
+  <si>
+    <t>PRE DOSE</t>
+  </si>
+  <si>
+    <t>DOSE</t>
+  </si>
+  <si>
+    <t>D14</t>
+  </si>
+  <si>
+    <t>PROG</t>
+  </si>
+  <si>
+    <t>FU</t>
+  </si>
+  <si>
+    <t>Pre Dose</t>
+  </si>
+  <si>
+    <t>Dosing</t>
+  </si>
+  <si>
+    <t>Day 14</t>
+  </si>
+  <si>
+    <t>Screen</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t>Decision</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>(EXIT)</t>
+  </si>
+  <si>
+    <t>condition</t>
+  </si>
+  <si>
+    <t>epoch</t>
+  </si>
+  <si>
+    <t>encounter</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>timingValue</t>
+  </si>
+  <si>
+    <t>toFrom</t>
+  </si>
+  <si>
+    <t>window</t>
+  </si>
+  <si>
+    <t>TIM1</t>
+  </si>
+  <si>
+    <t>Screening timing</t>
+  </si>
+  <si>
+    <t>BEFORE</t>
+  </si>
+  <si>
+    <t>2 days</t>
+  </si>
+  <si>
+    <t>S2S</t>
+  </si>
+  <si>
+    <t>TIM2</t>
+  </si>
+  <si>
+    <t>Pre dose timing</t>
+  </si>
+  <si>
+    <t>Pre dose</t>
+  </si>
+  <si>
+    <t>-4..0 hours</t>
+  </si>
+  <si>
+    <t>TIM3</t>
+  </si>
+  <si>
+    <t>Dosing anchor</t>
+  </si>
+  <si>
+    <t>FIXED</t>
+  </si>
+  <si>
+    <t>1 Day</t>
+  </si>
+  <si>
+    <t>TIM4</t>
+  </si>
+  <si>
+    <t>Day 14 timing</t>
+  </si>
+  <si>
+    <t>AFTER</t>
+  </si>
+  <si>
+    <t>14 days</t>
+  </si>
+  <si>
+    <t>-1..1 days</t>
+  </si>
+  <si>
+    <t>TIM5</t>
+  </si>
+  <si>
+    <t>Follow up timing</t>
+  </si>
+  <si>
+    <t>-3..3 days</t>
+  </si>
+  <si>
+    <t>Day 28</t>
+  </si>
+  <si>
+    <t>D28</t>
+  </si>
+  <si>
+    <t>Day 28 Optional</t>
+  </si>
+  <si>
+    <t>Check Opt In</t>
+  </si>
+  <si>
+    <t>FU: if opted out</t>
+  </si>
+  <si>
+    <t>Check opt In by subject</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>Day 28 timing</t>
+  </si>
+  <si>
+    <t>28 Days</t>
+  </si>
+  <si>
+    <t>42 Days</t>
+  </si>
+  <si>
+    <t>4 week visit</t>
+  </si>
+  <si>
+    <t>Day 42</t>
+  </si>
+  <si>
+    <t>6 week visit</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>BC:SYSBP, BC:DIABP</t>
+  </si>
+  <si>
+    <t>Optional safety activity</t>
+  </si>
+  <si>
+    <t>Optional activity</t>
+  </si>
+  <si>
+    <t>Procedures</t>
+  </si>
+  <si>
+    <t>Perform the procedures</t>
+  </si>
+  <si>
+    <t>Perform the optional weight data collection</t>
+  </si>
+  <si>
+    <t>Weight optional</t>
+  </si>
+  <si>
+    <t>BC:Weight</t>
+  </si>
+  <si>
+    <t>Optional Weight</t>
   </si>
 </sst>
 </file>
@@ -2031,11 +2167,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2370,206 +2506,206 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
-        <v>432</v>
+        <v>411</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>517</v>
+        <v>496</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
-        <v>504</v>
+        <v>483</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>432</v>
+        <v>411</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>505</v>
+        <v>484</v>
       </c>
       <c r="E16" s="19" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>506</v>
+        <v>485</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>518</v>
+        <v>497</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>507</v>
+        <v>486</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>508</v>
+        <v>487</v>
       </c>
       <c r="C17" t="s">
-        <v>509</v>
+        <v>488</v>
       </c>
       <c r="D17" t="s">
-        <v>510</v>
+        <v>489</v>
       </c>
       <c r="E17" t="s">
-        <v>515</v>
+        <v>494</v>
       </c>
       <c r="F17" s="24">
         <v>44927</v>
       </c>
       <c r="G17" t="s">
-        <v>539</v>
+        <v>518</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>512</v>
+        <v>491</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>508</v>
+        <v>487</v>
       </c>
       <c r="C18" t="s">
-        <v>513</v>
+        <v>492</v>
       </c>
       <c r="D18" t="s">
-        <v>514</v>
+        <v>493</v>
       </c>
       <c r="E18" t="s">
-        <v>516</v>
+        <v>495</v>
       </c>
       <c r="F18" s="24">
         <v>44927</v>
       </c>
       <c r="G18" t="s">
-        <v>511</v>
+        <v>490</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>512</v>
+        <v>491</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>508</v>
+        <v>487</v>
       </c>
       <c r="C19" t="s">
-        <v>513</v>
+        <v>492</v>
       </c>
       <c r="D19" t="s">
-        <v>514</v>
+        <v>493</v>
       </c>
       <c r="E19" t="s">
-        <v>516</v>
+        <v>495</v>
       </c>
       <c r="F19" s="24">
         <v>44958</v>
       </c>
       <c r="G19" t="s">
-        <v>562</v>
+        <v>541</v>
       </c>
     </row>
   </sheetData>
@@ -2578,17 +2714,231 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A0B1F19-81B2-DE4D-B058-6D33A4EF2886}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="18.5" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="6" width="11" customWidth="1"/>
+    <col min="7" max="9" width="13.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>411</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>484</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>591</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>592</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>593</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>594</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>596</v>
+      </c>
+      <c r="B2" t="s">
+        <v>597</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>598</v>
+      </c>
+      <c r="E2" t="s">
+        <v>574</v>
+      </c>
+      <c r="F2" t="s">
+        <v>575</v>
+      </c>
+      <c r="G2" t="s">
+        <v>599</v>
+      </c>
+      <c r="H2" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>601</v>
+      </c>
+      <c r="B3" t="s">
+        <v>602</v>
+      </c>
+      <c r="C3" t="s">
+        <v>603</v>
+      </c>
+      <c r="D3" t="s">
+        <v>598</v>
+      </c>
+      <c r="E3" t="s">
+        <v>575</v>
+      </c>
+      <c r="F3" t="s">
+        <v>576</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>600</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>605</v>
+      </c>
+      <c r="B4" t="s">
+        <v>606</v>
+      </c>
+      <c r="C4" t="s">
+        <v>581</v>
+      </c>
+      <c r="D4" t="s">
+        <v>607</v>
+      </c>
+      <c r="E4" t="s">
+        <v>576</v>
+      </c>
+      <c r="F4" t="s">
+        <v>576</v>
+      </c>
+      <c r="G4" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>609</v>
+      </c>
+      <c r="B5" t="s">
+        <v>610</v>
+      </c>
+      <c r="C5" t="s">
+        <v>582</v>
+      </c>
+      <c r="D5" t="s">
+        <v>611</v>
+      </c>
+      <c r="E5" t="s">
+        <v>577</v>
+      </c>
+      <c r="F5" t="s">
+        <v>576</v>
+      </c>
+      <c r="G5" t="s">
+        <v>612</v>
+      </c>
+      <c r="H5" t="s">
+        <v>600</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>609</v>
+      </c>
+      <c r="B6" t="s">
+        <v>624</v>
+      </c>
+      <c r="C6" t="s">
+        <v>617</v>
+      </c>
+      <c r="D6" t="s">
+        <v>611</v>
+      </c>
+      <c r="E6" t="s">
+        <v>618</v>
+      </c>
+      <c r="F6" t="s">
+        <v>576</v>
+      </c>
+      <c r="G6" t="s">
+        <v>625</v>
+      </c>
+      <c r="H6" t="s">
+        <v>600</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>614</v>
+      </c>
+      <c r="B7" t="s">
+        <v>615</v>
+      </c>
+      <c r="C7" t="s">
+        <v>177</v>
+      </c>
+      <c r="D7" t="s">
+        <v>611</v>
+      </c>
+      <c r="E7" t="s">
+        <v>579</v>
+      </c>
+      <c r="F7" t="s">
+        <v>576</v>
+      </c>
+      <c r="G7" t="s">
+        <v>626</v>
+      </c>
+      <c r="H7" t="s">
+        <v>600</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>616</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA8389B3-D1BB-1047-BA06-7E793B938DBA}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
-    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="38.83203125" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" customWidth="1"/>
     <col min="4" max="4" width="19.33203125" style="7" customWidth="1"/>
     <col min="5" max="5" width="29.6640625" customWidth="1"/>
@@ -2596,61 +2946,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
-        <v>432</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>505</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>230</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>231</v>
+      <c r="A1" s="19" t="s">
+        <v>411</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>484</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>210</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>232</v>
+        <v>212</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>25</v>
+        <v>634</v>
       </c>
       <c r="B3" t="s">
-        <v>233</v>
+        <v>635</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="E3" t="s">
-        <v>594</v>
+        <v>634</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>639</v>
+      </c>
+      <c r="B4" t="s">
+        <v>636</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>637</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="E4" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="A5" t="s">
+        <v>630</v>
+      </c>
+      <c r="B5" t="s">
+        <v>632</v>
+      </c>
+      <c r="C5" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E548DFC1-EB0E-374B-95D2-A04104B745FB}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -2668,72 +3040,72 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>432</v>
+        <v>411</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>581</v>
+        <v>560</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>581</v>
+        <v>560</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
-        <v>582</v>
+        <v>561</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="B5" t="s">
-        <v>582</v>
+        <v>561</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -2741,7 +3113,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C037A932-CB5B-8D43-956E-5F5C367E07FC}">
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -2760,84 +3132,84 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>432</v>
+        <v>411</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>550</v>
+        <v>529</v>
       </c>
       <c r="B2" t="s">
-        <v>559</v>
+        <v>538</v>
       </c>
       <c r="C2">
         <v>100</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>557</v>
+        <v>536</v>
       </c>
       <c r="B3" t="s">
-        <v>560</v>
+        <v>539</v>
       </c>
       <c r="C3">
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="F3" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>558</v>
+        <v>537</v>
       </c>
       <c r="B4" t="s">
-        <v>561</v>
+        <v>540</v>
       </c>
       <c r="C4">
         <v>20</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="F4" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -2845,7 +3217,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B908C5D6-C6A1-4043-A49A-69C599CFBAE9}">
   <dimension ref="A1:K26"/>
   <sheetViews>
@@ -2870,95 +3242,95 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>578</v>
+        <v>557</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>568</v>
+        <v>547</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>571</v>
+        <v>550</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>567</v>
+        <v>546</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>569</v>
+        <v>548</v>
       </c>
       <c r="I1" s="19" t="s">
-        <v>572</v>
+        <v>551</v>
       </c>
       <c r="J1" s="19" t="s">
-        <v>570</v>
+        <v>549</v>
       </c>
       <c r="K1" s="19" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>576</v>
+        <v>555</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>103</v>
-      </c>
       <c r="G2" s="12" t="s">
-        <v>573</v>
+        <v>552</v>
       </c>
       <c r="H2" s="12"/>
       <c r="I2" s="12" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="J2" s="10"/>
       <c r="K2" s="12" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>577</v>
+        <v>556</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>574</v>
+        <v>553</v>
       </c>
       <c r="H3" s="12"/>
       <c r="I3" s="12" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="J3" s="10"/>
       <c r="K3" s="12" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="34" x14ac:dyDescent="0.2">
@@ -2968,18 +3340,18 @@
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>575</v>
+        <v>554</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="12" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -3253,7 +3625,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBFC82B4-C495-A142-993D-B6A47D77A4C3}">
   <dimension ref="A1:H5"/>
   <sheetViews>
@@ -3274,55 +3646,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
-        <v>432</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>106</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="E1" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="F1" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="G1" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="H1" s="31" t="s">
-        <v>108</v>
+      <c r="A1" s="30" t="s">
+        <v>411</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="30" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -3334,7 +3706,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -3346,33 +3718,33 @@
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
       <c r="H4" s="10" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>580</v>
+        <v>559</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>579</v>
+        <v>558</v>
       </c>
     </row>
   </sheetData>
@@ -3380,11 +3752,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D608A778-255D-4443-A7EA-03049F1FC98F}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -3402,65 +3774,65 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>432</v>
+        <v>411</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>505</v>
+        <v>484</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="B2" t="s">
-        <v>588</v>
+        <v>567</v>
       </c>
       <c r="C2" t="s">
-        <v>588</v>
+        <v>567</v>
       </c>
       <c r="D2" t="s">
-        <v>591</v>
+        <v>570</v>
       </c>
       <c r="E2" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="B3" t="s">
-        <v>590</v>
+        <v>569</v>
       </c>
       <c r="C3" t="s">
-        <v>589</v>
+        <v>568</v>
       </c>
       <c r="D3" t="s">
-        <v>591</v>
+        <v>570</v>
       </c>
       <c r="E3" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="G3" t="s">
-        <v>592</v>
+        <v>571</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -3474,12 +3846,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3500D92E-6FB0-8D4D-97D2-7C2457E4D88B}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3495,137 +3867,157 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>432</v>
+        <v>411</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>505</v>
+        <v>484</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>586</v>
+        <v>565</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>587</v>
+        <v>566</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>181</v>
+        <v>163</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>179</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>182</v>
+        <v>164</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>183</v>
+        <v>165</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>17</v>
+        <v>582</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>173</v>
+        <v>627</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>18</v>
+        <v>617</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>178</v>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>623</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>629</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>628</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -3634,7 +4026,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{137D84F3-D0D8-A149-BA12-7DBD407EC782}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -3653,104 +4045,104 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>432</v>
+        <v>411</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>583</v>
+        <v>562</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>207</v>
+        <v>187</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>211</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>180</v>
+        <v>162</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>212</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -3759,7 +4151,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F40359-1191-3843-B5C3-38D19A754655}">
   <dimension ref="A1:D138"/>
   <sheetViews>
@@ -3777,1268 +4169,1234 @@
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>472</v>
+        <v>451</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>432</v>
+        <v>411</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>234</v>
+        <v>213</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>235</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="33" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="9" t="s">
-        <v>236</v>
+        <v>215</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>502</v>
+        <v>481</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>367</v>
+        <v>346</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>241</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>368</v>
+        <v>347</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>369</v>
+        <v>348</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>370</v>
+        <v>349</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>237</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>371</v>
+        <v>350</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>244</v>
+        <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>372</v>
+        <v>351</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>245</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>373</v>
+        <v>352</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>238</v>
+        <v>217</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="113" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>500</v>
+        <v>479</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>501</v>
+        <v>480</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>503</v>
+        <v>482</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>374</v>
+        <v>353</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>239</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>375</v>
+        <v>354</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>246</v>
+        <v>225</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>366</v>
+        <v>345</v>
       </c>
       <c r="B13" s="21"/>
       <c r="C13" s="9" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>376</v>
+        <v>355</v>
       </c>
       <c r="B14" s="21"/>
       <c r="C14" s="9" t="s">
-        <v>248</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>377</v>
+        <v>356</v>
       </c>
       <c r="B15" s="21"/>
       <c r="C15" s="9" t="s">
-        <v>249</v>
+        <v>228</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>378</v>
+        <v>357</v>
       </c>
       <c r="B16" s="21"/>
       <c r="C16" s="9" t="s">
-        <v>250</v>
+        <v>229</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>379</v>
+        <v>358</v>
       </c>
       <c r="B17" s="21"/>
       <c r="C17" s="9" t="s">
-        <v>251</v>
+        <v>230</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>455</v>
+        <v>434</v>
       </c>
       <c r="B18" s="21"/>
       <c r="C18" s="9" t="s">
-        <v>252</v>
+        <v>231</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>456</v>
+        <v>435</v>
       </c>
       <c r="B19" s="21"/>
       <c r="C19" s="9" t="s">
-        <v>253</v>
+        <v>232</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>433</v>
+        <v>412</v>
       </c>
       <c r="B20" s="21"/>
       <c r="C20" s="9" t="s">
-        <v>240</v>
+        <v>219</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
-        <v>457</v>
+        <v>436</v>
       </c>
       <c r="B21" s="21"/>
       <c r="C21" s="9" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>458</v>
+        <v>437</v>
       </c>
       <c r="B22" s="21"/>
       <c r="C22" s="9" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>459</v>
+        <v>438</v>
       </c>
       <c r="B23" s="21"/>
       <c r="C23" s="9" t="s">
-        <v>256</v>
+        <v>235</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>429</v>
+        <v>408</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>460</v>
+        <v>439</v>
       </c>
       <c r="B24" s="21"/>
       <c r="C24" s="9" t="s">
-        <v>257</v>
+        <v>236</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>430</v>
+        <v>409</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>461</v>
+        <v>440</v>
       </c>
       <c r="B25" s="21"/>
       <c r="C25" s="9" t="s">
-        <v>258</v>
+        <v>237</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>422</v>
+        <v>401</v>
       </c>
       <c r="B26" s="21"/>
       <c r="C26" s="9" t="s">
-        <v>259</v>
+        <v>238</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
-        <v>423</v>
+        <v>402</v>
       </c>
       <c r="B27" s="21"/>
       <c r="C27" s="9" t="s">
-        <v>260</v>
+        <v>239</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
-        <v>424</v>
+        <v>403</v>
       </c>
       <c r="B28" s="21"/>
       <c r="C28" s="9" t="s">
-        <v>261</v>
+        <v>240</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
-        <v>425</v>
+        <v>404</v>
       </c>
       <c r="B29" s="21"/>
       <c r="C29" s="9" t="s">
-        <v>262</v>
+        <v>241</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
-        <v>462</v>
+        <v>441</v>
       </c>
       <c r="B30" s="21"/>
       <c r="C30" s="9" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
-        <v>434</v>
+        <v>413</v>
       </c>
       <c r="B31" s="21"/>
       <c r="C31" s="9" t="s">
-        <v>264</v>
+        <v>243</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
-        <v>463</v>
+        <v>442</v>
       </c>
       <c r="B32" s="21"/>
       <c r="C32" s="9" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
-        <v>464</v>
+        <v>443</v>
       </c>
       <c r="B33" s="21"/>
       <c r="C33" s="9" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
-        <v>465</v>
+        <v>444</v>
       </c>
       <c r="B34" s="21"/>
       <c r="C34" s="9" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
-        <v>380</v>
+        <v>359</v>
       </c>
       <c r="B35" s="21"/>
       <c r="C35" s="9" t="s">
-        <v>268</v>
+        <v>247</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
-        <v>466</v>
+        <v>445</v>
       </c>
       <c r="B36" s="21"/>
       <c r="C36" s="9" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
-        <v>467</v>
+        <v>446</v>
       </c>
       <c r="B37" s="21"/>
       <c r="C37" s="9" t="s">
-        <v>270</v>
+        <v>249</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
-        <v>381</v>
+        <v>360</v>
       </c>
       <c r="B38" s="21"/>
       <c r="C38" s="9" t="s">
-        <v>271</v>
+        <v>250</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
-        <v>382</v>
+        <v>361</v>
       </c>
       <c r="B39" s="21"/>
       <c r="C39" s="9" t="s">
-        <v>272</v>
+        <v>251</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
-        <v>383</v>
+        <v>362</v>
       </c>
       <c r="B40" s="21"/>
       <c r="C40" s="9" t="s">
-        <v>273</v>
+        <v>252</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
-        <v>468</v>
+        <v>447</v>
       </c>
       <c r="B41" s="21"/>
       <c r="C41" s="9" t="s">
-        <v>274</v>
+        <v>253</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
-        <v>384</v>
+        <v>363</v>
       </c>
       <c r="B42" s="21"/>
       <c r="C42" s="9" t="s">
-        <v>275</v>
+        <v>254</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
-        <v>385</v>
+        <v>364</v>
       </c>
       <c r="B43" s="21"/>
       <c r="C43" s="9" t="s">
-        <v>276</v>
+        <v>255</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
-        <v>386</v>
+        <v>365</v>
       </c>
       <c r="B44" s="21"/>
       <c r="C44" s="9" t="s">
-        <v>277</v>
+        <v>256</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>431</v>
+        <v>410</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
-        <v>469</v>
+        <v>448</v>
       </c>
       <c r="B45" s="21"/>
       <c r="C45" s="9" t="s">
-        <v>278</v>
+        <v>257</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
-        <v>470</v>
+        <v>449</v>
       </c>
       <c r="B46" s="21"/>
       <c r="C46" s="9" t="s">
-        <v>279</v>
+        <v>258</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
-        <v>387</v>
+        <v>366</v>
       </c>
       <c r="B47" s="21"/>
       <c r="C47" s="9" t="s">
-        <v>280</v>
+        <v>259</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
-        <v>388</v>
+        <v>367</v>
       </c>
       <c r="B48" s="21"/>
       <c r="C48" s="9" t="s">
-        <v>281</v>
+        <v>260</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
-        <v>389</v>
+        <v>368</v>
       </c>
       <c r="B49" s="21"/>
       <c r="C49" s="9" t="s">
-        <v>282</v>
+        <v>261</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
-        <v>390</v>
+        <v>369</v>
       </c>
       <c r="B50" s="21"/>
       <c r="C50" s="9" t="s">
-        <v>283</v>
+        <v>262</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="10" t="s">
-        <v>435</v>
+        <v>414</v>
       </c>
       <c r="B51" s="21"/>
       <c r="C51" s="9" t="s">
-        <v>365</v>
+        <v>344</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
-        <v>471</v>
+        <v>450</v>
       </c>
       <c r="B52" s="21"/>
       <c r="C52" s="9" t="s">
-        <v>284</v>
+        <v>263</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="10" t="s">
-        <v>391</v>
+        <v>370</v>
       </c>
       <c r="B53" s="21"/>
       <c r="C53" s="9" t="s">
-        <v>285</v>
+        <v>264</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
-        <v>392</v>
+        <v>371</v>
       </c>
       <c r="B54" s="21"/>
       <c r="C54" s="9" t="s">
-        <v>286</v>
+        <v>265</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
-        <v>393</v>
+        <v>372</v>
       </c>
       <c r="B55" s="21"/>
       <c r="C55" s="9" t="s">
-        <v>287</v>
+        <v>266</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
-        <v>473</v>
+        <v>452</v>
       </c>
       <c r="B56" s="21"/>
       <c r="C56" s="9" t="s">
-        <v>288</v>
+        <v>267</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
-        <v>474</v>
+        <v>453</v>
       </c>
       <c r="B57" s="21"/>
       <c r="C57" s="9" t="s">
-        <v>289</v>
+        <v>268</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
-        <v>475</v>
+        <v>454</v>
       </c>
       <c r="B58" s="21"/>
       <c r="C58" s="9" t="s">
-        <v>290</v>
+        <v>269</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
-        <v>436</v>
+        <v>415</v>
       </c>
       <c r="B59" s="21"/>
       <c r="C59" s="9" t="s">
-        <v>291</v>
+        <v>270</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="10" t="s">
-        <v>476</v>
+        <v>455</v>
       </c>
       <c r="B60" s="21"/>
       <c r="C60" s="9" t="s">
-        <v>292</v>
+        <v>271</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="10" t="s">
-        <v>477</v>
+        <v>456</v>
       </c>
       <c r="B61" s="21"/>
       <c r="C61" s="9" t="s">
-        <v>293</v>
+        <v>272</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="10" t="s">
-        <v>478</v>
+        <v>457</v>
       </c>
       <c r="B62" s="21"/>
       <c r="C62" s="9" t="s">
-        <v>294</v>
+        <v>273</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="10" t="s">
-        <v>426</v>
+        <v>405</v>
       </c>
       <c r="B63" s="21"/>
       <c r="C63" s="9" t="s">
-        <v>295</v>
+        <v>274</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="10" t="s">
-        <v>394</v>
+        <v>373</v>
       </c>
       <c r="B64" s="21"/>
       <c r="C64" s="9" t="s">
-        <v>296</v>
+        <v>275</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="10" t="s">
-        <v>395</v>
+        <v>374</v>
       </c>
       <c r="B65" s="21"/>
       <c r="C65" s="9" t="s">
-        <v>297</v>
+        <v>276</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="10" t="s">
-        <v>396</v>
+        <v>375</v>
       </c>
       <c r="B66" s="21"/>
       <c r="C66" s="9" t="s">
-        <v>298</v>
+        <v>277</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="10" t="s">
-        <v>397</v>
+        <v>376</v>
       </c>
       <c r="B67" s="21"/>
       <c r="C67" s="9" t="s">
-        <v>299</v>
+        <v>278</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="10" t="s">
-        <v>479</v>
+        <v>458</v>
       </c>
       <c r="B68" s="21"/>
       <c r="C68" s="9" t="s">
-        <v>300</v>
+        <v>279</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="10" t="s">
-        <v>427</v>
+        <v>406</v>
       </c>
       <c r="B69" s="21"/>
       <c r="C69" s="9" t="s">
-        <v>301</v>
+        <v>280</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A70" s="10" t="s">
-        <v>398</v>
+        <v>377</v>
       </c>
       <c r="B70" s="21"/>
       <c r="C70" s="9" t="s">
-        <v>302</v>
+        <v>281</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" s="10" t="s">
-        <v>399</v>
+        <v>378</v>
       </c>
       <c r="B71" s="21"/>
       <c r="C71" s="9" t="s">
-        <v>303</v>
+        <v>282</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="10" t="s">
-        <v>400</v>
+        <v>379</v>
       </c>
       <c r="B72" s="21"/>
       <c r="C72" s="9" t="s">
-        <v>304</v>
+        <v>283</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="10" t="s">
-        <v>401</v>
+        <v>380</v>
       </c>
       <c r="B73" s="21"/>
       <c r="C73" s="9" t="s">
-        <v>305</v>
+        <v>284</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="10" t="s">
-        <v>402</v>
+        <v>381</v>
       </c>
       <c r="B74" s="21"/>
       <c r="C74" s="9" t="s">
-        <v>306</v>
+        <v>285</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="10" t="s">
-        <v>403</v>
+        <v>382</v>
       </c>
       <c r="B75" s="21"/>
       <c r="C75" s="9" t="s">
-        <v>307</v>
+        <v>286</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="10" t="s">
-        <v>404</v>
+        <v>383</v>
       </c>
       <c r="B76" s="21"/>
       <c r="C76" s="9" t="s">
-        <v>308</v>
+        <v>287</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="10" t="s">
-        <v>405</v>
+        <v>384</v>
       </c>
       <c r="B77" s="21"/>
       <c r="C77" s="9" t="s">
-        <v>309</v>
+        <v>288</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A78" s="10" t="s">
-        <v>406</v>
+        <v>385</v>
       </c>
       <c r="B78" s="21"/>
       <c r="C78" s="9" t="s">
-        <v>310</v>
+        <v>289</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" s="10" t="s">
-        <v>480</v>
+        <v>459</v>
       </c>
       <c r="B79" s="21"/>
       <c r="C79" s="9" t="s">
-        <v>311</v>
+        <v>290</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="10" t="s">
-        <v>407</v>
+        <v>386</v>
       </c>
       <c r="B80" s="21"/>
       <c r="C80" s="9" t="s">
-        <v>312</v>
+        <v>291</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="10" t="s">
-        <v>408</v>
+        <v>387</v>
       </c>
       <c r="B81" s="21"/>
       <c r="C81" s="9" t="s">
-        <v>313</v>
+        <v>292</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A82" s="10" t="s">
-        <v>481</v>
+        <v>460</v>
       </c>
       <c r="B82" s="21"/>
       <c r="C82" s="9" t="s">
-        <v>314</v>
+        <v>293</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" s="10" t="s">
-        <v>409</v>
+        <v>388</v>
       </c>
       <c r="B83" s="21"/>
       <c r="C83" s="9" t="s">
-        <v>315</v>
+        <v>294</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="10" t="s">
-        <v>410</v>
+        <v>389</v>
       </c>
       <c r="B84" s="21"/>
       <c r="C84" s="9" t="s">
-        <v>316</v>
+        <v>295</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A85" s="10" t="s">
-        <v>411</v>
+        <v>390</v>
       </c>
       <c r="B85" s="21"/>
       <c r="C85" s="9" t="s">
-        <v>317</v>
+        <v>296</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="10" t="s">
-        <v>412</v>
+        <v>391</v>
       </c>
       <c r="B86" s="21"/>
       <c r="C86" s="9" t="s">
-        <v>318</v>
+        <v>297</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A87" s="10" t="s">
-        <v>413</v>
+        <v>392</v>
       </c>
       <c r="B87" s="21"/>
       <c r="C87" s="9" t="s">
-        <v>319</v>
+        <v>298</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A88" s="10" t="s">
-        <v>482</v>
+        <v>461</v>
       </c>
       <c r="B88" s="21"/>
       <c r="C88" s="9" t="s">
-        <v>320</v>
+        <v>299</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="10" t="s">
-        <v>483</v>
+        <v>462</v>
       </c>
       <c r="B89" s="21"/>
       <c r="C89" s="9" t="s">
-        <v>321</v>
+        <v>300</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="10" t="s">
-        <v>484</v>
+        <v>463</v>
       </c>
       <c r="B90" s="21"/>
       <c r="C90" s="9" t="s">
-        <v>322</v>
+        <v>301</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="10" t="s">
-        <v>476</v>
+        <v>455</v>
       </c>
       <c r="B91" s="21"/>
       <c r="C91" s="9" t="s">
-        <v>323</v>
+        <v>302</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="10" t="s">
-        <v>428</v>
+        <v>407</v>
       </c>
       <c r="B92" s="21"/>
       <c r="C92" s="9" t="s">
-        <v>324</v>
+        <v>303</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="10" t="s">
-        <v>437</v>
+        <v>416</v>
       </c>
       <c r="B93" s="21"/>
       <c r="C93" s="9" t="s">
-        <v>325</v>
+        <v>304</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="10" t="s">
-        <v>485</v>
+        <v>464</v>
       </c>
       <c r="B94" s="21"/>
       <c r="C94" s="9" t="s">
-        <v>326</v>
+        <v>305</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="10" t="s">
-        <v>486</v>
+        <v>465</v>
       </c>
       <c r="B95" s="21"/>
       <c r="C95" s="9" t="s">
-        <v>327</v>
+        <v>306</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="10" t="s">
-        <v>414</v>
+        <v>393</v>
       </c>
       <c r="B96" s="21"/>
       <c r="C96" s="9" t="s">
-        <v>328</v>
+        <v>307</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="10" t="s">
-        <v>415</v>
+        <v>394</v>
       </c>
       <c r="B97" s="21"/>
       <c r="C97" s="9" t="s">
-        <v>329</v>
+        <v>308</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="10" t="s">
-        <v>416</v>
+        <v>395</v>
       </c>
       <c r="B98" s="21"/>
       <c r="C98" s="9" t="s">
-        <v>330</v>
+        <v>309</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="10" t="s">
-        <v>417</v>
+        <v>396</v>
       </c>
       <c r="B99" s="21"/>
       <c r="C99" s="9" t="s">
-        <v>331</v>
+        <v>310</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="10" t="s">
-        <v>418</v>
+        <v>397</v>
       </c>
       <c r="B100" s="21"/>
       <c r="C100" s="9" t="s">
-        <v>332</v>
+        <v>311</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="10" t="s">
-        <v>487</v>
+        <v>466</v>
       </c>
       <c r="B101" s="21"/>
       <c r="C101" s="9" t="s">
-        <v>333</v>
+        <v>312</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="10" t="s">
-        <v>488</v>
+        <v>467</v>
       </c>
       <c r="B102" s="21"/>
       <c r="C102" s="9" t="s">
-        <v>334</v>
+        <v>313</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="10" t="s">
-        <v>489</v>
+        <v>468</v>
       </c>
       <c r="B103" s="21"/>
       <c r="C103" s="9" t="s">
-        <v>335</v>
+        <v>314</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="10" t="s">
-        <v>490</v>
+        <v>469</v>
       </c>
       <c r="B104" s="21"/>
       <c r="C104" s="9" t="s">
-        <v>336</v>
+        <v>315</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="10" t="s">
-        <v>491</v>
+        <v>470</v>
       </c>
       <c r="B105" s="21"/>
       <c r="C105" s="9" t="s">
-        <v>337</v>
+        <v>316</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="10" t="s">
-        <v>492</v>
+        <v>471</v>
       </c>
       <c r="B106" s="21"/>
       <c r="C106" s="9" t="s">
-        <v>338</v>
+        <v>317</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="10" t="s">
-        <v>493</v>
+        <v>472</v>
       </c>
       <c r="B107" s="21"/>
       <c r="C107" s="9" t="s">
-        <v>339</v>
+        <v>318</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A108" s="10" t="s">
-        <v>438</v>
+        <v>417</v>
       </c>
       <c r="B108" s="21"/>
       <c r="C108" s="9" t="s">
-        <v>340</v>
+        <v>319</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A109" s="10" t="s">
-        <v>494</v>
+        <v>473</v>
       </c>
       <c r="B109" s="21"/>
       <c r="C109" s="9" t="s">
-        <v>341</v>
+        <v>320</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="10" t="s">
-        <v>495</v>
+        <v>474</v>
       </c>
       <c r="B110" s="21"/>
       <c r="C110" s="9" t="s">
-        <v>342</v>
+        <v>321</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="10" t="s">
-        <v>496</v>
+        <v>475</v>
       </c>
       <c r="B111" s="21"/>
       <c r="C111" s="9" t="s">
-        <v>343</v>
+        <v>322</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="10" t="s">
-        <v>497</v>
+        <v>476</v>
       </c>
       <c r="B112" s="21"/>
       <c r="C112" s="9" t="s">
-        <v>344</v>
+        <v>323</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="10" t="s">
-        <v>498</v>
+        <v>477</v>
       </c>
       <c r="B113" s="21"/>
       <c r="C113" s="9" t="s">
-        <v>345</v>
+        <v>324</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A114" s="10" t="s">
-        <v>439</v>
+        <v>418</v>
       </c>
       <c r="B114" s="21"/>
       <c r="C114" s="9" t="s">
-        <v>346</v>
+        <v>325</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A115" s="10" t="s">
-        <v>454</v>
+        <v>433</v>
       </c>
       <c r="B115" s="21"/>
       <c r="C115" s="9" t="s">
-        <v>347</v>
+        <v>326</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="10" t="s">
-        <v>453</v>
+        <v>432</v>
       </c>
       <c r="B116" s="21"/>
       <c r="C116" s="9" t="s">
-        <v>348</v>
+        <v>327</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="10" t="s">
-        <v>452</v>
+        <v>431</v>
       </c>
       <c r="B117" s="21"/>
       <c r="C117" s="9" t="s">
-        <v>349</v>
+        <v>328</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A118" s="10" t="s">
-        <v>440</v>
+        <v>419</v>
       </c>
       <c r="B118" s="21"/>
       <c r="C118" s="9" t="s">
-        <v>350</v>
+        <v>329</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="10" t="s">
-        <v>451</v>
+        <v>430</v>
       </c>
       <c r="B119" s="21"/>
       <c r="C119" s="9" t="s">
-        <v>351</v>
+        <v>330</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="10" t="s">
-        <v>450</v>
+        <v>429</v>
       </c>
       <c r="B120" s="21"/>
       <c r="C120" s="9" t="s">
-        <v>352</v>
+        <v>331</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="10" t="s">
-        <v>449</v>
+        <v>428</v>
       </c>
       <c r="B121" s="21"/>
       <c r="C121" s="9" t="s">
-        <v>353</v>
+        <v>332</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="10" t="s">
-        <v>448</v>
+        <v>427</v>
       </c>
       <c r="B122" s="21"/>
       <c r="C122" s="9" t="s">
-        <v>354</v>
+        <v>333</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A123" s="10" t="s">
-        <v>441</v>
+        <v>420</v>
       </c>
       <c r="B123" s="21"/>
       <c r="C123" s="9" t="s">
-        <v>355</v>
+        <v>334</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A124" s="10" t="s">
-        <v>447</v>
+        <v>426</v>
       </c>
       <c r="B124" s="21"/>
       <c r="C124" s="9" t="s">
-        <v>356</v>
+        <v>335</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="10" t="s">
-        <v>419</v>
+        <v>398</v>
       </c>
       <c r="B125" s="21"/>
       <c r="C125" s="9" t="s">
-        <v>357</v>
+        <v>336</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="10" t="s">
-        <v>420</v>
+        <v>399</v>
       </c>
       <c r="B126" s="21"/>
       <c r="C126" s="9" t="s">
-        <v>358</v>
+        <v>337</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="10" t="s">
-        <v>421</v>
+        <v>400</v>
       </c>
       <c r="B127" s="21"/>
       <c r="C127" s="9" t="s">
-        <v>359</v>
+        <v>338</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="10" t="s">
-        <v>446</v>
+        <v>425</v>
       </c>
       <c r="B128" s="21"/>
       <c r="C128" s="9" t="s">
-        <v>360</v>
+        <v>339</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="10" t="s">
-        <v>445</v>
+        <v>424</v>
       </c>
       <c r="B129" s="21"/>
       <c r="C129" s="9" t="s">
-        <v>361</v>
+        <v>340</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="10" t="s">
-        <v>444</v>
+        <v>423</v>
       </c>
       <c r="B130" s="21"/>
       <c r="C130" s="9" t="s">
-        <v>362</v>
+        <v>341</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="10" t="s">
-        <v>442</v>
+        <v>421</v>
       </c>
       <c r="B131" s="21"/>
       <c r="C131" s="9" t="s">
-        <v>363</v>
+        <v>342</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="10" t="s">
-        <v>443</v>
+        <v>422</v>
       </c>
       <c r="B132" s="21"/>
       <c r="C132" s="9" t="s">
-        <v>364</v>
+        <v>343</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="10" t="s">
-        <v>499</v>
+        <v>478</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="10" t="s">
-        <v>499</v>
+        <v>478</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="10" t="s">
-        <v>499</v>
+        <v>478</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="10" t="s">
-        <v>499</v>
+        <v>478</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="10" t="s">
-        <v>499</v>
+        <v>478</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="10" t="s">
-        <v>499</v>
+        <v>478</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1886B59F-3C17-014D-9C61-BEC33F421A82}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="25.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="B1" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="B2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5063,22 +5421,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
-        <v>519</v>
+        <v>498</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>520</v>
+        <v>499</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>521</v>
+        <v>500</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>522</v>
+        <v>501</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>523</v>
+        <v>502</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>532</v>
+        <v>511</v>
       </c>
       <c r="G1" s="10"/>
     </row>
@@ -5087,17 +5445,17 @@
         <v>4</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>525</v>
+        <v>504</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>527</v>
+        <v>506</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10" t="s">
-        <v>535</v>
+        <v>514</v>
       </c>
       <c r="G2" s="10"/>
     </row>
@@ -5106,17 +5464,17 @@
         <v>3</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>524</v>
+        <v>503</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>528</v>
+        <v>507</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="10" t="s">
-        <v>536</v>
+        <v>515</v>
       </c>
       <c r="G3" s="10"/>
     </row>
@@ -5125,19 +5483,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>529</v>
+        <v>508</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>530</v>
+        <v>509</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>531</v>
+        <v>510</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>537</v>
+        <v>516</v>
       </c>
       <c r="G4" s="10"/>
     </row>
@@ -5146,19 +5504,53 @@
         <v>1</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>533</v>
+        <v>512</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>526</v>
+        <v>505</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>534</v>
+        <v>513</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="10" t="s">
-        <v>538</v>
+        <v>517</v>
       </c>
       <c r="G5" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1886B59F-3C17-014D-9C61-BEC33F421A82}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" t="s">
+        <v>122</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5184,62 +5576,62 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="D1" s="17" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="E1" s="17" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="E3" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -5264,10 +5656,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="C1" s="27"/>
       <c r="D1" s="27"/>
@@ -5275,10 +5667,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>216</v>
+        <v>196</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>213</v>
+        <v>193</v>
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27"/>
@@ -5286,10 +5678,10 @@
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
@@ -5297,10 +5689,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="C4" s="29"/>
       <c r="D4" s="29"/>
@@ -5308,10 +5700,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="C5" s="29"/>
       <c r="D5" s="29"/>
@@ -5319,10 +5711,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="B6" s="27" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="C6" s="27"/>
       <c r="D6" s="27"/>
@@ -5330,10 +5722,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B7" s="27" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="C7" s="27"/>
       <c r="D7" s="27"/>
@@ -5341,10 +5733,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="C8" s="27"/>
       <c r="D8" s="27"/>
@@ -5352,10 +5744,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="C9" s="27"/>
       <c r="D9" s="27"/>
@@ -5363,7 +5755,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="B10" s="27"/>
       <c r="C10" s="27"/>
@@ -5372,53 +5764,53 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>205</v>
+        <v>185</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>206</v>
+        <v>186</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -5470,62 +5862,62 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>432</v>
+        <v>411</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>505</v>
+        <v>484</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>584</v>
+        <v>563</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>585</v>
+        <v>564</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>225</v>
+        <v>205</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>226</v>
+        <v>206</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>227</v>
+        <v>207</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>228</v>
+        <v>208</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -5554,72 +5946,72 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>432</v>
+        <v>411</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>505</v>
+        <v>484</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>217</v>
+        <v>197</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>218</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>219</v>
+        <v>199</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>221</v>
+        <v>201</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>223</v>
+        <v>203</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>224</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -5647,65 +6039,65 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>504</v>
+        <v>483</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>540</v>
+        <v>519</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>432</v>
+        <v>411</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>505</v>
+        <v>484</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>235</v>
+        <v>214</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>541</v>
+        <v>520</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>552</v>
+        <v>531</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>553</v>
+        <v>532</v>
       </c>
       <c r="C2" t="s">
-        <v>554</v>
+        <v>533</v>
       </c>
       <c r="D2" t="s">
-        <v>555</v>
+        <v>534</v>
       </c>
       <c r="F2" t="s">
-        <v>556</v>
+        <v>535</v>
       </c>
       <c r="G2" t="s">
-        <v>545</v>
+        <v>524</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>552</v>
+        <v>531</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>563</v>
+        <v>542</v>
       </c>
       <c r="C3" t="s">
-        <v>564</v>
+        <v>543</v>
       </c>
       <c r="D3" t="s">
-        <v>565</v>
+        <v>544</v>
       </c>
       <c r="F3" t="s">
-        <v>566</v>
+        <v>545</v>
       </c>
       <c r="G3" t="s">
-        <v>545</v>
+        <v>524</v>
       </c>
     </row>
   </sheetData>
@@ -5730,62 +6122,62 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>432</v>
+        <v>411</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>505</v>
+        <v>484</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>542</v>
+        <v>521</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>543</v>
+        <v>522</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>544</v>
+        <v>523</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>545</v>
+        <v>524</v>
       </c>
       <c r="B2" t="s">
-        <v>546</v>
+        <v>525</v>
       </c>
       <c r="C2" t="s">
-        <v>547</v>
+        <v>526</v>
       </c>
       <c r="D2" t="s">
-        <v>548</v>
+        <v>527</v>
       </c>
       <c r="E2" t="s">
-        <v>549</v>
+        <v>528</v>
       </c>
       <c r="F2" t="s">
-        <v>550</v>
+        <v>529</v>
       </c>
       <c r="G2" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>551</v>
+        <v>530</v>
       </c>
       <c r="E3" t="s">
-        <v>549</v>
+        <v>528</v>
       </c>
       <c r="F3" t="s">
-        <v>550</v>
+        <v>529</v>
       </c>
       <c r="G3" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -5795,13 +6187,13 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10:B11"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5809,258 +6201,318 @@
     <col min="1" max="1" width="16.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="29.5" style="3" customWidth="1"/>
     <col min="3" max="3" width="35.83203125" style="1" customWidth="1"/>
-    <col min="4" max="8" width="12.33203125" style="1" customWidth="1"/>
-    <col min="9" max="10" width="10.83203125" style="1"/>
+    <col min="4" max="9" width="12.33203125" style="1" customWidth="1"/>
+    <col min="10" max="11" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="C1" s="13" t="s">
+        <v>411</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E2" s="2" t="s">
+        <v>580</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="I2" s="31" t="s">
+        <v>619</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>484</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="1" t="s">
+      <c r="G3" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="H3" s="31" t="s">
+        <v>622</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="13"/>
+      <c r="C4" s="13" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="13" t="s">
-        <v>22</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>24</v>
+        <v>584</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>24</v>
+        <v>584</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>24</v>
+        <v>584</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>24</v>
+        <v>584</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
+        <v>585</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>584</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="13"/>
       <c r="C5" s="13" t="s">
-        <v>4</v>
+        <v>586</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>24</v>
+        <v>575</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>24</v>
+        <v>576</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>24</v>
+        <v>577</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>24</v>
+        <v>578</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
+        <v>618</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>579</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="13"/>
       <c r="C6" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>588</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="31" t="s">
+        <v>621</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="13" t="s">
-        <v>186</v>
+        <v>589</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>181</v>
+        <v>0</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>182</v>
+        <v>6</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>183</v>
+        <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>590</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B9" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="19" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="B10" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>25</v>
+        <v>634</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>593</v>
+        <v>572</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>639</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>638</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>630</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>631</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="F1:G1"/>
-  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add standard section initial code and tests
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/full_1.xlsx
+++ b/tests/integration_test_files/full_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B492DE0-0055-C44B-8330-D73D4FA14E86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11003728-49F7-1249-8307-04F57E2281D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29240" yWindow="5740" windowWidth="47180" windowHeight="20040" activeTab="2" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="30200" yWindow="500" windowWidth="34860" windowHeight="20040" firstSheet="10" activeTab="18" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="640">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="642">
   <si>
     <t>Screening</t>
   </si>
@@ -2003,6 +2003,12 @@
   </si>
   <si>
     <t>Somewhere|In a District|In a City|In a big state|12345|FRA</t>
+  </si>
+  <si>
+    <t>SECTION=M11Synopsis</t>
+  </si>
+  <si>
+    <t>SECTION = SoA</t>
   </si>
 </sst>
 </file>
@@ -2168,10 +2174,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3026,7 +3032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E548DFC1-EB0E-374B-95D2-A04104B745FB}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -4156,8 +4162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F40359-1191-3843-B5C3-38D19A754655}">
   <dimension ref="A1:D138"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4201,6 +4207,9 @@
       <c r="C3" s="9" t="s">
         <v>218</v>
       </c>
+      <c r="D3" s="9" t="s">
+        <v>640</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
@@ -4216,6 +4225,9 @@
       </c>
       <c r="C5" s="9" t="s">
         <v>220</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>641</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5562,7 +5574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9227F54-17C1-E44A-AD70-49AE8CBF35F9}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F3"/>
     </sheetView>
   </sheetViews>
@@ -5681,34 +5693,34 @@
       <c r="A3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="31" t="s">
         <v>147</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
@@ -5828,16 +5840,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6191,10 +6203,10 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Generate content, first cut
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/full_1.xlsx
+++ b/tests/integration_test_files/full_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11003728-49F7-1249-8307-04F57E2281D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83349F51-FF4A-8C4B-98E9-EF47684C7278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30200" yWindow="500" windowWidth="34860" windowHeight="20040" firstSheet="10" activeTab="18" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
@@ -1502,20 +1502,6 @@
     <t>Primary Objectives</t>
   </si>
   <si>
-    <r>
-      <t>&lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Menlo"/>
-        <family val="2"/>
-      </rPr>
-      <t>usdm:ref klass="StudyIdentifier" id="StudyIdentifier_1" attribute="studyIdentifier"/&gt;</t>
-    </r>
-  </si>
-  <si>
     <t>&lt;table&gt;
   &lt;tr&gt;
     &lt;th style="vertical-align: top"&gt;Primary Objective&lt;/th&gt;
@@ -2005,17 +1991,20 @@
     <t>Somewhere|In a District|In a City|In a big state|12345|FRA</t>
   </si>
   <si>
-    <t>SECTION=M11Synopsis</t>
-  </si>
-  <si>
-    <t>SECTION = SoA</t>
+    <t>TITLE PAGE</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>section = M11-title-page</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2052,12 +2041,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Menlo"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -2515,7 +2498,7 @@
         <v>409</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2624,7 +2607,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>409</v>
@@ -2633,85 +2616,85 @@
         <v>43</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="E16" s="19" t="s">
         <v>42</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
+        <v>483</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>484</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="C17" t="s">
         <v>485</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>486</v>
       </c>
-      <c r="D17" t="s">
-        <v>487</v>
-      </c>
       <c r="E17" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F17" s="24">
         <v>44927</v>
       </c>
       <c r="G17" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
+        <v>488</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>484</v>
+      </c>
+      <c r="C18" t="s">
         <v>489</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>485</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>490</v>
       </c>
-      <c r="D18" t="s">
-        <v>491</v>
-      </c>
       <c r="E18" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F18" s="24">
         <v>44927</v>
       </c>
       <c r="G18" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
+        <v>488</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>484</v>
+      </c>
+      <c r="C19" t="s">
         <v>489</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>485</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>490</v>
       </c>
-      <c r="D19" t="s">
-        <v>491</v>
-      </c>
       <c r="E19" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F19" s="24">
         <v>44958</v>
       </c>
       <c r="G19" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
   </sheetData>
@@ -2742,190 +2725,190 @@
         <v>43</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>42</v>
       </c>
       <c r="E1" s="19" t="s">
+        <v>588</v>
+      </c>
+      <c r="F1" s="19" t="s">
         <v>589</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="G1" s="19" t="s">
         <v>590</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="H1" s="19" t="s">
         <v>591</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="I1" s="19" t="s">
         <v>592</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>593</v>
+      </c>
+      <c r="B2" t="s">
         <v>594</v>
-      </c>
-      <c r="B2" t="s">
-        <v>595</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>595</v>
+      </c>
+      <c r="E2" t="s">
+        <v>571</v>
+      </c>
+      <c r="F2" t="s">
+        <v>572</v>
+      </c>
+      <c r="G2" t="s">
         <v>596</v>
       </c>
-      <c r="E2" t="s">
-        <v>572</v>
-      </c>
-      <c r="F2" t="s">
-        <v>573</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>597</v>
-      </c>
-      <c r="H2" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>598</v>
+      </c>
+      <c r="B3" t="s">
         <v>599</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>600</v>
       </c>
-      <c r="C3" t="s">
-        <v>601</v>
-      </c>
       <c r="D3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E3" t="s">
+        <v>572</v>
+      </c>
+      <c r="F3" t="s">
         <v>573</v>
-      </c>
-      <c r="F3" t="s">
-        <v>574</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
       </c>
       <c r="H3" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>602</v>
+      </c>
+      <c r="B4" t="s">
         <v>603</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>578</v>
+      </c>
+      <c r="D4" t="s">
         <v>604</v>
       </c>
-      <c r="C4" t="s">
-        <v>579</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>573</v>
+      </c>
+      <c r="F4" t="s">
+        <v>573</v>
+      </c>
+      <c r="G4" t="s">
         <v>605</v>
-      </c>
-      <c r="E4" t="s">
-        <v>574</v>
-      </c>
-      <c r="F4" t="s">
-        <v>574</v>
-      </c>
-      <c r="G4" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>606</v>
+      </c>
+      <c r="B5" t="s">
         <v>607</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>579</v>
+      </c>
+      <c r="D5" t="s">
         <v>608</v>
       </c>
-      <c r="C5" t="s">
-        <v>580</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>574</v>
+      </c>
+      <c r="F5" t="s">
+        <v>573</v>
+      </c>
+      <c r="G5" t="s">
         <v>609</v>
       </c>
-      <c r="E5" t="s">
-        <v>575</v>
-      </c>
-      <c r="F5" t="s">
-        <v>574</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
+        <v>597</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>610</v>
-      </c>
-      <c r="H5" t="s">
-        <v>598</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B6" t="s">
+        <v>621</v>
+      </c>
+      <c r="C6" t="s">
+        <v>614</v>
+      </c>
+      <c r="D6" t="s">
+        <v>608</v>
+      </c>
+      <c r="E6" t="s">
+        <v>615</v>
+      </c>
+      <c r="F6" t="s">
+        <v>573</v>
+      </c>
+      <c r="G6" t="s">
         <v>622</v>
       </c>
-      <c r="C6" t="s">
-        <v>615</v>
-      </c>
-      <c r="D6" t="s">
-        <v>609</v>
-      </c>
-      <c r="E6" t="s">
-        <v>616</v>
-      </c>
-      <c r="F6" t="s">
-        <v>574</v>
-      </c>
-      <c r="G6" t="s">
-        <v>623</v>
-      </c>
       <c r="H6" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>611</v>
+      </c>
+      <c r="B7" t="s">
         <v>612</v>
-      </c>
-      <c r="B7" t="s">
-        <v>613</v>
       </c>
       <c r="C7" t="s">
         <v>175</v>
       </c>
       <c r="D7" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E7" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="F7" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="G7" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="H7" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
   </sheetData>
@@ -2959,7 +2942,7 @@
         <v>43</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D1" s="25" t="s">
         <v>208</v>
@@ -2981,41 +2964,41 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>631</v>
+      </c>
+      <c r="B3" t="s">
         <v>632</v>
       </c>
-      <c r="B3" t="s">
-        <v>633</v>
-      </c>
       <c r="C3" s="4" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B4" t="s">
+        <v>633</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>634</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>635</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>146</v>
       </c>
       <c r="E4" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B5" t="s">
+        <v>629</v>
+      </c>
+      <c r="C5" t="s">
         <v>630</v>
-      </c>
-      <c r="C5" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -3063,7 +3046,7 @@
         <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C2" t="s">
         <v>45</v>
@@ -3077,7 +3060,7 @@
         <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="C3" t="s">
         <v>45</v>
@@ -3091,7 +3074,7 @@
         <v>78</v>
       </c>
       <c r="B4" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C4" t="s">
         <v>47</v>
@@ -3105,7 +3088,7 @@
         <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C5" t="s">
         <v>47</v>
@@ -3160,10 +3143,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B2" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -3180,10 +3163,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C3">
         <v>20</v>
@@ -3200,10 +3183,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B4" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C4">
         <v>20</v>
@@ -3248,34 +3231,34 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>63</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>64</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="G1" s="19" t="s">
         <v>65</v>
       </c>
       <c r="H1" s="19" t="s">
+        <v>545</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>548</v>
+      </c>
+      <c r="J1" s="19" t="s">
         <v>546</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>549</v>
-      </c>
-      <c r="J1" s="19" t="s">
-        <v>547</v>
       </c>
       <c r="K1" s="19" t="s">
         <v>66</v>
@@ -3286,7 +3269,7 @@
         <v>82</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -3299,7 +3282,7 @@
         <v>84</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="H2" s="12"/>
       <c r="I2" s="12" t="s">
@@ -3315,7 +3298,7 @@
         <v>83</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12" t="s">
@@ -3328,7 +3311,7 @@
         <v>85</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="H3" s="12"/>
       <c r="I3" s="12" t="s">
@@ -3349,7 +3332,7 @@
         <v>86</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12" t="s">
@@ -3738,7 +3721,7 @@
         <v>92</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>126</v>
@@ -3750,7 +3733,7 @@
         <v>85</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
   </sheetData>
@@ -3786,7 +3769,7 @@
         <v>43</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>138</v>
@@ -3806,13 +3789,13 @@
         <v>142</v>
       </c>
       <c r="B2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="E2" t="s">
         <v>143</v>
@@ -3823,13 +3806,13 @@
         <v>144</v>
       </c>
       <c r="B3" t="s">
+        <v>566</v>
+      </c>
+      <c r="C3" t="s">
+        <v>565</v>
+      </c>
+      <c r="D3" t="s">
         <v>567</v>
-      </c>
-      <c r="C3" t="s">
-        <v>566</v>
-      </c>
-      <c r="D3" t="s">
-        <v>568</v>
       </c>
       <c r="E3" t="s">
         <v>145</v>
@@ -3838,7 +3821,7 @@
         <v>146</v>
       </c>
       <c r="G3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -3880,16 +3863,16 @@
         <v>43</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>42</v>
       </c>
       <c r="E1" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="F1" s="19" t="s">
         <v>563</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>564</v>
       </c>
       <c r="G1" s="19" t="s">
         <v>148</v>
@@ -3975,7 +3958,7 @@
         <v>153</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>154</v>
@@ -3992,10 +3975,10 @@
         <v>165</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>154</v>
@@ -4009,13 +3992,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>154</v>
@@ -4058,7 +4041,7 @@
         <v>169</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>148</v>
@@ -4160,10 +4143,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F40359-1191-3843-B5C3-38D19A754655}">
-  <dimension ref="A1:D138"/>
+  <dimension ref="A1:D139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4188,1199 +4171,1197 @@
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="33" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
-        <v>13</v>
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>640</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="9" t="s">
-        <v>213</v>
+        <v>639</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>479</v>
+        <v>641</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>344</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B3" s="21"/>
       <c r="C3" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>640</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>641</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>214</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
         <v>350</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C10" s="9" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="113" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
+    <row r="11" spans="1:4" ht="113" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
         <v>477</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C11" s="9" t="s">
         <v>478</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
-        <v>351</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>216</v>
+      <c r="D11" s="9" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>343</v>
-      </c>
-      <c r="B13" s="21"/>
+        <v>352</v>
+      </c>
       <c r="C13" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="B14" s="21"/>
       <c r="C14" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B15" s="21"/>
       <c r="C15" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B16" s="21"/>
       <c r="C16" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B17" s="21"/>
       <c r="C17" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>432</v>
+        <v>356</v>
       </c>
       <c r="B18" s="21"/>
       <c r="C18" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B19" s="21"/>
       <c r="C19" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>410</v>
+        <v>433</v>
       </c>
       <c r="B20" s="21"/>
       <c r="C20" s="9" t="s">
-        <v>217</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
-        <v>434</v>
+        <v>410</v>
       </c>
       <c r="B21" s="21"/>
       <c r="C21" s="9" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B22" s="21"/>
       <c r="C22" s="9" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B23" s="21"/>
       <c r="C23" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>406</v>
+        <v>232</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B24" s="21"/>
       <c r="C24" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="85" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B25" s="21"/>
       <c r="C25" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>407</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>399</v>
+        <v>438</v>
       </c>
       <c r="B26" s="21"/>
       <c r="C26" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B27" s="21"/>
       <c r="C27" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B28" s="21"/>
       <c r="C28" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B29" s="21"/>
       <c r="C29" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
-        <v>439</v>
+        <v>402</v>
       </c>
       <c r="B30" s="21"/>
       <c r="C30" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
-        <v>411</v>
+        <v>439</v>
       </c>
       <c r="B31" s="21"/>
       <c r="C31" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
-        <v>440</v>
+        <v>411</v>
       </c>
       <c r="B32" s="21"/>
       <c r="C32" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B33" s="21"/>
       <c r="C33" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B34" s="21"/>
       <c r="C34" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
-        <v>357</v>
+        <v>442</v>
       </c>
       <c r="B35" s="21"/>
       <c r="C35" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
-        <v>443</v>
+        <v>357</v>
       </c>
       <c r="B36" s="21"/>
       <c r="C36" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B37" s="21"/>
       <c r="C37" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
-        <v>358</v>
+        <v>444</v>
       </c>
       <c r="B38" s="21"/>
       <c r="C38" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B39" s="21"/>
       <c r="C39" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B40" s="21"/>
       <c r="C40" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
-        <v>445</v>
+        <v>360</v>
       </c>
       <c r="B41" s="21"/>
       <c r="C41" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
-        <v>361</v>
+        <v>445</v>
       </c>
       <c r="B42" s="21"/>
       <c r="C42" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B43" s="21"/>
       <c r="C43" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B44" s="21"/>
       <c r="C44" s="9" t="s">
-        <v>254</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>408</v>
+        <v>253</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
-        <v>446</v>
+        <v>363</v>
       </c>
       <c r="B45" s="21"/>
       <c r="C45" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B46" s="21"/>
       <c r="C46" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
-        <v>364</v>
+        <v>447</v>
       </c>
       <c r="B47" s="21"/>
       <c r="C47" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B48" s="21"/>
       <c r="C48" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B49" s="21"/>
       <c r="C49" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B50" s="21"/>
       <c r="C50" s="9" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="10" t="s">
-        <v>412</v>
+        <v>367</v>
       </c>
       <c r="B51" s="21"/>
       <c r="C51" s="9" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
-        <v>448</v>
+        <v>412</v>
       </c>
       <c r="B52" s="21"/>
       <c r="C52" s="9" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="10" t="s">
-        <v>368</v>
+        <v>448</v>
       </c>
       <c r="B53" s="21"/>
       <c r="C53" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B54" s="21"/>
       <c r="C54" s="9" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B55" s="21"/>
       <c r="C55" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
-        <v>450</v>
+        <v>370</v>
       </c>
       <c r="B56" s="21"/>
       <c r="C56" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B57" s="21"/>
       <c r="C57" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B58" s="21"/>
       <c r="C58" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
-        <v>413</v>
+        <v>452</v>
       </c>
       <c r="B59" s="21"/>
       <c r="C59" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="10" t="s">
-        <v>453</v>
+        <v>413</v>
       </c>
       <c r="B60" s="21"/>
       <c r="C60" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="10" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B61" s="21"/>
       <c r="C61" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="10" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B62" s="21"/>
       <c r="C62" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="10" t="s">
-        <v>403</v>
+        <v>455</v>
       </c>
       <c r="B63" s="21"/>
       <c r="C63" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="10" t="s">
-        <v>371</v>
+        <v>403</v>
       </c>
       <c r="B64" s="21"/>
       <c r="C64" s="9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="10" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B65" s="21"/>
       <c r="C65" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="10" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B66" s="21"/>
       <c r="C66" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="10" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B67" s="21"/>
       <c r="C67" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="10" t="s">
-        <v>456</v>
+        <v>374</v>
       </c>
       <c r="B68" s="21"/>
       <c r="C68" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="10" t="s">
-        <v>404</v>
+        <v>456</v>
       </c>
       <c r="B69" s="21"/>
       <c r="C69" s="9" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="10" t="s">
-        <v>375</v>
+        <v>404</v>
       </c>
       <c r="B70" s="21"/>
       <c r="C70" s="9" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A71" s="10" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B71" s="21"/>
       <c r="C71" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="10" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B72" s="21"/>
       <c r="C72" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="10" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B73" s="21"/>
       <c r="C73" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B74" s="21"/>
       <c r="C74" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B75" s="21"/>
       <c r="C75" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="10" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B76" s="21"/>
       <c r="C76" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="10" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B77" s="21"/>
       <c r="C77" s="9" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="10" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B78" s="21"/>
       <c r="C78" s="9" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A79" s="10" t="s">
-        <v>457</v>
+        <v>383</v>
       </c>
       <c r="B79" s="21"/>
       <c r="C79" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="10" t="s">
-        <v>384</v>
+        <v>457</v>
       </c>
       <c r="B80" s="21"/>
       <c r="C80" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="10" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B81" s="21"/>
       <c r="C81" s="9" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="10" t="s">
-        <v>458</v>
+        <v>385</v>
       </c>
       <c r="B82" s="21"/>
       <c r="C82" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A83" s="10" t="s">
-        <v>386</v>
+        <v>458</v>
       </c>
       <c r="B83" s="21"/>
       <c r="C83" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="10" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B84" s="21"/>
       <c r="C84" s="9" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="10" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B85" s="21"/>
       <c r="C85" s="9" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A86" s="10" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B86" s="21"/>
       <c r="C86" s="9" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="10" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B87" s="21"/>
       <c r="C87" s="9" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A88" s="10" t="s">
-        <v>459</v>
+        <v>390</v>
       </c>
       <c r="B88" s="21"/>
       <c r="C88" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="10" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B89" s="21"/>
       <c r="C89" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="10" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B90" s="21"/>
       <c r="C90" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="10" t="s">
-        <v>453</v>
+        <v>461</v>
       </c>
       <c r="B91" s="21"/>
       <c r="C91" s="9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="10" t="s">
-        <v>405</v>
+        <v>453</v>
       </c>
       <c r="B92" s="21"/>
       <c r="C92" s="9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="10" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
       <c r="B93" s="21"/>
       <c r="C93" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="10" t="s">
-        <v>462</v>
+        <v>414</v>
       </c>
       <c r="B94" s="21"/>
       <c r="C94" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="10" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B95" s="21"/>
       <c r="C95" s="9" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="10" t="s">
-        <v>391</v>
+        <v>463</v>
       </c>
       <c r="B96" s="21"/>
       <c r="C96" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="10" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B97" s="21"/>
       <c r="C97" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="10" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B98" s="21"/>
       <c r="C98" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="10" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B99" s="21"/>
       <c r="C99" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="10" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B100" s="21"/>
       <c r="C100" s="9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="10" t="s">
-        <v>464</v>
+        <v>395</v>
       </c>
       <c r="B101" s="21"/>
       <c r="C101" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="10" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B102" s="21"/>
       <c r="C102" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="10" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B103" s="21"/>
       <c r="C103" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="10" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B104" s="21"/>
       <c r="C104" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="10" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B105" s="21"/>
       <c r="C105" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="10" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B106" s="21"/>
       <c r="C106" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="10" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B107" s="21"/>
       <c r="C107" s="9" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="10" t="s">
-        <v>415</v>
+        <v>470</v>
       </c>
       <c r="B108" s="21"/>
       <c r="C108" s="9" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A109" s="10" t="s">
-        <v>471</v>
+        <v>415</v>
       </c>
       <c r="B109" s="21"/>
       <c r="C109" s="9" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="10" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B110" s="21"/>
       <c r="C110" s="9" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="10" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B111" s="21"/>
       <c r="C111" s="9" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="10" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B112" s="21"/>
       <c r="C112" s="9" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="10" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B113" s="21"/>
       <c r="C113" s="9" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="10" t="s">
-        <v>416</v>
+        <v>475</v>
       </c>
       <c r="B114" s="21"/>
       <c r="C114" s="9" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A115" s="10" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="B115" s="21"/>
       <c r="C115" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="10" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B116" s="21"/>
       <c r="C116" s="9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="10" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="B117" s="21"/>
       <c r="C117" s="9" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="10" t="s">
-        <v>417</v>
+        <v>429</v>
       </c>
       <c r="B118" s="21"/>
       <c r="C118" s="9" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A119" s="10" t="s">
-        <v>428</v>
+        <v>417</v>
       </c>
       <c r="B119" s="21"/>
       <c r="C119" s="9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="10" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B120" s="21"/>
       <c r="C120" s="9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="10" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B121" s="21"/>
       <c r="C121" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="10" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="B122" s="21"/>
       <c r="C122" s="9" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="10" t="s">
-        <v>418</v>
+        <v>425</v>
       </c>
       <c r="B123" s="21"/>
       <c r="C123" s="9" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A124" s="10" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="B124" s="21"/>
       <c r="C124" s="9" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="10" t="s">
-        <v>396</v>
+        <v>424</v>
       </c>
       <c r="B125" s="21"/>
       <c r="C125" s="9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="10" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B126" s="21"/>
       <c r="C126" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="10" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B127" s="21"/>
       <c r="C127" s="9" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="10" t="s">
-        <v>423</v>
+        <v>398</v>
       </c>
       <c r="B128" s="21"/>
       <c r="C128" s="9" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="10" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="B129" s="21"/>
       <c r="C129" s="9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="10" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="B130" s="21"/>
       <c r="C130" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="10" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="B131" s="21"/>
       <c r="C131" s="9" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B132" s="21"/>
       <c r="C132" s="9" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A133" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="B133" s="21"/>
+      <c r="C133" s="9" t="s">
         <v>341</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A133" s="10" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
@@ -5405,6 +5386,11 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="10" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139" s="10" t="s">
         <v>476</v>
       </c>
     </row>
@@ -5434,22 +5420,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
+        <v>495</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>496</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="C1" s="16" t="s">
         <v>497</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>498</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>499</v>
       </c>
-      <c r="E1" s="16" t="s">
-        <v>500</v>
-      </c>
       <c r="F1" s="26" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G1" s="10"/>
     </row>
@@ -5458,17 +5444,17 @@
         <v>4</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>146</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="G2" s="10"/>
     </row>
@@ -5477,17 +5463,17 @@
         <v>3</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>146</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="10" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G3" s="10"/>
     </row>
@@ -5496,19 +5482,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>146</v>
       </c>
       <c r="D4" s="10" t="s">
+        <v>506</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>507</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>508</v>
-      </c>
       <c r="F4" s="10" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G4" s="10"/>
     </row>
@@ -5517,17 +5503,17 @@
         <v>1</v>
       </c>
       <c r="B5" s="10" t="s">
+        <v>509</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>502</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>510</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>503</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>511</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="10" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G5" s="10"/>
     </row>
@@ -5624,7 +5610,7 @@
         <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -5644,7 +5630,7 @@
         <v>37</v>
       </c>
       <c r="F3" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
   </sheetData>
@@ -5881,16 +5867,16 @@
         <v>43</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>42</v>
       </c>
       <c r="E1" s="19" t="s">
+        <v>560</v>
+      </c>
+      <c r="F1" s="19" t="s">
         <v>561</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -5965,7 +5951,7 @@
         <v>43</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>42</v>
@@ -6052,10 +6038,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>409</v>
@@ -6064,53 +6050,53 @@
         <v>43</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F1" s="19" t="s">
         <v>212</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>528</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>529</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" t="s">
         <v>530</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>531</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>532</v>
       </c>
-      <c r="F2" t="s">
-        <v>533</v>
-      </c>
       <c r="G2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>539</v>
+      </c>
+      <c r="C3" t="s">
         <v>540</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>541</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>542</v>
       </c>
-      <c r="F3" t="s">
-        <v>543</v>
-      </c>
       <c r="G3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
   </sheetData>
@@ -6141,39 +6127,39 @@
         <v>43</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D1" s="19" t="s">
+        <v>518</v>
+      </c>
+      <c r="E1" s="19" t="s">
         <v>519</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>520</v>
       </c>
       <c r="F1" s="19" t="s">
         <v>76</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>521</v>
+      </c>
+      <c r="B2" t="s">
         <v>522</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>523</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>524</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>525</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>526</v>
-      </c>
-      <c r="F2" t="s">
-        <v>527</v>
       </c>
       <c r="G2" t="s">
         <v>53</v>
@@ -6181,13 +6167,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E3" t="s">
+        <v>525</v>
+      </c>
+      <c r="F3" t="s">
         <v>526</v>
-      </c>
-      <c r="F3" t="s">
-        <v>527</v>
       </c>
       <c r="G3" t="s">
         <v>62</v>
@@ -6229,25 +6215,25 @@
         <v>409</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>574</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>576</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>616</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -6264,19 +6250,19 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>578</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>579</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>580</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="I2" s="28" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>175</v>
@@ -6290,10 +6276,10 @@
         <v>137</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>6</v>
@@ -6302,13 +6288,13 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>175</v>
@@ -6320,65 +6306,65 @@
         <v>42</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>582</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>582</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>582</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>582</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>583</v>
-      </c>
       <c r="I4" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
       <c r="C5" s="13" t="s">
+        <v>583</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>584</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>573</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>574</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>575</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>576</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>616</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>577</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>585</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
       <c r="C6" s="13" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="28" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -6387,7 +6373,7 @@
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="13" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>0</v>
@@ -6412,7 +6398,7 @@
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="13" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>161</v>
@@ -6431,7 +6417,7 @@
         <v>165</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -6470,10 +6456,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>2</v>
@@ -6498,10 +6484,10 @@
         <v>8</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>2</v>
@@ -6516,10 +6502,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
+        <v>627</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>628</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>629</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
First cut IE M11 output
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/full_1.xlsx
+++ b/tests/integration_test_files/full_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83349F51-FF4A-8C4B-98E9-EF47684C7278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5BDE28F-252B-DF4C-AA1D-A8F9E895DE62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30200" yWindow="500" windowWidth="34860" windowHeight="20040" firstSheet="10" activeTab="18" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="62940" yWindow="5560" windowWidth="34860" windowHeight="20040" firstSheet="10" activeTab="18" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -1275,20 +1275,6 @@
     <t>8.1.1</t>
   </si>
   <si>
-    <t>&lt;p&gt;Inclusion criteria are:&lt;/p&gt;
-&lt;ul&gt;
-  &lt;li&gt;1. Something&lt;/li&gt;
-  &lt;li&gt;2. Something else&lt;/li&gt;
-&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Exclusion criteria are:&lt;/p&gt;
-&lt;ul&gt;
-  &lt;li&gt;1. Dont do this&lt;/li&gt;
-  &lt;li&gt;2. And don't do that&lt;/li&gt;
-&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Blinding and unblinding text here please&lt;/p&gt;</t>
   </si>
   <si>
@@ -1997,7 +1983,13 @@
     <t>0</t>
   </si>
   <si>
-    <t>section = M11-title-page</t>
+    <t>&lt;usdm:section name="M11-title-page"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;usdm:section name="M11-inclusion"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;usdm:section name="M11-exclusion"&gt;</t>
   </si>
 </sst>
 </file>
@@ -2157,10 +2149,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2495,10 +2487,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2607,94 +2599,94 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>43</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E16" s="19" t="s">
         <v>42</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>482</v>
+      </c>
+      <c r="C17" t="s">
         <v>483</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="D17" t="s">
         <v>484</v>
       </c>
-      <c r="C17" t="s">
-        <v>485</v>
-      </c>
-      <c r="D17" t="s">
-        <v>486</v>
-      </c>
       <c r="E17" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="F17" s="24">
         <v>44927</v>
       </c>
       <c r="G17" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
+        <v>486</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>482</v>
+      </c>
+      <c r="C18" t="s">
+        <v>487</v>
+      </c>
+      <c r="D18" t="s">
         <v>488</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>484</v>
-      </c>
-      <c r="C18" t="s">
-        <v>489</v>
-      </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>490</v>
-      </c>
-      <c r="E18" t="s">
-        <v>492</v>
       </c>
       <c r="F18" s="24">
         <v>44927</v>
       </c>
       <c r="G18" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
+        <v>486</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>482</v>
+      </c>
+      <c r="C19" t="s">
+        <v>487</v>
+      </c>
+      <c r="D19" t="s">
         <v>488</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>484</v>
-      </c>
-      <c r="C19" t="s">
-        <v>489</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>490</v>
-      </c>
-      <c r="E19" t="s">
-        <v>492</v>
       </c>
       <c r="F19" s="24">
         <v>44958</v>
       </c>
       <c r="G19" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
   </sheetData>
@@ -2719,196 +2711,196 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>43</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>42</v>
       </c>
       <c r="E1" s="19" t="s">
+        <v>586</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>587</v>
+      </c>
+      <c r="G1" s="19" t="s">
         <v>588</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="H1" s="19" t="s">
         <v>589</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="I1" s="19" t="s">
         <v>590</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>591</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="B2" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>593</v>
+      </c>
+      <c r="E2" t="s">
+        <v>569</v>
+      </c>
+      <c r="F2" t="s">
+        <v>570</v>
+      </c>
+      <c r="G2" t="s">
+        <v>594</v>
+      </c>
+      <c r="H2" t="s">
         <v>595</v>
-      </c>
-      <c r="E2" t="s">
-        <v>571</v>
-      </c>
-      <c r="F2" t="s">
-        <v>572</v>
-      </c>
-      <c r="G2" t="s">
-        <v>596</v>
-      </c>
-      <c r="H2" t="s">
-        <v>597</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>596</v>
+      </c>
+      <c r="B3" t="s">
+        <v>597</v>
+      </c>
+      <c r="C3" t="s">
         <v>598</v>
       </c>
-      <c r="B3" t="s">
-        <v>599</v>
-      </c>
-      <c r="C3" t="s">
-        <v>600</v>
-      </c>
       <c r="D3" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="E3" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="F3" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
       </c>
       <c r="H3" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>600</v>
+      </c>
+      <c r="B4" t="s">
+        <v>601</v>
+      </c>
+      <c r="C4" t="s">
+        <v>576</v>
+      </c>
+      <c r="D4" t="s">
         <v>602</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
+        <v>571</v>
+      </c>
+      <c r="F4" t="s">
+        <v>571</v>
+      </c>
+      <c r="G4" t="s">
         <v>603</v>
-      </c>
-      <c r="C4" t="s">
-        <v>578</v>
-      </c>
-      <c r="D4" t="s">
-        <v>604</v>
-      </c>
-      <c r="E4" t="s">
-        <v>573</v>
-      </c>
-      <c r="F4" t="s">
-        <v>573</v>
-      </c>
-      <c r="G4" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>604</v>
+      </c>
+      <c r="B5" t="s">
+        <v>605</v>
+      </c>
+      <c r="C5" t="s">
+        <v>577</v>
+      </c>
+      <c r="D5" t="s">
         <v>606</v>
       </c>
-      <c r="B5" t="s">
+      <c r="E5" t="s">
+        <v>572</v>
+      </c>
+      <c r="F5" t="s">
+        <v>571</v>
+      </c>
+      <c r="G5" t="s">
         <v>607</v>
       </c>
-      <c r="C5" t="s">
-        <v>579</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="H5" t="s">
+        <v>595</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>608</v>
-      </c>
-      <c r="E5" t="s">
-        <v>574</v>
-      </c>
-      <c r="F5" t="s">
-        <v>573</v>
-      </c>
-      <c r="G5" t="s">
-        <v>609</v>
-      </c>
-      <c r="H5" t="s">
-        <v>597</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>610</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>604</v>
+      </c>
+      <c r="B6" t="s">
+        <v>619</v>
+      </c>
+      <c r="C6" t="s">
+        <v>612</v>
+      </c>
+      <c r="D6" t="s">
         <v>606</v>
       </c>
-      <c r="B6" t="s">
-        <v>621</v>
-      </c>
-      <c r="C6" t="s">
-        <v>614</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
+        <v>613</v>
+      </c>
+      <c r="F6" t="s">
+        <v>571</v>
+      </c>
+      <c r="G6" t="s">
+        <v>620</v>
+      </c>
+      <c r="H6" t="s">
+        <v>595</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>608</v>
-      </c>
-      <c r="E6" t="s">
-        <v>615</v>
-      </c>
-      <c r="F6" t="s">
-        <v>573</v>
-      </c>
-      <c r="G6" t="s">
-        <v>622</v>
-      </c>
-      <c r="H6" t="s">
-        <v>597</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>610</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="B7" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="C7" t="s">
         <v>175</v>
       </c>
       <c r="D7" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="E7" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="F7" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="G7" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="H7" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
   </sheetData>
@@ -2936,13 +2928,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>43</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D1" s="25" t="s">
         <v>208</v>
@@ -2964,41 +2956,41 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="B3" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B4" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>146</v>
       </c>
       <c r="E4" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>625</v>
+      </c>
+      <c r="B5" t="s">
         <v>627</v>
       </c>
-      <c r="B5" t="s">
-        <v>629</v>
-      </c>
       <c r="C5" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -3029,7 +3021,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>42</v>
@@ -3046,7 +3038,7 @@
         <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C2" t="s">
         <v>45</v>
@@ -3060,7 +3052,7 @@
         <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C3" t="s">
         <v>45</v>
@@ -3074,7 +3066,7 @@
         <v>78</v>
       </c>
       <c r="B4" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C4" t="s">
         <v>47</v>
@@ -3088,7 +3080,7 @@
         <v>80</v>
       </c>
       <c r="B5" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C5" t="s">
         <v>47</v>
@@ -3121,7 +3113,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>51</v>
@@ -3143,10 +3135,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="B2" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -3163,10 +3155,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="B3" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C3">
         <v>20</v>
@@ -3183,10 +3175,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B4" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C4">
         <v>20</v>
@@ -3231,34 +3223,34 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>63</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>64</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="G1" s="19" t="s">
         <v>65</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="I1" s="19" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="J1" s="19" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="K1" s="19" t="s">
         <v>66</v>
@@ -3269,7 +3261,7 @@
         <v>82</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -3282,7 +3274,7 @@
         <v>84</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="H2" s="12"/>
       <c r="I2" s="12" t="s">
@@ -3298,7 +3290,7 @@
         <v>83</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12" t="s">
@@ -3311,7 +3303,7 @@
         <v>85</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="H3" s="12"/>
       <c r="I3" s="12" t="s">
@@ -3332,7 +3324,7 @@
         <v>86</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12" t="s">
@@ -3636,7 +3628,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="27" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B1" s="27" t="s">
         <v>87</v>
@@ -3721,7 +3713,7 @@
         <v>92</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>126</v>
@@ -3733,7 +3725,7 @@
         <v>85</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
   </sheetData>
@@ -3763,13 +3755,13 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>43</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>138</v>
@@ -3789,13 +3781,13 @@
         <v>142</v>
       </c>
       <c r="B2" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C2" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="D2" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="E2" t="s">
         <v>143</v>
@@ -3806,13 +3798,13 @@
         <v>144</v>
       </c>
       <c r="B3" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C3" t="s">
+        <v>563</v>
+      </c>
+      <c r="D3" t="s">
         <v>565</v>
-      </c>
-      <c r="D3" t="s">
-        <v>567</v>
       </c>
       <c r="E3" t="s">
         <v>145</v>
@@ -3821,7 +3813,7 @@
         <v>146</v>
       </c>
       <c r="G3" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -3857,22 +3849,22 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>43</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>42</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="G1" s="19" t="s">
         <v>148</v>
@@ -3958,7 +3950,7 @@
         <v>153</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>154</v>
@@ -3975,10 +3967,10 @@
         <v>165</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>154</v>
@@ -3992,13 +3984,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>154</v>
@@ -4035,13 +4027,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>169</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>148</v>
@@ -4145,8 +4137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F40359-1191-3843-B5C3-38D19A754655}">
   <dimension ref="A1:D139"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4159,10 +4151,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C1" s="20" t="s">
         <v>211</v>
@@ -4173,14 +4165,14 @@
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="9" t="s">
+        <v>637</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>639</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -4250,13 +4242,13 @@
     </row>
     <row r="11" spans="1:4" ht="113" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
+        <v>475</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>476</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>477</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>478</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>479</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -4322,7 +4314,7 @@
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="B19" s="21"/>
       <c r="C19" s="9" t="s">
@@ -4331,7 +4323,7 @@
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="B20" s="21"/>
       <c r="C20" s="9" t="s">
@@ -4340,7 +4332,7 @@
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B21" s="21"/>
       <c r="C21" s="9" t="s">
@@ -4349,7 +4341,7 @@
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B22" s="21"/>
       <c r="C22" s="9" t="s">
@@ -4358,40 +4350,40 @@
     </row>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B23" s="21"/>
       <c r="C23" s="9" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="B24" s="21"/>
       <c r="C24" s="9" t="s">
         <v>233</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="85" x14ac:dyDescent="0.2">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B25" s="21"/>
       <c r="C25" s="9" t="s">
         <v>234</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>407</v>
+        <v>641</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B26" s="21"/>
       <c r="C26" s="9" t="s">
@@ -4436,7 +4428,7 @@
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="B31" s="21"/>
       <c r="C31" s="9" t="s">
@@ -4445,7 +4437,7 @@
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="B32" s="21"/>
       <c r="C32" s="9" t="s">
@@ -4454,7 +4446,7 @@
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="B33" s="21"/>
       <c r="C33" s="9" t="s">
@@ -4463,7 +4455,7 @@
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="B34" s="21"/>
       <c r="C34" s="9" t="s">
@@ -4472,7 +4464,7 @@
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="B35" s="21"/>
       <c r="C35" s="9" t="s">
@@ -4490,7 +4482,7 @@
     </row>
     <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B37" s="21"/>
       <c r="C37" s="9" t="s">
@@ -4499,7 +4491,7 @@
     </row>
     <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="B38" s="21"/>
       <c r="C38" s="9" t="s">
@@ -4535,7 +4527,7 @@
     </row>
     <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B42" s="21"/>
       <c r="C42" s="9" t="s">
@@ -4569,12 +4561,12 @@
         <v>254</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="B46" s="21"/>
       <c r="C46" s="9" t="s">
@@ -4583,7 +4575,7 @@
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="B47" s="21"/>
       <c r="C47" s="9" t="s">
@@ -4628,7 +4620,7 @@
     </row>
     <row r="52" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="B52" s="21"/>
       <c r="C52" s="9" t="s">
@@ -4637,7 +4629,7 @@
     </row>
     <row r="53" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="10" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B53" s="21"/>
       <c r="C53" s="9" t="s">
@@ -4673,7 +4665,7 @@
     </row>
     <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="B57" s="21"/>
       <c r="C57" s="9" t="s">
@@ -4682,7 +4674,7 @@
     </row>
     <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B58" s="21"/>
       <c r="C58" s="9" t="s">
@@ -4691,7 +4683,7 @@
     </row>
     <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B59" s="21"/>
       <c r="C59" s="9" t="s">
@@ -4700,7 +4692,7 @@
     </row>
     <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="10" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B60" s="21"/>
       <c r="C60" s="9" t="s">
@@ -4709,7 +4701,7 @@
     </row>
     <row r="61" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="10" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B61" s="21"/>
       <c r="C61" s="9" t="s">
@@ -4718,7 +4710,7 @@
     </row>
     <row r="62" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="10" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B62" s="21"/>
       <c r="C62" s="9" t="s">
@@ -4727,7 +4719,7 @@
     </row>
     <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="10" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B63" s="21"/>
       <c r="C63" s="9" t="s">
@@ -4781,7 +4773,7 @@
     </row>
     <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="10" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="B69" s="21"/>
       <c r="C69" s="9" t="s">
@@ -4880,7 +4872,7 @@
     </row>
     <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="10" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="B80" s="21"/>
       <c r="C80" s="9" t="s">
@@ -4907,7 +4899,7 @@
     </row>
     <row r="83" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A83" s="10" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="B83" s="21"/>
       <c r="C83" s="9" t="s">
@@ -4961,7 +4953,7 @@
     </row>
     <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="10" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B89" s="21"/>
       <c r="C89" s="9" t="s">
@@ -4970,7 +4962,7 @@
     </row>
     <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="10" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="B90" s="21"/>
       <c r="C90" s="9" t="s">
@@ -4979,7 +4971,7 @@
     </row>
     <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="10" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B91" s="21"/>
       <c r="C91" s="9" t="s">
@@ -4988,7 +4980,7 @@
     </row>
     <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="10" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="B92" s="21"/>
       <c r="C92" s="9" t="s">
@@ -5006,7 +4998,7 @@
     </row>
     <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="10" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B94" s="21"/>
       <c r="C94" s="9" t="s">
@@ -5015,7 +5007,7 @@
     </row>
     <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="10" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="B95" s="21"/>
       <c r="C95" s="9" t="s">
@@ -5024,7 +5016,7 @@
     </row>
     <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="10" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="B96" s="21"/>
       <c r="C96" s="9" t="s">
@@ -5078,7 +5070,7 @@
     </row>
     <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="10" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B102" s="21"/>
       <c r="C102" s="9" t="s">
@@ -5087,7 +5079,7 @@
     </row>
     <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="10" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="B103" s="21"/>
       <c r="C103" s="9" t="s">
@@ -5096,7 +5088,7 @@
     </row>
     <row r="104" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="10" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="B104" s="21"/>
       <c r="C104" s="9" t="s">
@@ -5105,7 +5097,7 @@
     </row>
     <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="10" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="B105" s="21"/>
       <c r="C105" s="9" t="s">
@@ -5114,7 +5106,7 @@
     </row>
     <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="10" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B106" s="21"/>
       <c r="C106" s="9" t="s">
@@ -5123,7 +5115,7 @@
     </row>
     <row r="107" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="10" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B107" s="21"/>
       <c r="C107" s="9" t="s">
@@ -5132,7 +5124,7 @@
     </row>
     <row r="108" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="10" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="B108" s="21"/>
       <c r="C108" s="9" t="s">
@@ -5141,7 +5133,7 @@
     </row>
     <row r="109" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A109" s="10" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B109" s="21"/>
       <c r="C109" s="9" t="s">
@@ -5150,7 +5142,7 @@
     </row>
     <row r="110" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="10" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="B110" s="21"/>
       <c r="C110" s="9" t="s">
@@ -5159,7 +5151,7 @@
     </row>
     <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="10" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B111" s="21"/>
       <c r="C111" s="9" t="s">
@@ -5168,7 +5160,7 @@
     </row>
     <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="10" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="B112" s="21"/>
       <c r="C112" s="9" t="s">
@@ -5177,7 +5169,7 @@
     </row>
     <row r="113" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="10" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B113" s="21"/>
       <c r="C113" s="9" t="s">
@@ -5186,7 +5178,7 @@
     </row>
     <row r="114" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="10" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B114" s="21"/>
       <c r="C114" s="9" t="s">
@@ -5195,7 +5187,7 @@
     </row>
     <row r="115" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A115" s="10" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="B115" s="21"/>
       <c r="C115" s="9" t="s">
@@ -5204,7 +5196,7 @@
     </row>
     <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="10" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B116" s="21"/>
       <c r="C116" s="9" t="s">
@@ -5213,7 +5205,7 @@
     </row>
     <row r="117" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="10" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="B117" s="21"/>
       <c r="C117" s="9" t="s">
@@ -5222,7 +5214,7 @@
     </row>
     <row r="118" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="10" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="B118" s="21"/>
       <c r="C118" s="9" t="s">
@@ -5231,7 +5223,7 @@
     </row>
     <row r="119" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A119" s="10" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="B119" s="21"/>
       <c r="C119" s="9" t="s">
@@ -5240,7 +5232,7 @@
     </row>
     <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="10" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="B120" s="21"/>
       <c r="C120" s="9" t="s">
@@ -5249,7 +5241,7 @@
     </row>
     <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="10" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="B121" s="21"/>
       <c r="C121" s="9" t="s">
@@ -5258,7 +5250,7 @@
     </row>
     <row r="122" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="10" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="B122" s="21"/>
       <c r="C122" s="9" t="s">
@@ -5267,7 +5259,7 @@
     </row>
     <row r="123" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="10" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="B123" s="21"/>
       <c r="C123" s="9" t="s">
@@ -5276,7 +5268,7 @@
     </row>
     <row r="124" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A124" s="10" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B124" s="21"/>
       <c r="C124" s="9" t="s">
@@ -5285,7 +5277,7 @@
     </row>
     <row r="125" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="10" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="B125" s="21"/>
       <c r="C125" s="9" t="s">
@@ -5321,7 +5313,7 @@
     </row>
     <row r="129" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="10" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="B129" s="21"/>
       <c r="C129" s="9" t="s">
@@ -5330,7 +5322,7 @@
     </row>
     <row r="130" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="10" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B130" s="21"/>
       <c r="C130" s="9" t="s">
@@ -5339,7 +5331,7 @@
     </row>
     <row r="131" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="10" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="B131" s="21"/>
       <c r="C131" s="9" t="s">
@@ -5348,7 +5340,7 @@
     </row>
     <row r="132" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="10" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="B132" s="21"/>
       <c r="C132" s="9" t="s">
@@ -5357,7 +5349,7 @@
     </row>
     <row r="133" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" s="10" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B133" s="21"/>
       <c r="C133" s="9" t="s">
@@ -5366,32 +5358,32 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="10" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="10" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="10" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="10" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="10" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="10" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
   </sheetData>
@@ -5420,22 +5412,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
+        <v>493</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>494</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>495</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>496</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>497</v>
       </c>
-      <c r="D1" s="16" t="s">
-        <v>498</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>499</v>
-      </c>
       <c r="F1" s="26" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="G1" s="10"/>
     </row>
@@ -5444,17 +5436,17 @@
         <v>4</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>146</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="G2" s="10"/>
     </row>
@@ -5463,17 +5455,17 @@
         <v>3</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>146</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="10" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="G3" s="10"/>
     </row>
@@ -5482,19 +5474,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>146</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="G4" s="10"/>
     </row>
@@ -5503,17 +5495,17 @@
         <v>1</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="10" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="G5" s="10"/>
     </row>
@@ -5610,7 +5602,7 @@
         <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -5630,7 +5622,7 @@
         <v>37</v>
       </c>
       <c r="F3" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
   </sheetData>
@@ -5679,34 +5671,34 @@
       <c r="A3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="30" t="s">
         <v>147</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="30" t="s">
         <v>115</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
@@ -5826,16 +5818,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5861,22 +5853,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>43</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>42</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -5945,13 +5937,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>43</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>42</v>
@@ -6038,65 +6030,65 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>43</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="F1" s="19" t="s">
         <v>212</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>526</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>527</v>
+      </c>
+      <c r="C2" t="s">
         <v>528</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="D2" t="s">
         <v>529</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" t="s">
         <v>530</v>
       </c>
-      <c r="D2" t="s">
-        <v>531</v>
-      </c>
-      <c r="F2" t="s">
-        <v>532</v>
-      </c>
       <c r="G2" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>537</v>
+      </c>
+      <c r="C3" t="s">
+        <v>538</v>
+      </c>
+      <c r="D3" t="s">
         <v>539</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>540</v>
       </c>
-      <c r="D3" t="s">
-        <v>541</v>
-      </c>
-      <c r="F3" t="s">
-        <v>542</v>
-      </c>
       <c r="G3" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
     </row>
   </sheetData>
@@ -6121,45 +6113,45 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>43</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F1" s="19" t="s">
         <v>76</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>519</v>
+      </c>
+      <c r="B2" t="s">
+        <v>520</v>
+      </c>
+      <c r="C2" t="s">
         <v>521</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>522</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>523</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>524</v>
-      </c>
-      <c r="E2" t="s">
-        <v>525</v>
-      </c>
-      <c r="F2" t="s">
-        <v>526</v>
       </c>
       <c r="G2" t="s">
         <v>53</v>
@@ -6167,13 +6159,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="E3" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="F3" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="G3" t="s">
         <v>62</v>
@@ -6212,28 +6204,28 @@
         <v>133</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>571</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>574</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>575</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>615</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -6250,19 +6242,19 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>575</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>576</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>577</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>578</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>579</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="I2" s="28" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>175</v>
@@ -6276,10 +6268,10 @@
         <v>137</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>6</v>
@@ -6288,13 +6280,13 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>175</v>
@@ -6306,65 +6298,65 @@
         <v>42</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
       <c r="C5" s="13" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="H5" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>574</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>575</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>615</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>576</v>
-      </c>
       <c r="J5" s="2" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
       <c r="C6" s="13" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="28" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -6373,7 +6365,7 @@
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="13" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>0</v>
@@ -6398,7 +6390,7 @@
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="13" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>161</v>
@@ -6417,7 +6409,7 @@
         <v>165</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -6456,10 +6448,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>2</v>
@@ -6484,10 +6476,10 @@
         <v>8</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>2</v>
@@ -6502,10 +6494,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Next cut for criteria
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/full_1.xlsx
+++ b/tests/integration_test_files/full_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5BDE28F-252B-DF4C-AA1D-A8F9E895DE62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E33B31BB-7ED5-8742-9D78-7F2003425A72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="62940" yWindow="5560" windowWidth="34860" windowHeight="20040" firstSheet="10" activeTab="18" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="62940" yWindow="5560" windowWidth="34860" windowHeight="20040" firstSheet="2" activeTab="6" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="646">
   <si>
     <t>Screening</t>
   </si>
@@ -1990,6 +1990,18 @@
   </si>
   <si>
     <t>&lt;usdm:section name="M11-exclusion"&gt;</t>
+  </si>
+  <si>
+    <t>Exclusion</t>
+  </si>
+  <si>
+    <t>Drug A</t>
+  </si>
+  <si>
+    <t>Ever taken drug A</t>
+  </si>
+  <si>
+    <t>Subjects has been treated with Drug A at any time in the past</t>
   </si>
 </sst>
 </file>
@@ -4137,8 +4149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F40359-1191-3843-B5C3-38D19A754655}">
   <dimension ref="A1:D139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="A11" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6012,10 +6024,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED1B92D-F8EC-D24D-81E6-6B85449D22F0}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6023,7 +6035,7 @@
     <col min="1" max="1" width="13.1640625" customWidth="1"/>
     <col min="2" max="2" width="10.1640625" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="4" max="4" width="29.5" customWidth="1"/>
     <col min="5" max="5" width="10.1640625" customWidth="1"/>
     <col min="6" max="6" width="64.83203125" customWidth="1"/>
   </cols>
@@ -6089,6 +6101,23 @@
       </c>
       <c r="G3" t="s">
         <v>519</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>642</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>527</v>
+      </c>
+      <c r="C4" t="s">
+        <v>643</v>
+      </c>
+      <c r="D4" t="s">
+        <v>644</v>
+      </c>
+      <c r="F4" t="s">
+        <v>645</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add syntax support for Objectives and Endpoints
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/full_1.xlsx
+++ b/tests/integration_test_files/full_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1374DD37-736B-CE49-9011-0CF2CDBE2399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDF2412-6191-1E44-9783-14C3003D13F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="62940" yWindow="5560" windowWidth="34860" windowHeight="20040" firstSheet="3" activeTab="6" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="51660" yWindow="5560" windowWidth="46140" windowHeight="20040" firstSheet="7" activeTab="13" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="651">
   <si>
     <t>Screening</t>
   </si>
@@ -268,9 +268,6 @@
   </si>
   <si>
     <t>Primary Endpoint</t>
-  </si>
-  <si>
-    <t>The secondary efficacy objective for this study is to evaluate the efficacy of TCZ compared with placebo in combination with SOC for the treatment of severe COVID-19 pneumonia</t>
   </si>
   <si>
     <t>Study Secondary Objective</t>
@@ -2002,6 +1999,24 @@
   </si>
   <si>
     <t>Subjects has been treated with Drug A at any time in the past</t>
+  </si>
+  <si>
+    <t>objectiveDictionary</t>
+  </si>
+  <si>
+    <t>endpointDictionary</t>
+  </si>
+  <si>
+    <t>OE_Dict</t>
+  </si>
+  <si>
+    <t>Dictionary for OE</t>
+  </si>
+  <si>
+    <t>OE Dictionary</t>
+  </si>
+  <si>
+    <t>The secondary efficacy objective for this study is to evaluate the efficacy of TCZ compared with placebo in combination with SOC for the treatment of severe COVID-19 pneumonia over the age of [min_age]</t>
   </si>
 </sst>
 </file>
@@ -2499,10 +2514,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2539,63 +2554,63 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>113</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>13</v>
@@ -2603,102 +2618,102 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>43</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E16" s="19" t="s">
         <v>42</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
+        <v>480</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>481</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="C17" t="s">
         <v>482</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>483</v>
       </c>
-      <c r="D17" t="s">
-        <v>484</v>
-      </c>
       <c r="E17" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F17" s="24">
         <v>44927</v>
       </c>
       <c r="G17" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
+        <v>485</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="C18" t="s">
         <v>486</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>482</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>487</v>
       </c>
-      <c r="D18" t="s">
-        <v>488</v>
-      </c>
       <c r="E18" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="F18" s="24">
         <v>44927</v>
       </c>
       <c r="G18" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
+        <v>485</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="C19" t="s">
         <v>486</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>482</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>487</v>
       </c>
-      <c r="D19" t="s">
-        <v>488</v>
-      </c>
       <c r="E19" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="F19" s="24">
         <v>44958</v>
       </c>
       <c r="G19" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
   </sheetData>
@@ -2723,196 +2738,196 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>43</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>42</v>
       </c>
       <c r="E1" s="19" t="s">
+        <v>585</v>
+      </c>
+      <c r="F1" s="19" t="s">
         <v>586</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="G1" s="19" t="s">
         <v>587</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="H1" s="19" t="s">
         <v>588</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="I1" s="19" t="s">
         <v>589</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>590</v>
+      </c>
+      <c r="B2" t="s">
         <v>591</v>
-      </c>
-      <c r="B2" t="s">
-        <v>592</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>592</v>
+      </c>
+      <c r="E2" t="s">
+        <v>568</v>
+      </c>
+      <c r="F2" t="s">
+        <v>569</v>
+      </c>
+      <c r="G2" t="s">
         <v>593</v>
       </c>
-      <c r="E2" t="s">
-        <v>569</v>
-      </c>
-      <c r="F2" t="s">
-        <v>570</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>594</v>
-      </c>
-      <c r="H2" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>595</v>
+      </c>
+      <c r="B3" t="s">
         <v>596</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>597</v>
       </c>
-      <c r="C3" t="s">
-        <v>598</v>
-      </c>
       <c r="D3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E3" t="s">
+        <v>569</v>
+      </c>
+      <c r="F3" t="s">
         <v>570</v>
-      </c>
-      <c r="F3" t="s">
-        <v>571</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
       </c>
       <c r="H3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>599</v>
+      </c>
+      <c r="B4" t="s">
         <v>600</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>575</v>
+      </c>
+      <c r="D4" t="s">
         <v>601</v>
       </c>
-      <c r="C4" t="s">
-        <v>576</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>570</v>
+      </c>
+      <c r="F4" t="s">
+        <v>570</v>
+      </c>
+      <c r="G4" t="s">
         <v>602</v>
-      </c>
-      <c r="E4" t="s">
-        <v>571</v>
-      </c>
-      <c r="F4" t="s">
-        <v>571</v>
-      </c>
-      <c r="G4" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>603</v>
+      </c>
+      <c r="B5" t="s">
         <v>604</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>576</v>
+      </c>
+      <c r="D5" t="s">
         <v>605</v>
       </c>
-      <c r="C5" t="s">
-        <v>577</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>571</v>
+      </c>
+      <c r="F5" t="s">
+        <v>570</v>
+      </c>
+      <c r="G5" t="s">
         <v>606</v>
       </c>
-      <c r="E5" t="s">
-        <v>572</v>
-      </c>
-      <c r="F5" t="s">
-        <v>571</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
+        <v>594</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>607</v>
-      </c>
-      <c r="H5" t="s">
-        <v>595</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B6" t="s">
+        <v>618</v>
+      </c>
+      <c r="C6" t="s">
+        <v>611</v>
+      </c>
+      <c r="D6" t="s">
+        <v>605</v>
+      </c>
+      <c r="E6" t="s">
+        <v>612</v>
+      </c>
+      <c r="F6" t="s">
+        <v>570</v>
+      </c>
+      <c r="G6" t="s">
         <v>619</v>
       </c>
-      <c r="C6" t="s">
-        <v>612</v>
-      </c>
-      <c r="D6" t="s">
-        <v>606</v>
-      </c>
-      <c r="E6" t="s">
-        <v>613</v>
-      </c>
-      <c r="F6" t="s">
-        <v>571</v>
-      </c>
-      <c r="G6" t="s">
-        <v>620</v>
-      </c>
       <c r="H6" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>608</v>
+      </c>
+      <c r="B7" t="s">
         <v>609</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
+        <v>174</v>
+      </c>
+      <c r="D7" t="s">
+        <v>605</v>
+      </c>
+      <c r="E7" t="s">
+        <v>573</v>
+      </c>
+      <c r="F7" t="s">
+        <v>570</v>
+      </c>
+      <c r="G7" t="s">
+        <v>620</v>
+      </c>
+      <c r="H7" t="s">
+        <v>594</v>
+      </c>
+      <c r="I7" s="6" t="s">
         <v>610</v>
-      </c>
-      <c r="C7" t="s">
-        <v>175</v>
-      </c>
-      <c r="D7" t="s">
-        <v>606</v>
-      </c>
-      <c r="E7" t="s">
-        <v>574</v>
-      </c>
-      <c r="F7" t="s">
-        <v>571</v>
-      </c>
-      <c r="G7" t="s">
-        <v>621</v>
-      </c>
-      <c r="H7" t="s">
-        <v>595</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>611</v>
       </c>
     </row>
   </sheetData>
@@ -2940,19 +2955,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>43</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D1" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="E1" s="19" t="s">
         <v>208</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2960,7 +2975,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
@@ -2968,41 +2983,41 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>628</v>
+      </c>
+      <c r="B3" t="s">
         <v>629</v>
       </c>
-      <c r="B3" t="s">
-        <v>630</v>
-      </c>
       <c r="C3" s="4" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B4" t="s">
+        <v>630</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>631</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>632</v>
-      </c>
       <c r="D4" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E4" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B5" t="s">
+        <v>626</v>
+      </c>
+      <c r="C5" t="s">
         <v>627</v>
-      </c>
-      <c r="C5" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -3033,7 +3048,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>42</v>
@@ -3047,10 +3062,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C2" t="s">
         <v>45</v>
@@ -3061,10 +3076,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C3" t="s">
         <v>45</v>
@@ -3075,10 +3090,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C4" t="s">
         <v>47</v>
@@ -3089,10 +3104,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C5" t="s">
         <v>47</v>
@@ -3125,7 +3140,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>51</v>
@@ -3147,10 +3162,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B2" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -3167,10 +3182,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C3">
         <v>20</v>
@@ -3187,10 +3202,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C4">
         <v>20</v>
@@ -3212,10 +3227,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B908C5D6-C6A1-4043-A49A-69C599CFBAE9}">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3224,56 +3239,63 @@
     <col min="2" max="2" width="20.1640625" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" customWidth="1"/>
     <col min="4" max="4" width="40.83203125" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="22.83203125" customWidth="1"/>
-    <col min="8" max="8" width="15.5" customWidth="1"/>
-    <col min="9" max="9" width="48.6640625" customWidth="1"/>
-    <col min="10" max="10" width="18.33203125" customWidth="1"/>
-    <col min="11" max="11" width="21.1640625" customWidth="1"/>
+    <col min="5" max="6" width="24.6640625" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="22.83203125" customWidth="1"/>
+    <col min="9" max="9" width="15.5" customWidth="1"/>
+    <col min="10" max="10" width="48.6640625" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" customWidth="1"/>
+    <col min="12" max="12" width="21.1640625" customWidth="1"/>
+    <col min="13" max="13" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>63</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>64</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>541</v>
+        <v>645</v>
       </c>
       <c r="G1" s="19" t="s">
+        <v>540</v>
+      </c>
+      <c r="H1" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="I1" s="19" t="s">
+        <v>542</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>545</v>
+      </c>
+      <c r="K1" s="19" t="s">
         <v>543</v>
       </c>
-      <c r="I1" s="19" t="s">
-        <v>546</v>
-      </c>
-      <c r="J1" s="19" t="s">
-        <v>544</v>
-      </c>
-      <c r="K1" s="19" t="s">
+      <c r="L1" s="19" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+      <c r="M1" s="19" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -3282,72 +3304,77 @@
       <c r="E2" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="12" t="s">
-        <v>84</v>
-      </c>
+      <c r="F2" s="12"/>
       <c r="G2" s="12" t="s">
-        <v>547</v>
-      </c>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>546</v>
+      </c>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="J2" s="10"/>
-      <c r="K2" s="12" t="s">
+      <c r="K2" s="10"/>
+      <c r="L2" s="12" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="85" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12" t="s">
+        <v>650</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="F3" s="12" t="s">
+        <v>647</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>547</v>
+      </c>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>548</v>
-      </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="K3" s="10"/>
+      <c r="L3" s="12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
-      <c r="F4" s="12" t="s">
-        <v>86</v>
-      </c>
+      <c r="F4" s="12"/>
       <c r="G4" s="12" t="s">
-        <v>549</v>
-      </c>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>548</v>
+      </c>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="K4" s="10"/>
+      <c r="L4" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="J4" s="10"/>
-      <c r="K4" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
@@ -3358,8 +3385,9 @@
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5" s="9"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -3370,8 +3398,9 @@
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6" s="9"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
       <c r="D7" s="9"/>
@@ -3382,8 +3411,9 @@
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7" s="9"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -3394,8 +3424,9 @@
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8" s="9"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
@@ -3406,8 +3437,9 @@
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9" s="9"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
@@ -3418,8 +3450,9 @@
       <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10" s="9"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -3430,8 +3463,9 @@
       <c r="I11" s="9"/>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11" s="9"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -3442,8 +3476,9 @@
       <c r="I12" s="9"/>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -3454,8 +3489,9 @@
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L13" s="9"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
@@ -3466,8 +3502,9 @@
       <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L14" s="9"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -3478,8 +3515,9 @@
       <c r="I15" s="9"/>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L15" s="9"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
@@ -3490,8 +3528,9 @@
       <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L16" s="9"/>
+    </row>
+    <row r="17" spans="2:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
@@ -3502,8 +3541,9 @@
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L17" s="9"/>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
@@ -3514,8 +3554,9 @@
       <c r="I18" s="9"/>
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L18" s="9"/>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -3526,8 +3567,9 @@
       <c r="I19" s="9"/>
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L19" s="9"/>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -3538,8 +3580,9 @@
       <c r="I20" s="9"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L20" s="9"/>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
@@ -3550,8 +3593,9 @@
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L21" s="9"/>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
@@ -3562,8 +3606,9 @@
       <c r="I22" s="9"/>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L22" s="9"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -3574,8 +3619,9 @@
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L23" s="9"/>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -3586,8 +3632,9 @@
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L24" s="9"/>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
@@ -3598,8 +3645,9 @@
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="L25" s="9"/>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
@@ -3610,6 +3658,7 @@
       <c r="I26" s="9"/>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
+      <c r="L26" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -3640,54 +3689,54 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="27" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B1" s="27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C1" s="27" t="s">
         <v>51</v>
       </c>
       <c r="D1" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="27" t="s">
         <v>88</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="F1" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="G1" s="27" t="s">
-        <v>81</v>
-      </c>
-      <c r="H1" s="27" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="E2" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" s="12" t="s">
         <v>93</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -3699,7 +3748,7 @@
       <c r="F3" s="10"/>
       <c r="G3" s="10"/>
       <c r="H3" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -3711,33 +3760,33 @@
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
       <c r="H4" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="C5" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>553</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>554</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>126</v>
-      </c>
       <c r="F5" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
   </sheetData>
@@ -3767,65 +3816,65 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>43</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D1" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="F1" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="14" t="s">
         <v>140</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" t="s">
+        <v>561</v>
+      </c>
+      <c r="C2" t="s">
+        <v>561</v>
+      </c>
+      <c r="D2" t="s">
+        <v>564</v>
+      </c>
+      <c r="E2" t="s">
         <v>142</v>
-      </c>
-      <c r="B2" t="s">
-        <v>562</v>
-      </c>
-      <c r="C2" t="s">
-        <v>562</v>
-      </c>
-      <c r="D2" t="s">
-        <v>565</v>
-      </c>
-      <c r="E2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" t="s">
+        <v>563</v>
+      </c>
+      <c r="C3" t="s">
+        <v>562</v>
+      </c>
+      <c r="D3" t="s">
+        <v>564</v>
+      </c>
+      <c r="E3" t="s">
         <v>144</v>
       </c>
-      <c r="B3" t="s">
-        <v>564</v>
-      </c>
-      <c r="C3" t="s">
-        <v>563</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F3" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="G3" t="s">
         <v>565</v>
-      </c>
-      <c r="E3" t="s">
-        <v>145</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>146</v>
-      </c>
-      <c r="G3" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -3861,157 +3910,157 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>43</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>42</v>
       </c>
       <c r="E1" s="19" t="s">
+        <v>559</v>
+      </c>
+      <c r="F1" s="19" t="s">
         <v>560</v>
       </c>
-      <c r="F1" s="19" t="s">
-        <v>561</v>
-      </c>
       <c r="G1" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="H1" s="19" t="s">
         <v>148</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>155</v>
-      </c>
       <c r="F2" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>155</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>155</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>576</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>577</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="E5" s="3" t="s">
-        <v>155</v>
-      </c>
       <c r="F5" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>155</v>
-      </c>
       <c r="F6" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -4039,104 +4088,104 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D1" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="E1" s="19" t="s">
         <v>148</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>179</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>181</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -4149,8 +4198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F40359-1191-3843-B5C3-38D19A754655}">
   <dimension ref="A1:D139"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4163,28 +4212,28 @@
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C1" s="20" t="s">
+        <v>210</v>
+      </c>
+      <c r="D1" s="20" t="s">
         <v>211</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="9" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -4193,1209 +4242,1209 @@
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="113" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
+        <v>474</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>475</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="D11" s="9" t="s">
         <v>476</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B14" s="21"/>
       <c r="C14" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B15" s="21"/>
       <c r="C15" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B16" s="21"/>
       <c r="C16" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B17" s="21"/>
       <c r="C17" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B18" s="21"/>
       <c r="C18" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B19" s="21"/>
       <c r="C19" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B20" s="21"/>
       <c r="C20" s="9" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B21" s="21"/>
       <c r="C21" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="10" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B22" s="21"/>
       <c r="C22" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B23" s="21"/>
       <c r="C23" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="10" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B24" s="21"/>
       <c r="C24" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="10" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B25" s="21"/>
       <c r="C25" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="10" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B26" s="21"/>
       <c r="C26" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="10" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B27" s="21"/>
       <c r="C27" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="10" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B28" s="21"/>
       <c r="C28" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="10" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B29" s="21"/>
       <c r="C29" s="9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="10" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B30" s="21"/>
       <c r="C30" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="10" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B31" s="21"/>
       <c r="C31" s="9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="10" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B32" s="21"/>
       <c r="C32" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="10" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B33" s="21"/>
       <c r="C33" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="10" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B34" s="21"/>
       <c r="C34" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="10" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B35" s="21"/>
       <c r="C35" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B36" s="21"/>
       <c r="C36" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="10" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B37" s="21"/>
       <c r="C37" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B38" s="21"/>
       <c r="C38" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="10" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B39" s="21"/>
       <c r="C39" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B40" s="21"/>
       <c r="C40" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B41" s="21"/>
       <c r="C41" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B42" s="21"/>
       <c r="C42" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B43" s="21"/>
       <c r="C43" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B44" s="21"/>
       <c r="C44" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="10" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B45" s="21"/>
       <c r="C45" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B46" s="21"/>
       <c r="C46" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="10" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B47" s="21"/>
       <c r="C47" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="10" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B48" s="21"/>
       <c r="C48" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B49" s="21"/>
       <c r="C49" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="10" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B50" s="21"/>
       <c r="C50" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="10" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B51" s="21"/>
       <c r="C51" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="10" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B52" s="21"/>
       <c r="C52" s="9" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="10" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B53" s="21"/>
       <c r="C53" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A54" s="10" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B54" s="21"/>
       <c r="C54" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B55" s="21"/>
       <c r="C55" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B56" s="21"/>
       <c r="C56" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B57" s="21"/>
       <c r="C57" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B58" s="21"/>
       <c r="C58" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B59" s="21"/>
       <c r="C59" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="10" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B60" s="21"/>
       <c r="C60" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="61" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B61" s="21"/>
       <c r="C61" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="62" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="10" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B62" s="21"/>
       <c r="C62" s="9" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="10" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B63" s="21"/>
       <c r="C63" s="9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="10" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B64" s="21"/>
       <c r="C64" s="9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="10" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B65" s="21"/>
       <c r="C65" s="9" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="10" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B66" s="21"/>
       <c r="C66" s="9" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="10" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B67" s="21"/>
       <c r="C67" s="9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A68" s="10" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B68" s="21"/>
       <c r="C68" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="10" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B69" s="21"/>
       <c r="C69" s="9" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="10" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B70" s="21"/>
       <c r="C70" s="9" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A71" s="10" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B71" s="21"/>
       <c r="C71" s="9" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="72" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" s="10" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B72" s="21"/>
       <c r="C72" s="9" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" s="10" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B73" s="21"/>
       <c r="C73" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" s="10" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B74" s="21"/>
       <c r="C74" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B75" s="21"/>
       <c r="C75" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B76" s="21"/>
       <c r="C76" s="9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" s="10" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B77" s="21"/>
       <c r="C77" s="9" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" s="10" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B78" s="21"/>
       <c r="C78" s="9" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A79" s="10" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B79" s="21"/>
       <c r="C79" s="9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" s="10" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B80" s="21"/>
       <c r="C80" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" s="10" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B81" s="21"/>
       <c r="C81" s="9" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" s="10" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B82" s="21"/>
       <c r="C82" s="9" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="83" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A83" s="10" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B83" s="21"/>
       <c r="C83" s="9" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A84" s="10" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B84" s="21"/>
       <c r="C84" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="85" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="10" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B85" s="21"/>
       <c r="C85" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="86" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A86" s="10" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B86" s="21"/>
       <c r="C86" s="9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A87" s="10" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B87" s="21"/>
       <c r="C87" s="9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="88" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A88" s="10" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B88" s="21"/>
       <c r="C88" s="9" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A89" s="10" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B89" s="21"/>
       <c r="C89" s="9" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A90" s="10" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B90" s="21"/>
       <c r="C90" s="9" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A91" s="10" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B91" s="21"/>
       <c r="C91" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A92" s="10" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B92" s="21"/>
       <c r="C92" s="9" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="10" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B93" s="21"/>
       <c r="C93" s="9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="10" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B94" s="21"/>
       <c r="C94" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="10" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B95" s="21"/>
       <c r="C95" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="10" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B96" s="21"/>
       <c r="C96" s="9" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A97" s="10" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B97" s="21"/>
       <c r="C97" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A98" s="10" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B98" s="21"/>
       <c r="C98" s="9" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A99" s="10" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B99" s="21"/>
       <c r="C99" s="9" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A100" s="10" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B100" s="21"/>
       <c r="C100" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A101" s="10" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B101" s="21"/>
       <c r="C101" s="9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A102" s="10" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B102" s="21"/>
       <c r="C102" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A103" s="10" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B103" s="21"/>
       <c r="C103" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A104" s="10" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B104" s="21"/>
       <c r="C104" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A105" s="10" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B105" s="21"/>
       <c r="C105" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A106" s="10" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B106" s="21"/>
       <c r="C106" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A107" s="10" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B107" s="21"/>
       <c r="C107" s="9" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="108" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A108" s="10" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B108" s="21"/>
       <c r="C108" s="9" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="109" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A109" s="10" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B109" s="21"/>
       <c r="C109" s="9" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="110" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A110" s="10" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B110" s="21"/>
       <c r="C110" s="9" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A111" s="10" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B111" s="21"/>
       <c r="C111" s="9" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A112" s="10" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B112" s="21"/>
       <c r="C112" s="9" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="113" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A113" s="10" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B113" s="21"/>
       <c r="C113" s="9" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="114" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A114" s="10" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B114" s="21"/>
       <c r="C114" s="9" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="115" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A115" s="10" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B115" s="21"/>
       <c r="C115" s="9" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="10" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B116" s="21"/>
       <c r="C116" s="9" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="117" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A117" s="10" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B117" s="21"/>
       <c r="C117" s="9" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="118" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A118" s="10" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B118" s="21"/>
       <c r="C118" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="119" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A119" s="10" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B119" s="21"/>
       <c r="C119" s="9" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A120" s="10" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B120" s="21"/>
       <c r="C120" s="9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A121" s="10" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B121" s="21"/>
       <c r="C121" s="9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="122" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A122" s="10" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B122" s="21"/>
       <c r="C122" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="123" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A123" s="10" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B123" s="21"/>
       <c r="C123" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="124" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A124" s="10" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B124" s="21"/>
       <c r="C124" s="9" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="125" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A125" s="10" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B125" s="21"/>
       <c r="C125" s="9" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="126" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A126" s="10" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B126" s="21"/>
       <c r="C126" s="9" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="127" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A127" s="10" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B127" s="21"/>
       <c r="C127" s="9" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="128" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A128" s="10" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B128" s="21"/>
       <c r="C128" s="9" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="129" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A129" s="10" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B129" s="21"/>
       <c r="C129" s="9" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="130" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A130" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B130" s="21"/>
       <c r="C130" s="9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="131" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A131" s="10" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B131" s="21"/>
       <c r="C131" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="132" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A132" s="10" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B132" s="21"/>
       <c r="C132" s="9" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="133" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A133" s="10" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B133" s="21"/>
       <c r="C133" s="9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="10" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="10" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="10" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="10" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="10" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="10" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
   </sheetData>
@@ -5424,22 +5473,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
+        <v>492</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>493</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="C1" s="16" t="s">
         <v>494</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>495</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>496</v>
       </c>
-      <c r="E1" s="16" t="s">
-        <v>497</v>
-      </c>
       <c r="F1" s="26" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G1" s="10"/>
     </row>
@@ -5448,17 +5497,17 @@
         <v>4</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G2" s="10"/>
     </row>
@@ -5467,17 +5516,17 @@
         <v>3</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="10" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="G3" s="10"/>
     </row>
@@ -5486,19 +5535,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
+        <v>502</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>503</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="D4" s="10" t="s">
+      <c r="E4" s="10" t="s">
         <v>504</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>505</v>
-      </c>
       <c r="F4" s="10" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G4" s="10"/>
     </row>
@@ -5507,17 +5556,17 @@
         <v>1</v>
       </c>
       <c r="B5" s="10" t="s">
+        <v>506</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>499</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>507</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>500</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>508</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="10" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="G5" s="10"/>
     </row>
@@ -5541,18 +5590,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" t="s">
         <v>119</v>
-      </c>
-      <c r="B2" t="s">
-        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -5608,13 +5657,13 @@
         <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E2" t="s">
         <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -5628,13 +5677,13 @@
         <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E3" t="s">
         <v>37</v>
       </c>
       <c r="F3" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
   </sheetData>
@@ -5659,10 +5708,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B1" s="29" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C1" s="29"/>
       <c r="D1" s="29"/>
@@ -5670,10 +5719,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C2" s="29"/>
       <c r="D2" s="29"/>
@@ -5684,7 +5733,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C3" s="31"/>
       <c r="D3" s="31"/>
@@ -5695,7 +5744,7 @@
         <v>29</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C4" s="30"/>
       <c r="D4" s="30"/>
@@ -5706,7 +5755,7 @@
         <v>30</v>
       </c>
       <c r="B5" s="30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="30"/>
@@ -5717,7 +5766,7 @@
         <v>31</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C6" s="29"/>
       <c r="D6" s="29"/>
@@ -5728,7 +5777,7 @@
         <v>33</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="29"/>
@@ -5739,7 +5788,7 @@
         <v>32</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C8" s="29"/>
       <c r="D8" s="29"/>
@@ -5747,10 +5796,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C9" s="29"/>
       <c r="D9" s="29"/>
@@ -5758,7 +5807,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B10" s="29"/>
       <c r="C10" s="29"/>
@@ -5767,7 +5816,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>26</v>
@@ -5787,16 +5836,16 @@
         <v>24</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>171</v>
-      </c>
       <c r="D13" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -5804,16 +5853,16 @@
         <v>25</v>
       </c>
       <c r="B14" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>171</v>
-      </c>
       <c r="D14" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -5865,22 +5914,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>43</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>42</v>
       </c>
       <c r="E1" s="19" t="s">
+        <v>557</v>
+      </c>
+      <c r="F1" s="19" t="s">
         <v>558</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -5888,19 +5937,19 @@
         <v>24</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>203</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>205</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -5914,13 +5963,13 @@
         <v>25</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>205</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -5949,13 +5998,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>43</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>42</v>
@@ -5966,13 +6015,13 @@
         <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5980,13 +6029,13 @@
         <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -5994,13 +6043,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -6008,13 +6057,13 @@
         <v>27</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
@@ -6026,7 +6075,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED1B92D-F8EC-D24D-81E6-6B85449D22F0}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -6042,82 +6091,82 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>43</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>525</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>526</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" t="s">
         <v>527</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>528</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>529</v>
       </c>
-      <c r="F2" t="s">
-        <v>530</v>
-      </c>
       <c r="G2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="C3" t="s">
         <v>537</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>538</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>539</v>
       </c>
-      <c r="F3" t="s">
-        <v>540</v>
-      </c>
       <c r="G3" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>641</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>526</v>
+      </c>
+      <c r="C4" t="s">
         <v>642</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>527</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>643</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>644</v>
-      </c>
-      <c r="F4" t="s">
-        <v>645</v>
       </c>
     </row>
   </sheetData>
@@ -6127,9 +6176,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EB40753-8F7D-3941-9F21-F336F33F75CC}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -6142,45 +6193,45 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>43</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D1" s="19" t="s">
+        <v>515</v>
+      </c>
+      <c r="E1" s="19" t="s">
         <v>516</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="19" t="s">
         <v>517</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>518</v>
+      </c>
+      <c r="B2" t="s">
         <v>519</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>520</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>521</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>522</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>523</v>
-      </c>
-      <c r="F2" t="s">
-        <v>524</v>
       </c>
       <c r="G2" t="s">
         <v>53</v>
@@ -6188,16 +6239,39 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="E3" t="s">
+        <v>522</v>
+      </c>
+      <c r="F3" t="s">
         <v>523</v>
-      </c>
-      <c r="F3" t="s">
-        <v>524</v>
       </c>
       <c r="G3" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>647</v>
+      </c>
+      <c r="B4" t="s">
+        <v>648</v>
+      </c>
+      <c r="C4" t="s">
+        <v>649</v>
+      </c>
+      <c r="D4" t="s">
+        <v>521</v>
+      </c>
+      <c r="E4" t="s">
+        <v>522</v>
+      </c>
+      <c r="F4" t="s">
+        <v>523</v>
+      </c>
+      <c r="G4" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -6227,42 +6301,42 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>133</v>
-      </c>
       <c r="C1" s="13" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>569</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>571</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>572</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>573</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>613</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>134</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>135</v>
       </c>
       <c r="C2" s="13" t="s">
         <v>43</v>
@@ -6271,36 +6345,36 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>576</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>577</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="I2" s="28" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>137</v>
-      </c>
       <c r="C3" s="13" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>6</v>
@@ -6309,16 +6383,16 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -6327,65 +6401,65 @@
         <v>42</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>578</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>579</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>579</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>579</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>579</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>580</v>
-      </c>
       <c r="I4" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
       <c r="C5" s="13" t="s">
+        <v>580</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>581</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>570</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>571</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>572</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>573</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>613</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>574</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
       <c r="C6" s="13" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="28" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -6394,7 +6468,7 @@
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="13" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>0</v>
@@ -6419,26 +6493,26 @@
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="13" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>164</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -6449,7 +6523,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -6477,10 +6551,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>2</v>
@@ -6505,10 +6579,10 @@
         <v>8</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>2</v>
@@ -6523,10 +6597,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
+        <v>624</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>625</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>626</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Add on Objectives and Endpoints syntax template support
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/full_1.xlsx
+++ b/tests/integration_test_files/full_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDF2412-6191-1E44-9783-14C3003D13F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3CAB2C-23D1-0C4F-AD74-A6BB2F04CB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51660" yWindow="5560" windowWidth="46140" windowHeight="20040" firstSheet="7" activeTab="13" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="51660" yWindow="5560" windowWidth="46140" windowHeight="20040" firstSheet="7" activeTab="18" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -1485,18 +1485,6 @@
     <t>Primary Objectives</t>
   </si>
   <si>
-    <t>&lt;table&gt;
-  &lt;tr&gt;
-    &lt;th style="vertical-align: top"&gt;Primary Objective&lt;/th&gt;
-    &lt;th style="vertical-align: top"&gt;Primary Endpoint&lt;/th&gt;
-  &lt;/tr&gt;
-  &lt;tr&gt;
-    &lt;td style="vertical-align: top"&gt;&lt;usdm:ref klass="Objective" namexref="OBJ1" attribute="description"/&gt;&lt;/td&gt;
-    &lt;td style="vertical-align: top"&gt;&lt;usdm:ref klass="Endpoint" id="Endpoint_1" attribute="description"/&gt;&lt;/td&gt;
-  &lt;/tr&gt;
-&lt;/table&gt;</t>
-  </si>
-  <si>
     <t>category</t>
   </si>
   <si>
@@ -2017,6 +2005,9 @@
   </si>
   <si>
     <t>The secondary efficacy objective for this study is to evaluate the efficacy of TCZ compared with placebo in combination with SOC for the treatment of severe COVID-19 pneumonia over the age of [min_age]</t>
+  </si>
+  <si>
+    <t>&lt;usdm:section name="M11-objective-endpoints"&gt;</t>
   </si>
 </sst>
 </file>
@@ -2176,10 +2167,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2517,7 +2508,7 @@
         <v>406</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2626,7 +2617,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>406</v>
@@ -2635,85 +2626,85 @@
         <v>43</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E16" s="19" t="s">
         <v>42</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
+        <v>479</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>480</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="C17" t="s">
         <v>481</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>482</v>
       </c>
-      <c r="D17" t="s">
-        <v>483</v>
-      </c>
       <c r="E17" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F17" s="24">
         <v>44927</v>
       </c>
       <c r="G17" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
+        <v>484</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>480</v>
+      </c>
+      <c r="C18" t="s">
         <v>485</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>481</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>486</v>
       </c>
-      <c r="D18" t="s">
-        <v>487</v>
-      </c>
       <c r="E18" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F18" s="24">
         <v>44927</v>
       </c>
       <c r="G18" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="10" t="s">
+        <v>484</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>480</v>
+      </c>
+      <c r="C19" t="s">
         <v>485</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>481</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>486</v>
       </c>
-      <c r="D19" t="s">
-        <v>487</v>
-      </c>
       <c r="E19" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F19" s="24">
         <v>44958</v>
       </c>
       <c r="G19" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
   </sheetData>
@@ -2744,190 +2735,190 @@
         <v>43</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>42</v>
       </c>
       <c r="E1" s="19" t="s">
+        <v>584</v>
+      </c>
+      <c r="F1" s="19" t="s">
         <v>585</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="G1" s="19" t="s">
         <v>586</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="H1" s="19" t="s">
         <v>587</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="I1" s="19" t="s">
         <v>588</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>589</v>
+      </c>
+      <c r="B2" t="s">
         <v>590</v>
-      </c>
-      <c r="B2" t="s">
-        <v>591</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>591</v>
+      </c>
+      <c r="E2" t="s">
+        <v>567</v>
+      </c>
+      <c r="F2" t="s">
+        <v>568</v>
+      </c>
+      <c r="G2" t="s">
         <v>592</v>
       </c>
-      <c r="E2" t="s">
-        <v>568</v>
-      </c>
-      <c r="F2" t="s">
-        <v>569</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>593</v>
-      </c>
-      <c r="H2" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>594</v>
+      </c>
+      <c r="B3" t="s">
         <v>595</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>596</v>
       </c>
-      <c r="C3" t="s">
-        <v>597</v>
-      </c>
       <c r="D3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E3" t="s">
+        <v>568</v>
+      </c>
+      <c r="F3" t="s">
         <v>569</v>
-      </c>
-      <c r="F3" t="s">
-        <v>570</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
       </c>
       <c r="H3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>598</v>
+      </c>
+      <c r="B4" t="s">
         <v>599</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>574</v>
+      </c>
+      <c r="D4" t="s">
         <v>600</v>
       </c>
-      <c r="C4" t="s">
-        <v>575</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
+        <v>569</v>
+      </c>
+      <c r="F4" t="s">
+        <v>569</v>
+      </c>
+      <c r="G4" t="s">
         <v>601</v>
-      </c>
-      <c r="E4" t="s">
-        <v>570</v>
-      </c>
-      <c r="F4" t="s">
-        <v>570</v>
-      </c>
-      <c r="G4" t="s">
-        <v>602</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>602</v>
+      </c>
+      <c r="B5" t="s">
         <v>603</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>575</v>
+      </c>
+      <c r="D5" t="s">
         <v>604</v>
       </c>
-      <c r="C5" t="s">
-        <v>576</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>570</v>
+      </c>
+      <c r="F5" t="s">
+        <v>569</v>
+      </c>
+      <c r="G5" t="s">
         <v>605</v>
       </c>
-      <c r="E5" t="s">
-        <v>571</v>
-      </c>
-      <c r="F5" t="s">
-        <v>570</v>
-      </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
+        <v>593</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>606</v>
-      </c>
-      <c r="H5" t="s">
-        <v>594</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>607</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B6" t="s">
+        <v>617</v>
+      </c>
+      <c r="C6" t="s">
+        <v>610</v>
+      </c>
+      <c r="D6" t="s">
+        <v>604</v>
+      </c>
+      <c r="E6" t="s">
+        <v>611</v>
+      </c>
+      <c r="F6" t="s">
+        <v>569</v>
+      </c>
+      <c r="G6" t="s">
         <v>618</v>
       </c>
-      <c r="C6" t="s">
-        <v>611</v>
-      </c>
-      <c r="D6" t="s">
-        <v>605</v>
-      </c>
-      <c r="E6" t="s">
-        <v>612</v>
-      </c>
-      <c r="F6" t="s">
-        <v>570</v>
-      </c>
-      <c r="G6" t="s">
-        <v>619</v>
-      </c>
       <c r="H6" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>607</v>
+      </c>
+      <c r="B7" t="s">
         <v>608</v>
-      </c>
-      <c r="B7" t="s">
-        <v>609</v>
       </c>
       <c r="C7" t="s">
         <v>174</v>
       </c>
       <c r="D7" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="E7" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F7" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="G7" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="H7" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
   </sheetData>
@@ -2961,7 +2952,7 @@
         <v>43</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D1" s="25" t="s">
         <v>207</v>
@@ -2983,41 +2974,41 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="B3" t="s">
         <v>628</v>
       </c>
-      <c r="B3" t="s">
-        <v>629</v>
-      </c>
       <c r="C3" s="4" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B4" t="s">
+        <v>629</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>630</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>631</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>145</v>
       </c>
       <c r="E4" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B5" t="s">
+        <v>625</v>
+      </c>
+      <c r="C5" t="s">
         <v>626</v>
-      </c>
-      <c r="C5" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -3065,7 +3056,7 @@
         <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C2" t="s">
         <v>45</v>
@@ -3079,7 +3070,7 @@
         <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C3" t="s">
         <v>45</v>
@@ -3093,7 +3084,7 @@
         <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C4" t="s">
         <v>47</v>
@@ -3107,7 +3098,7 @@
         <v>79</v>
       </c>
       <c r="B5" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C5" t="s">
         <v>47</v>
@@ -3162,10 +3153,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B2" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -3182,10 +3173,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C3">
         <v>20</v>
@@ -3202,10 +3193,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="B4" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C4">
         <v>20</v>
@@ -3229,7 +3220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B908C5D6-C6A1-4043-A49A-69C599CFBAE9}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -3251,43 +3242,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>63</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>64</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H1" s="19" t="s">
         <v>65</v>
       </c>
       <c r="I1" s="19" t="s">
+        <v>541</v>
+      </c>
+      <c r="J1" s="19" t="s">
+        <v>544</v>
+      </c>
+      <c r="K1" s="19" t="s">
         <v>542</v>
-      </c>
-      <c r="J1" s="19" t="s">
-        <v>545</v>
-      </c>
-      <c r="K1" s="19" t="s">
-        <v>543</v>
       </c>
       <c r="L1" s="19" t="s">
         <v>66</v>
       </c>
       <c r="M1" s="19" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="68" x14ac:dyDescent="0.2">
@@ -3295,7 +3286,7 @@
         <v>81</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -3309,7 +3300,7 @@
         <v>83</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="I2" s="12"/>
       <c r="J2" s="12" t="s">
@@ -3325,23 +3316,23 @@
         <v>82</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>71</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>84</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="I3" s="12"/>
       <c r="J3" s="12" t="s">
@@ -3363,7 +3354,7 @@
         <v>85</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="I4" s="12"/>
       <c r="J4" s="12" t="s">
@@ -3774,7 +3765,7 @@
         <v>91</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>125</v>
@@ -3786,7 +3777,7 @@
         <v>84</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
   </sheetData>
@@ -3822,7 +3813,7 @@
         <v>43</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>137</v>
@@ -3842,13 +3833,13 @@
         <v>141</v>
       </c>
       <c r="B2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="C2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D2" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="E2" t="s">
         <v>142</v>
@@ -3859,13 +3850,13 @@
         <v>143</v>
       </c>
       <c r="B3" t="s">
+        <v>562</v>
+      </c>
+      <c r="C3" t="s">
+        <v>561</v>
+      </c>
+      <c r="D3" t="s">
         <v>563</v>
-      </c>
-      <c r="C3" t="s">
-        <v>562</v>
-      </c>
-      <c r="D3" t="s">
-        <v>564</v>
       </c>
       <c r="E3" t="s">
         <v>144</v>
@@ -3874,7 +3865,7 @@
         <v>145</v>
       </c>
       <c r="G3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -3916,16 +3907,16 @@
         <v>43</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>42</v>
       </c>
       <c r="E1" s="19" t="s">
+        <v>558</v>
+      </c>
+      <c r="F1" s="19" t="s">
         <v>559</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>560</v>
       </c>
       <c r="G1" s="19" t="s">
         <v>147</v>
@@ -4011,7 +4002,7 @@
         <v>152</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>153</v>
@@ -4028,10 +4019,10 @@
         <v>164</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>153</v>
@@ -4045,13 +4036,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>153</v>
@@ -4094,7 +4085,7 @@
         <v>168</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>147</v>
@@ -4198,8 +4189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F40359-1191-3843-B5C3-38D19A754655}">
   <dimension ref="A1:D139"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24:D25"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4226,14 +4217,14 @@
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="9" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -4301,7 +4292,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="113" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>474</v>
       </c>
@@ -4309,7 +4300,7 @@
         <v>475</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>476</v>
+        <v>650</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -4427,7 +4418,7 @@
         <v>232</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -4439,7 +4430,7 @@
         <v>233</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5473,22 +5464,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
+        <v>491</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>492</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="C1" s="16" t="s">
         <v>493</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>494</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>495</v>
       </c>
-      <c r="E1" s="16" t="s">
-        <v>496</v>
-      </c>
       <c r="F1" s="26" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G1" s="10"/>
     </row>
@@ -5497,17 +5488,17 @@
         <v>4</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>145</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G2" s="10"/>
     </row>
@@ -5516,17 +5507,17 @@
         <v>3</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>145</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="10" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G3" s="10"/>
     </row>
@@ -5535,19 +5526,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>145</v>
       </c>
       <c r="D4" s="10" t="s">
+        <v>502</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>503</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>504</v>
-      </c>
       <c r="F4" s="10" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="G4" s="10"/>
     </row>
@@ -5556,17 +5547,17 @@
         <v>1</v>
       </c>
       <c r="B5" s="10" t="s">
+        <v>505</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>506</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>499</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>507</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="10" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G5" s="10"/>
     </row>
@@ -5663,7 +5654,7 @@
         <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -5683,7 +5674,7 @@
         <v>37</v>
       </c>
       <c r="F3" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
   </sheetData>
@@ -5732,34 +5723,34 @@
       <c r="A3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="31" t="s">
         <v>114</v>
       </c>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
@@ -5879,16 +5870,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5920,16 +5911,16 @@
         <v>43</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>42</v>
       </c>
       <c r="E1" s="19" t="s">
+        <v>556</v>
+      </c>
+      <c r="F1" s="19" t="s">
         <v>557</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -6004,7 +5995,7 @@
         <v>43</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>42</v>
@@ -6091,10 +6082,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>406</v>
@@ -6103,70 +6094,70 @@
         <v>43</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="F1" s="19" t="s">
         <v>211</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>524</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>525</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" t="s">
         <v>526</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>527</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>528</v>
       </c>
-      <c r="F2" t="s">
-        <v>529</v>
-      </c>
       <c r="G2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="C3" t="s">
         <v>536</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>537</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>538</v>
       </c>
-      <c r="F3" t="s">
-        <v>539</v>
-      </c>
       <c r="G3" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>640</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>525</v>
+      </c>
+      <c r="C4" t="s">
         <v>641</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>526</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>642</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" t="s">
         <v>643</v>
-      </c>
-      <c r="F4" t="s">
-        <v>644</v>
       </c>
     </row>
   </sheetData>
@@ -6199,39 +6190,39 @@
         <v>43</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D1" s="19" t="s">
+        <v>514</v>
+      </c>
+      <c r="E1" s="19" t="s">
         <v>515</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>516</v>
       </c>
       <c r="F1" s="19" t="s">
         <v>75</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>517</v>
+      </c>
+      <c r="B2" t="s">
         <v>518</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>519</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>520</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>521</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>522</v>
-      </c>
-      <c r="F2" t="s">
-        <v>523</v>
       </c>
       <c r="G2" t="s">
         <v>53</v>
@@ -6239,13 +6230,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="E3" t="s">
+        <v>521</v>
+      </c>
+      <c r="F3" t="s">
         <v>522</v>
-      </c>
-      <c r="F3" t="s">
-        <v>523</v>
       </c>
       <c r="G3" t="s">
         <v>62</v>
@@ -6253,22 +6244,22 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>646</v>
+      </c>
+      <c r="B4" t="s">
         <v>647</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>648</v>
       </c>
-      <c r="C4" t="s">
-        <v>649</v>
-      </c>
       <c r="D4" t="s">
+        <v>520</v>
+      </c>
+      <c r="E4" t="s">
         <v>521</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>522</v>
-      </c>
-      <c r="F4" t="s">
-        <v>523</v>
       </c>
       <c r="G4" t="s">
         <v>53</v>
@@ -6310,25 +6301,25 @@
         <v>406</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>568</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>569</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>571</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>572</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>612</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -6345,19 +6336,19 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>574</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>575</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>576</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="I2" s="28" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>174</v>
@@ -6371,10 +6362,10 @@
         <v>136</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>6</v>
@@ -6383,13 +6374,13 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>174</v>
@@ -6401,65 +6392,65 @@
         <v>42</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>577</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>578</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>578</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>578</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>578</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>579</v>
-      </c>
       <c r="I4" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
       <c r="C5" s="13" t="s">
+        <v>579</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>568</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>569</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>570</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>611</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="J5" s="2" t="s">
         <v>580</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>569</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>570</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>571</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>572</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>612</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>573</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
       <c r="C6" s="13" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="28" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -6468,7 +6459,7 @@
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="13" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>0</v>
@@ -6493,7 +6484,7 @@
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="13" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>160</v>
@@ -6512,7 +6503,7 @@
         <v>164</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -6551,10 +6542,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>2</v>
@@ -6579,10 +6570,10 @@
         <v>8</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>2</v>
@@ -6597,10 +6588,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
+        <v>623</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>624</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>625</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Update test fro new scenario
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/full_1.xlsx
+++ b/tests/integration_test_files/full_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3CAB2C-23D1-0C4F-AD74-A6BB2F04CB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D7F3DF-CA01-5F4A-B7C8-102D0FC5A05B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51660" yWindow="5560" windowWidth="46140" windowHeight="20040" firstSheet="7" activeTab="18" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="41060" yWindow="5560" windowWidth="56740" windowHeight="20040" activeTab="6" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="658">
   <si>
     <t>Screening</t>
   </si>
@@ -2008,6 +2008,27 @@
   </si>
   <si>
     <t>&lt;usdm:section name="M11-objective-endpoints"&gt;</t>
+  </si>
+  <si>
+    <t>Berber_Dict</t>
+  </si>
+  <si>
+    <t>Dictionary for Berber Example</t>
+  </si>
+  <si>
+    <t>Berber Dictionary</t>
+  </si>
+  <si>
+    <t>xxxx</t>
+  </si>
+  <si>
+    <t>Berber</t>
+  </si>
+  <si>
+    <t>Test for Berber</t>
+  </si>
+  <si>
+    <t>Pick up activity [xxxx]</t>
   </si>
 </sst>
 </file>
@@ -2931,7 +2952,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4189,7 +4210,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F40359-1191-3843-B5C3-38D19A754655}">
   <dimension ref="A1:D139"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -6064,10 +6085,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED1B92D-F8EC-D24D-81E6-6B85449D22F0}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6160,6 +6181,26 @@
         <v>643</v>
       </c>
     </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>640</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="C5" t="s">
+        <v>655</v>
+      </c>
+      <c r="D5" t="s">
+        <v>656</v>
+      </c>
+      <c r="F5" t="s">
+        <v>657</v>
+      </c>
+      <c r="G5" t="s">
+        <v>651</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6167,16 +6208,17 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EB40753-8F7D-3941-9F21-F336F33F75CC}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.33203125" customWidth="1"/>
-    <col min="2" max="4" width="18.83203125" customWidth="1"/>
+    <col min="2" max="2" width="28.6640625" customWidth="1"/>
+    <col min="3" max="4" width="18.83203125" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="31.83203125" customWidth="1"/>
@@ -6263,6 +6305,29 @@
       </c>
       <c r="G4" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>651</v>
+      </c>
+      <c r="B5" t="s">
+        <v>652</v>
+      </c>
+      <c r="C5" t="s">
+        <v>653</v>
+      </c>
+      <c r="D5" t="s">
+        <v>654</v>
+      </c>
+      <c r="E5" t="s">
+        <v>577</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" t="s">
+        <v>477</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Further updates to readme and infographic
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/full_1.xlsx
+++ b/tests/integration_test_files/full_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D7F3DF-CA01-5F4A-B7C8-102D0FC5A05B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724EB825-CF10-464D-87F1-EF934203CC59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41060" yWindow="5560" windowWidth="56740" windowHeight="20040" activeTab="6" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="68220" yWindow="4440" windowWidth="34080" windowHeight="20040" firstSheet="10" activeTab="15" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -2188,10 +2188,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3046,7 +3046,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E548DFC1-EB0E-374B-95D2-A04104B745FB}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -3241,8 +3241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B908C5D6-C6A1-4043-A49A-69C599CFBAE9}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="E1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3683,7 +3683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBFC82B4-C495-A142-993D-B6A47D77A4C3}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -3810,7 +3810,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D608A778-255D-4443-A7EA-03049F1FC98F}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -5470,7 +5470,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5744,34 +5744,34 @@
       <c r="A3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
@@ -5891,16 +5891,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6087,8 +6087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED1B92D-F8EC-D24D-81E6-6B85449D22F0}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add encounter window feature
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/full_1.xlsx
+++ b/tests/integration_test_files/full_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA018A78-26B4-8B4A-91D2-F06ECFC956F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE8645E-DAE1-4242-885E-5C00505EE4B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24560" yWindow="500" windowWidth="33820" windowHeight="26040" firstSheet="11" activeTab="20" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="24560" yWindow="500" windowWidth="44940" windowHeight="26040" firstSheet="3" activeTab="16" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="678">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="678">
   <si>
     <t>Screening</t>
   </si>
@@ -2297,25 +2297,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4026,10 +4026,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3500D92E-6FB0-8D4D-97D2-7C2457E4D88B}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4044,7 +4044,7 @@
     <col min="9" max="9" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
         <v>406</v>
       </c>
@@ -4069,8 +4069,11 @@
       <c r="H1" s="19" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I1" s="19" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>160</v>
       </c>
@@ -4095,8 +4098,11 @@
       <c r="H2" s="3" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I2" s="7" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>161</v>
       </c>
@@ -4115,8 +4121,11 @@
       <c r="F3" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I3" s="7" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>162</v>
       </c>
@@ -4138,8 +4147,9 @@
       <c r="G4" s="3" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>163</v>
       </c>
@@ -4158,8 +4168,11 @@
       <c r="F5" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I5" s="7" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>164</v>
       </c>
@@ -4178,8 +4191,11 @@
       <c r="F6" s="3" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I6" s="7" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>616</v>
       </c>
@@ -4197,6 +4213,9 @@
       </c>
       <c r="F7" s="3" t="s">
         <v>157</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>607</v>
       </c>
     </row>
   </sheetData>
@@ -5749,7 +5768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6CCACBD-9050-2546-A791-CCDEA21B15F7}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -5760,94 +5779,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="36" t="s">
         <v>670</v>
       </c>
-      <c r="B1" s="33"/>
+      <c r="B1" s="36"/>
     </row>
     <row r="2" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="31" t="s">
         <v>675</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="30" t="s">
         <v>676</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="32" t="s">
         <v>658</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="29" t="s">
         <v>663</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="32" t="s">
         <v>659</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="29" t="s">
         <v>664</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="32" t="s">
         <v>660</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="29" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="32" t="s">
         <v>662</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="29" t="s">
         <v>666</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="32" t="s">
         <v>661</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="29" t="s">
         <v>667</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="37" t="s">
         <v>671</v>
       </c>
-      <c r="B10" s="34"/>
+      <c r="B10" s="37"/>
     </row>
     <row r="11" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="36" t="s">
+      <c r="A11" s="31" t="s">
         <v>675</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="30" t="s">
         <v>676</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="37" t="s">
+      <c r="A12" s="32" t="s">
         <v>677</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="29" t="s">
         <v>672</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="32" t="s">
         <v>668</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="29" t="s">
         <v>673</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="32" t="s">
         <v>669</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="29" t="s">
         <v>674</v>
       </c>
     </row>
@@ -5971,109 +5990,109 @@
       <c r="A1" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="33" t="s">
         <v>191</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="33" t="s">
         <v>190</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
     </row>
     <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="33" t="s">
         <v>129</v>
       </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
@@ -6140,16 +6159,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6589,7 +6608,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
       <selection pane="bottomRight" activeCell="F5" sqref="F5"/>

</xml_diff>

<commit_message>
Title sheet updates and trace
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/full_1.xlsx
+++ b/tests/integration_test_files/full_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE8645E-DAE1-4242-885E-5C00505EE4B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD1B003-2F51-944A-85CE-A1B175F8B8E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24560" yWindow="500" windowWidth="44940" windowHeight="26040" firstSheet="3" activeTab="16" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="24560" yWindow="500" windowWidth="44940" windowHeight="26040" activeTab="2" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="678">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="691">
   <si>
     <t>Screening</t>
   </si>
@@ -2090,6 +2090,45 @@
   </si>
   <si>
     <t>On line tool (requires username and password)</t>
+  </si>
+  <si>
+    <t>EU</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>WHO</t>
+  </si>
+  <si>
+    <t>EU CT</t>
+  </si>
+  <si>
+    <t>FDA</t>
+  </si>
+  <si>
+    <t>Regulatory Agency</t>
+  </si>
+  <si>
+    <t>European Union</t>
+  </si>
+  <si>
+    <t>Food &amp; Drug Administration</t>
+  </si>
+  <si>
+    <t>World Health Organisation</t>
+  </si>
+  <si>
+    <t>UN</t>
+  </si>
+  <si>
+    <t>EU12345</t>
+  </si>
+  <si>
+    <t>IND12345</t>
+  </si>
+  <si>
+    <t>WHO12345</t>
   </si>
 </sst>
 </file>
@@ -4028,8 +4067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3500D92E-6FB0-8D4D-97D2-7C2457E4D88B}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4041,7 +4080,7 @@
     <col min="5" max="5" width="21.6640625" style="3" customWidth="1"/>
     <col min="6" max="6" width="20.83203125" style="3" customWidth="1"/>
     <col min="7" max="8" width="22" style="3" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -4069,7 +4108,7 @@
       <c r="H1" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="25" t="s">
         <v>588</v>
       </c>
     </row>
@@ -4147,7 +4186,6 @@
       <c r="G4" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="I4" s="7"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -5891,16 +5929,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9227F54-17C1-E44A-AD70-49AE8CBF35F9}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F3"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.33203125" customWidth="1"/>
-    <col min="2" max="3" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" customWidth="1"/>
     <col min="4" max="4" width="23.33203125" customWidth="1"/>
     <col min="5" max="5" width="22.33203125" customWidth="1"/>
     <col min="6" max="6" width="52.5" customWidth="1"/>
@@ -5964,6 +6003,57 @@
       </c>
       <c r="F3" t="s">
         <v>634</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>678</v>
+      </c>
+      <c r="B4" t="s">
+        <v>681</v>
+      </c>
+      <c r="C4" t="s">
+        <v>684</v>
+      </c>
+      <c r="D4" t="s">
+        <v>683</v>
+      </c>
+      <c r="E4" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>679</v>
+      </c>
+      <c r="B5" t="s">
+        <v>682</v>
+      </c>
+      <c r="C5" t="s">
+        <v>685</v>
+      </c>
+      <c r="D5" t="s">
+        <v>683</v>
+      </c>
+      <c r="E5" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>687</v>
+      </c>
+      <c r="B6" t="s">
+        <v>680</v>
+      </c>
+      <c r="C6" t="s">
+        <v>686</v>
+      </c>
+      <c r="D6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E6" t="s">
+        <v>690</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix approval date issue
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/full_1.xlsx
+++ b/tests/integration_test_files/full_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD1B003-2F51-944A-85CE-A1B175F8B8E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1B345A-03AA-354A-9537-D51D39B1BE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24560" yWindow="500" windowWidth="44940" windowHeight="26040" activeTab="2" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="24560" yWindow="500" windowWidth="44940" windowHeight="26040" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="689">
   <si>
     <t>Screening</t>
   </si>
@@ -1498,9 +1498,6 @@
     <t>study_version</t>
   </si>
   <si>
-    <t>Approval</t>
-  </si>
-  <si>
     <t>Design approval date</t>
   </si>
   <si>
@@ -1658,9 +1655,6 @@
   </si>
   <si>
     <t>Population three, old age group</t>
-  </si>
-  <si>
-    <t>region:asia</t>
   </si>
   <si>
     <t>02</t>
@@ -2344,10 +2338,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2670,10 +2664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53AA772F-4124-4842-BA10-D27E5C5CE960}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2692,7 +2686,7 @@
         <v>406</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -2819,7 +2813,7 @@
         <v>478</v>
       </c>
       <c r="G16" s="16" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -2827,68 +2821,45 @@
         <v>479</v>
       </c>
       <c r="B17" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="C17" t="s">
         <v>480</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>481</v>
       </c>
-      <c r="D17" t="s">
-        <v>482</v>
-      </c>
       <c r="E17" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="F17" s="24">
-        <v>44927</v>
+        <v>44911</v>
       </c>
       <c r="G17" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
+        <v>483</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>485</v>
+      </c>
+      <c r="C18" t="s">
         <v>484</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>480</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>485</v>
       </c>
-      <c r="D18" t="s">
-        <v>486</v>
-      </c>
       <c r="E18" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F18" s="24">
         <v>44927</v>
       </c>
       <c r="G18" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
-        <v>484</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>480</v>
-      </c>
-      <c r="C19" t="s">
-        <v>485</v>
-      </c>
-      <c r="D19" t="s">
-        <v>486</v>
-      </c>
-      <c r="E19" t="s">
-        <v>488</v>
-      </c>
-      <c r="F19" s="24">
-        <v>44958</v>
-      </c>
-      <c r="G19" t="s">
-        <v>534</v>
+        <v>482</v>
       </c>
     </row>
   </sheetData>
@@ -2925,184 +2896,184 @@
         <v>42</v>
       </c>
       <c r="E1" s="19" t="s">
+        <v>582</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>583</v>
+      </c>
+      <c r="G1" s="19" t="s">
         <v>584</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="H1" s="19" t="s">
         <v>585</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="I1" s="19" t="s">
         <v>586</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>587</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B2" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>589</v>
+      </c>
+      <c r="E2" t="s">
+        <v>565</v>
+      </c>
+      <c r="F2" t="s">
+        <v>566</v>
+      </c>
+      <c r="G2" t="s">
+        <v>590</v>
+      </c>
+      <c r="H2" t="s">
         <v>591</v>
-      </c>
-      <c r="E2" t="s">
-        <v>567</v>
-      </c>
-      <c r="F2" t="s">
-        <v>568</v>
-      </c>
-      <c r="G2" t="s">
-        <v>592</v>
-      </c>
-      <c r="H2" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>592</v>
+      </c>
+      <c r="B3" t="s">
+        <v>593</v>
+      </c>
+      <c r="C3" t="s">
         <v>594</v>
       </c>
-      <c r="B3" t="s">
-        <v>595</v>
-      </c>
-      <c r="C3" t="s">
-        <v>596</v>
-      </c>
       <c r="D3" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="E3" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="F3" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="G3" t="s">
         <v>7</v>
       </c>
       <c r="H3" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>596</v>
+      </c>
+      <c r="B4" t="s">
+        <v>597</v>
+      </c>
+      <c r="C4" t="s">
+        <v>572</v>
+      </c>
+      <c r="D4" t="s">
         <v>598</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
+        <v>567</v>
+      </c>
+      <c r="F4" t="s">
+        <v>567</v>
+      </c>
+      <c r="G4" t="s">
         <v>599</v>
-      </c>
-      <c r="C4" t="s">
-        <v>574</v>
-      </c>
-      <c r="D4" t="s">
-        <v>600</v>
-      </c>
-      <c r="E4" t="s">
-        <v>569</v>
-      </c>
-      <c r="F4" t="s">
-        <v>569</v>
-      </c>
-      <c r="G4" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>600</v>
+      </c>
+      <c r="B5" t="s">
+        <v>601</v>
+      </c>
+      <c r="C5" t="s">
+        <v>573</v>
+      </c>
+      <c r="D5" t="s">
         <v>602</v>
       </c>
-      <c r="B5" t="s">
+      <c r="E5" t="s">
+        <v>568</v>
+      </c>
+      <c r="F5" t="s">
+        <v>567</v>
+      </c>
+      <c r="G5" t="s">
         <v>603</v>
       </c>
-      <c r="C5" t="s">
-        <v>575</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="H5" t="s">
+        <v>591</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>604</v>
-      </c>
-      <c r="E5" t="s">
-        <v>570</v>
-      </c>
-      <c r="F5" t="s">
-        <v>569</v>
-      </c>
-      <c r="G5" t="s">
-        <v>605</v>
-      </c>
-      <c r="H5" t="s">
-        <v>593</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>600</v>
+      </c>
+      <c r="B6" t="s">
+        <v>615</v>
+      </c>
+      <c r="C6" t="s">
+        <v>608</v>
+      </c>
+      <c r="D6" t="s">
         <v>602</v>
       </c>
-      <c r="B6" t="s">
-        <v>617</v>
-      </c>
-      <c r="C6" t="s">
-        <v>610</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
+        <v>609</v>
+      </c>
+      <c r="F6" t="s">
+        <v>567</v>
+      </c>
+      <c r="G6" t="s">
+        <v>616</v>
+      </c>
+      <c r="H6" t="s">
+        <v>591</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>604</v>
-      </c>
-      <c r="E6" t="s">
-        <v>611</v>
-      </c>
-      <c r="F6" t="s">
-        <v>569</v>
-      </c>
-      <c r="G6" t="s">
-        <v>618</v>
-      </c>
-      <c r="H6" t="s">
-        <v>593</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="B7" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C7" t="s">
         <v>174</v>
       </c>
       <c r="D7" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="E7" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="F7" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="G7" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="H7" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
   </sheetData>
@@ -3158,41 +3129,41 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B3" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B4" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>145</v>
       </c>
       <c r="E4" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>621</v>
+      </c>
+      <c r="B5" t="s">
         <v>623</v>
       </c>
-      <c r="B5" t="s">
-        <v>625</v>
-      </c>
       <c r="C5" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -3240,7 +3211,7 @@
         <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C2" t="s">
         <v>45</v>
@@ -3254,7 +3225,7 @@
         <v>78</v>
       </c>
       <c r="B3" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C3" t="s">
         <v>45</v>
@@ -3268,7 +3239,7 @@
         <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C4" t="s">
         <v>47</v>
@@ -3282,7 +3253,7 @@
         <v>79</v>
       </c>
       <c r="B5" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C5" t="s">
         <v>47</v>
@@ -3337,10 +3308,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -3357,10 +3328,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C3">
         <v>20</v>
@@ -3377,10 +3348,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B4" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C4">
         <v>20</v>
@@ -3426,43 +3397,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="B1" s="19" t="s">
         <v>63</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="D1" s="19" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="E1" s="19" t="s">
         <v>64</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="H1" s="19" t="s">
         <v>65</v>
       </c>
       <c r="I1" s="19" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="J1" s="19" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="K1" s="19" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="L1" s="19" t="s">
         <v>66</v>
       </c>
       <c r="M1" s="19" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="68" x14ac:dyDescent="0.2">
@@ -3470,7 +3441,7 @@
         <v>81</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="12" t="s">
@@ -3484,7 +3455,7 @@
         <v>83</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="I2" s="12"/>
       <c r="J2" s="12" t="s">
@@ -3500,23 +3471,23 @@
         <v>82</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>71</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>84</v>
       </c>
       <c r="H3" s="12" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="I3" s="12"/>
       <c r="J3" s="12" t="s">
@@ -3538,7 +3509,7 @@
         <v>85</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="I4" s="12"/>
       <c r="J4" s="12" t="s">
@@ -3949,7 +3920,7 @@
         <v>91</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>125</v>
@@ -3961,7 +3932,7 @@
         <v>84</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
   </sheetData>
@@ -4017,13 +3988,13 @@
         <v>141</v>
       </c>
       <c r="B2" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C2" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="D2" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="E2" t="s">
         <v>142</v>
@@ -4034,13 +4005,13 @@
         <v>143</v>
       </c>
       <c r="B3" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C3" t="s">
+        <v>559</v>
+      </c>
+      <c r="D3" t="s">
         <v>561</v>
-      </c>
-      <c r="D3" t="s">
-        <v>563</v>
       </c>
       <c r="E3" t="s">
         <v>144</v>
@@ -4049,7 +4020,7 @@
         <v>145</v>
       </c>
       <c r="G3" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -4097,10 +4068,10 @@
         <v>42</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="G1" s="19" t="s">
         <v>147</v>
@@ -4109,7 +4080,7 @@
         <v>148</v>
       </c>
       <c r="I1" s="25" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -4138,7 +4109,7 @@
         <v>158</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -4161,7 +4132,7 @@
         <v>156</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -4195,7 +4166,7 @@
         <v>152</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>153</v>
@@ -4207,7 +4178,7 @@
         <v>156</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -4215,10 +4186,10 @@
         <v>164</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>153</v>
@@ -4230,18 +4201,18 @@
         <v>156</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>153</v>
@@ -4253,7 +4224,7 @@
         <v>157</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
   </sheetData>
@@ -4287,7 +4258,7 @@
         <v>168</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>147</v>
@@ -4419,14 +4390,14 @@
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B2" s="21"/>
       <c r="C2" s="9" t="s">
+        <v>633</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>635</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -4502,7 +4473,7 @@
         <v>475</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -4620,7 +4591,7 @@
         <v>232</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -4632,7 +4603,7 @@
         <v>233</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5666,22 +5637,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
+        <v>490</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>491</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="C1" s="16" t="s">
         <v>492</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>493</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>494</v>
       </c>
-      <c r="E1" s="16" t="s">
-        <v>495</v>
-      </c>
       <c r="F1" s="26" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G1" s="10"/>
     </row>
@@ -5690,17 +5661,17 @@
         <v>4</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>145</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G2" s="10"/>
     </row>
@@ -5709,17 +5680,17 @@
         <v>3</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>145</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="10" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G3" s="10"/>
     </row>
@@ -5728,19 +5699,19 @@
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>145</v>
       </c>
       <c r="D4" s="10" t="s">
+        <v>501</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>502</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>503</v>
-      </c>
       <c r="F4" s="10" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G4" s="10"/>
     </row>
@@ -5749,17 +5720,17 @@
         <v>1</v>
       </c>
       <c r="B5" s="10" t="s">
+        <v>504</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>497</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>505</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>498</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>506</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="10" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="G5" s="10"/>
     </row>
@@ -5818,94 +5789,94 @@
   <sheetData>
     <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B1" s="36"/>
     </row>
     <row r="2" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="37" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="B10" s="37"/>
     </row>
     <row r="11" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="32" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="32" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
   </sheetData>
@@ -5931,7 +5902,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9227F54-17C1-E44A-AD70-49AE8CBF35F9}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -5982,7 +5953,7 @@
         <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -6002,58 +5973,58 @@
         <v>37</v>
       </c>
       <c r="F3" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="B4" t="s">
+        <v>679</v>
+      </c>
+      <c r="C4" t="s">
+        <v>682</v>
+      </c>
+      <c r="D4" t="s">
         <v>681</v>
       </c>
-      <c r="C4" t="s">
-        <v>684</v>
-      </c>
-      <c r="D4" t="s">
-        <v>683</v>
-      </c>
       <c r="E4" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="B5" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="C5" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="D5" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="E5" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="B6" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="C6" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="D6" t="s">
         <v>127</v>
       </c>
       <c r="E6" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
     </row>
   </sheetData>
@@ -6102,34 +6073,34 @@
       <c r="A3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="34" t="s">
+      <c r="B5" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
@@ -6249,16 +6220,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B5:E5"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B8:E8"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B5:E5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6296,10 +6267,10 @@
         <v>42</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -6464,7 +6435,7 @@
         <v>476</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>406</v>
@@ -6479,84 +6450,84 @@
         <v>211</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>523</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>524</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" t="s">
         <v>525</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>526</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>527</v>
       </c>
-      <c r="F2" t="s">
-        <v>528</v>
-      </c>
       <c r="G2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>533</v>
+      </c>
+      <c r="C3" t="s">
+        <v>534</v>
+      </c>
+      <c r="D3" t="s">
         <v>535</v>
       </c>
-      <c r="C3" t="s">
+      <c r="F3" t="s">
         <v>536</v>
       </c>
-      <c r="D3" t="s">
-        <v>537</v>
-      </c>
-      <c r="F3" t="s">
-        <v>538</v>
-      </c>
       <c r="G3" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>638</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>524</v>
+      </c>
+      <c r="C4" t="s">
+        <v>639</v>
+      </c>
+      <c r="D4" t="s">
         <v>640</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>525</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="F4" t="s">
         <v>641</v>
-      </c>
-      <c r="D4" t="s">
-        <v>642</v>
-      </c>
-      <c r="F4" t="s">
-        <v>643</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C5" t="s">
+        <v>653</v>
+      </c>
+      <c r="D5" t="s">
+        <v>654</v>
+      </c>
+      <c r="F5" t="s">
         <v>655</v>
       </c>
-      <c r="D5" t="s">
-        <v>656</v>
-      </c>
-      <c r="F5" t="s">
-        <v>657</v>
-      </c>
       <c r="G5" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
     </row>
   </sheetData>
@@ -6593,36 +6564,36 @@
         <v>477</v>
       </c>
       <c r="D1" s="19" t="s">
+        <v>513</v>
+      </c>
+      <c r="E1" s="19" t="s">
         <v>514</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>515</v>
       </c>
       <c r="F1" s="19" t="s">
         <v>75</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>516</v>
+      </c>
+      <c r="B2" t="s">
         <v>517</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>518</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>519</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>520</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>521</v>
-      </c>
-      <c r="F2" t="s">
-        <v>522</v>
       </c>
       <c r="G2" t="s">
         <v>53</v>
@@ -6630,13 +6601,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="E3" t="s">
+        <v>520</v>
+      </c>
+      <c r="F3" t="s">
         <v>521</v>
-      </c>
-      <c r="F3" t="s">
-        <v>522</v>
       </c>
       <c r="G3" t="s">
         <v>62</v>
@@ -6644,22 +6615,22 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>644</v>
+      </c>
+      <c r="B4" t="s">
+        <v>645</v>
+      </c>
+      <c r="C4" t="s">
         <v>646</v>
       </c>
-      <c r="B4" t="s">
-        <v>647</v>
-      </c>
-      <c r="C4" t="s">
-        <v>648</v>
-      </c>
       <c r="D4" t="s">
+        <v>519</v>
+      </c>
+      <c r="E4" t="s">
         <v>520</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>521</v>
-      </c>
-      <c r="F4" t="s">
-        <v>522</v>
       </c>
       <c r="G4" t="s">
         <v>53</v>
@@ -6667,19 +6638,19 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>649</v>
+      </c>
+      <c r="B5" t="s">
+        <v>650</v>
+      </c>
+      <c r="C5" t="s">
         <v>651</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>652</v>
       </c>
-      <c r="C5" t="s">
-        <v>653</v>
-      </c>
-      <c r="D5" t="s">
-        <v>654</v>
-      </c>
       <c r="E5" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>5</v>
@@ -6724,25 +6695,25 @@
         <v>406</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>565</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>567</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>568</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>569</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>570</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>571</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>611</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="34" x14ac:dyDescent="0.2">
@@ -6759,19 +6730,19 @@
         <v>0</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>571</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>573</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>574</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>575</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="I2" s="28" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>174</v>
@@ -6788,7 +6759,7 @@
         <v>477</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>6</v>
@@ -6797,13 +6768,13 @@
         <v>1</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="H3" s="28" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>174</v>
@@ -6815,65 +6786,65 @@
         <v>42</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="13"/>
       <c r="C5" s="13" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>566</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>567</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>568</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>569</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="H5" s="2" t="s">
+        <v>609</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>570</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>571</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>611</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>572</v>
-      </c>
       <c r="J5" s="2" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="13"/>
       <c r="C6" s="13" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="28" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -6882,7 +6853,7 @@
       <c r="A7" s="10"/>
       <c r="B7" s="10"/>
       <c r="C7" s="13" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>0</v>
@@ -6907,7 +6878,7 @@
       <c r="A8" s="10"/>
       <c r="B8" s="10"/>
       <c r="C8" s="13" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>160</v>
@@ -6926,7 +6897,7 @@
         <v>164</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -6965,10 +6936,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>2</v>
@@ -6993,10 +6964,10 @@
         <v>8</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>2</v>
@@ -7011,10 +6982,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Add PDF key and improve error messages
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/full_1.xlsx
+++ b/tests/integration_test_files/full_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1B345A-03AA-354A-9537-D51D39B1BE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6999D15-763A-2047-98C9-03DE24B5C6A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24560" yWindow="500" windowWidth="44940" windowHeight="26040" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="38940" yWindow="500" windowWidth="44940" windowHeight="26040" firstSheet="6" activeTab="16" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="689">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="690">
   <si>
     <t>Screening</t>
   </si>
@@ -2123,6 +2123,9 @@
   </si>
   <si>
     <t>WHO12345</t>
+  </si>
+  <si>
+    <t>TIM6</t>
   </si>
 </sst>
 </file>
@@ -2338,10 +2341,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2666,7 +2669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53AA772F-4124-4842-BA10-D27E5C5CE960}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -2871,7 +2874,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A0B1F19-81B2-DE4D-B058-6D33A4EF2886}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0"/>
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3020,7 +3025,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>600</v>
+        <v>605</v>
       </c>
       <c r="B6" t="s">
         <v>615</v>
@@ -3049,7 +3054,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>605</v>
+        <v>689</v>
       </c>
       <c r="B7" t="s">
         <v>606</v>
@@ -4038,8 +4043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3500D92E-6FB0-8D4D-97D2-7C2457E4D88B}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4178,7 +4183,7 @@
         <v>156</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>596</v>
+        <v>600</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -4201,7 +4206,7 @@
         <v>156</v>
       </c>
       <c r="I6" s="7" t="s">
-        <v>600</v>
+        <v>605</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -4224,7 +4229,7 @@
         <v>157</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>605</v>
+        <v>689</v>
       </c>
     </row>
   </sheetData>
@@ -6073,34 +6078,34 @@
       <c r="A3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="34" t="s">
         <v>114</v>
       </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
@@ -6220,16 +6225,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6669,7 +6674,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
       <selection pane="bottomRight" activeCell="F5" sqref="F5"/>

</xml_diff>

<commit_message>
Update example file. Missed in previous release
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/full_1.xlsx
+++ b/tests/integration_test_files/full_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555060E6-C39F-3148-BF9D-0589625395CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB907C0-2DE8-7944-B12C-C1097C30B007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53480" yWindow="500" windowWidth="44940" windowHeight="26040" firstSheet="3" activeTab="7" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="53480" yWindow="500" windowWidth="44940" windowHeight="26040" firstSheet="2" activeTab="16" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -22,19 +22,21 @@
     <sheet name="studyDesignEligibilityCriteria" sheetId="19" r:id="rId7"/>
     <sheet name="dictionaries" sheetId="23" r:id="rId8"/>
     <sheet name="mainTimeline" sheetId="1" r:id="rId9"/>
-    <sheet name="studyDesignTiming" sheetId="25" r:id="rId10"/>
-    <sheet name="studyDesignActivities" sheetId="16" r:id="rId11"/>
-    <sheet name="studyDesignIndications" sheetId="6" r:id="rId12"/>
-    <sheet name="studyDesignInterventions" sheetId="27" r:id="rId13"/>
-    <sheet name="studyDesignPopulations" sheetId="7" r:id="rId14"/>
-    <sheet name="studyDesignOE" sheetId="8" r:id="rId15"/>
-    <sheet name="studyDesignEstimands" sheetId="9" r:id="rId16"/>
-    <sheet name="studyDesignProcedures" sheetId="11" r:id="rId17"/>
-    <sheet name="studyDesignEncounters" sheetId="12" r:id="rId18"/>
-    <sheet name="studyDesignElements" sheetId="13" r:id="rId19"/>
-    <sheet name="studyDesignContent" sheetId="17" r:id="rId20"/>
-    <sheet name="configuration" sheetId="10" r:id="rId21"/>
-    <sheet name="usefulInfo" sheetId="26" r:id="rId22"/>
+    <sheet name="Sheet1" sheetId="28" r:id="rId10"/>
+    <sheet name="studyDesignTiming" sheetId="25" r:id="rId11"/>
+    <sheet name="studyDesignActivities" sheetId="16" r:id="rId12"/>
+    <sheet name="studyDesignIndications" sheetId="6" r:id="rId13"/>
+    <sheet name="studyDesignInterventions" sheetId="27" r:id="rId14"/>
+    <sheet name="studyDesignPopulations" sheetId="7" r:id="rId15"/>
+    <sheet name="studyDesignOE" sheetId="8" r:id="rId16"/>
+    <sheet name="Sheet2" sheetId="29" r:id="rId17"/>
+    <sheet name="studyDesignEstimands" sheetId="9" r:id="rId18"/>
+    <sheet name="studyDesignProcedures" sheetId="11" r:id="rId19"/>
+    <sheet name="studyDesignEncounters" sheetId="12" r:id="rId20"/>
+    <sheet name="studyDesignElements" sheetId="13" r:id="rId21"/>
+    <sheet name="studyDesignContent" sheetId="17" r:id="rId22"/>
+    <sheet name="configuration" sheetId="10" r:id="rId23"/>
+    <sheet name="usefulInfo" sheetId="26" r:id="rId24"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="726">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="726">
   <si>
     <t>Screening</t>
   </si>
@@ -2458,10 +2460,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2988,6 +2990,18 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B76FC554-66AC-E24E-8285-2C16201A5A8B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A0B1F19-81B2-DE4D-B058-6D33A4EF2886}">
   <dimension ref="A1:I7"/>
   <sheetViews>
@@ -3203,7 +3217,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA8389B3-D1BB-1047-BA06-7E793B938DBA}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -3298,7 +3312,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E548DFC1-EB0E-374B-95D2-A04104B745FB}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -3360,7 +3374,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86117B3B-3975-3B4E-8ED4-B6979F031A31}">
   <dimension ref="A1:S3"/>
   <sheetViews>
@@ -3574,7 +3588,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C037A932-CB5B-8D43-956E-5F5C367E07FC}">
   <dimension ref="A1:I4"/>
   <sheetViews>
@@ -3673,7 +3687,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B908C5D6-C6A1-4043-A49A-69C599CFBAE9}">
   <dimension ref="A1:M26"/>
   <sheetViews>
@@ -4115,7 +4129,132 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E21BFD86-228C-9E4F-A6E0-17C33821FA3D}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40" customWidth="1"/>
+    <col min="2" max="2" width="92.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
+        <v>650</v>
+      </c>
+      <c r="B1" s="38"/>
+    </row>
+    <row r="2" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
+        <v>655</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="32" t="s">
+        <v>638</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="32" t="s">
+        <v>639</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="32" t="s">
+        <v>640</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="32" t="s">
+        <v>642</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="32" t="s">
+        <v>641</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="39" t="s">
+        <v>651</v>
+      </c>
+      <c r="B10" s="39"/>
+    </row>
+    <row r="11" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" s="31" t="s">
+        <v>655</v>
+      </c>
+      <c r="B11" s="30" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="32" t="s">
+        <v>657</v>
+      </c>
+      <c r="B12" s="29" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="32" t="s">
+        <v>648</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="32" t="s">
+        <v>649</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>654</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A10:B10"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{8095E3C2-5E8C-CD42-9844-EF750C313C05}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{21593E62-5188-8D40-8EDA-0B7363B2CE1D}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{E1F9617B-866B-F347-8AE6-4F68B78A1880}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{5C05D2D5-DDA4-424E-9721-32B897827DE4}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{93A65D4B-7872-D845-BE5F-B7B119471ECA}"/>
+    <hyperlink ref="B12" r:id="rId6" xr:uid="{C42104DA-D938-D547-A04F-2E7BDE4D535E}"/>
+    <hyperlink ref="B13" r:id="rId7" xr:uid="{AA302D20-8437-9340-B21E-D6FAA7FE938A}"/>
+    <hyperlink ref="B14" r:id="rId8" xr:uid="{89159574-3276-2C4D-AF11-A432372C1C35}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBFC82B4-C495-A142-993D-B6A47D77A4C3}">
   <dimension ref="A1:H5"/>
   <sheetViews>
@@ -4242,7 +4381,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D608A778-255D-4443-A7EA-03049F1FC98F}">
   <dimension ref="A1:G5"/>
   <sheetViews>
@@ -4332,330 +4471,6 @@
       <c r="D5" s="4"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3500D92E-6FB0-8D4D-97D2-7C2457E4D88B}">
-  <dimension ref="A1:I7"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="7.33203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9" style="3" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="20.83203125" style="3" customWidth="1"/>
-    <col min="7" max="8" width="22" style="3" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="7" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
-        <v>395</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>466</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>538</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>539</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="I1" s="25" t="s">
-        <v>568</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>150</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>152</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>555</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>582</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>153</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>600</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>590</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>596</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>602</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>601</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>671</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{137D84F3-D0D8-A149-BA12-7DBD407EC782}">
-  <dimension ref="A1:E6"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9.1640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="24.83203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="15" style="3" customWidth="1"/>
-    <col min="4" max="4" width="23.5" style="3" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
-        <v>395</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>535</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>159</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>160</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>161</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>162</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4783,6 +4598,330 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3500D92E-6FB0-8D4D-97D2-7C2457E4D88B}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="7.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="9" style="3" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="20.83203125" style="3" customWidth="1"/>
+    <col min="7" max="8" width="22" style="3" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="7" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>395</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>466</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>538</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>539</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>590</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>596</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>671</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{137D84F3-D0D8-A149-BA12-7DBD407EC782}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15" style="3" customWidth="1"/>
+    <col min="4" max="4" width="23.5" style="3" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>395</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>535</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>162</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F40359-1191-3843-B5C3-38D19A754655}">
   <dimension ref="A1:D139"/>
   <sheetViews>
@@ -6041,7 +6180,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1886B59F-3C17-014D-9C61-BEC33F421A82}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -6075,7 +6214,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6CCACBD-9050-2546-A791-CCDEA21B15F7}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -6375,34 +6514,34 @@
       <c r="A3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
@@ -6522,16 +6661,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="B5:E5"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6841,7 +6980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EB40753-8F7D-3941-9F21-F336F33F75CC}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Tweaks and readme updates
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/full_1.xlsx
+++ b/tests/integration_test_files/full_1.xlsx
@@ -8,33 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C87364B-3093-454E-82D6-F3C74D9FE1B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83943463-07EF-224D-AA1D-957E4EB531FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="500" windowWidth="44940" windowHeight="26040" firstSheet="5" activeTab="7" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="1740" yWindow="500" windowWidth="44940" windowHeight="26040" activeTab="4" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
     <sheet name="studyAmendments" sheetId="18" r:id="rId2"/>
     <sheet name="studyIdentifiers" sheetId="3" r:id="rId3"/>
     <sheet name="studyDesign" sheetId="4" r:id="rId4"/>
-    <sheet name="studyDesignArms" sheetId="15" r:id="rId5"/>
-    <sheet name="studyDesignEpochs" sheetId="14" r:id="rId6"/>
-    <sheet name="studyDesignEligibilityCriteria" sheetId="19" r:id="rId7"/>
-    <sheet name="dictionaries" sheetId="23" r:id="rId8"/>
-    <sheet name="mainTimeline" sheetId="1" r:id="rId9"/>
-    <sheet name="studyDesignTiming" sheetId="25" r:id="rId10"/>
-    <sheet name="studyDesignActivities" sheetId="16" r:id="rId11"/>
-    <sheet name="studyDesignIndications" sheetId="6" r:id="rId12"/>
-    <sheet name="studyDesignInterventions" sheetId="27" r:id="rId13"/>
-    <sheet name="studyDesignPopulations" sheetId="7" r:id="rId14"/>
-    <sheet name="studyDesignOE" sheetId="8" r:id="rId15"/>
-    <sheet name="studyDesignEstimands" sheetId="9" r:id="rId16"/>
-    <sheet name="studyDesignProcedures" sheetId="11" r:id="rId17"/>
-    <sheet name="studyDesignEncounters" sheetId="12" r:id="rId18"/>
-    <sheet name="studyDesignElements" sheetId="13" r:id="rId19"/>
-    <sheet name="studyDesignContent" sheetId="17" r:id="rId20"/>
-    <sheet name="configuration" sheetId="10" r:id="rId21"/>
-    <sheet name="usefulInfo" sheetId="26" r:id="rId22"/>
+    <sheet name="studyDesignSites" sheetId="30" r:id="rId5"/>
+    <sheet name="studyDesignArms" sheetId="15" r:id="rId6"/>
+    <sheet name="studyDesignEpochs" sheetId="14" r:id="rId7"/>
+    <sheet name="studyDesignEligibilityCriteria" sheetId="19" r:id="rId8"/>
+    <sheet name="dictionaries" sheetId="23" r:id="rId9"/>
+    <sheet name="mainTimeline" sheetId="1" r:id="rId10"/>
+    <sheet name="studyDesignTiming" sheetId="25" r:id="rId11"/>
+    <sheet name="studyDesignActivities" sheetId="16" r:id="rId12"/>
+    <sheet name="studyDesignIndications" sheetId="6" r:id="rId13"/>
+    <sheet name="studyDesignInterventions" sheetId="27" r:id="rId14"/>
+    <sheet name="studyDesignPopulations" sheetId="7" r:id="rId15"/>
+    <sheet name="studyDesignOE" sheetId="8" r:id="rId16"/>
+    <sheet name="studyDesignEstimands" sheetId="9" r:id="rId17"/>
+    <sheet name="studyDesignProcedures" sheetId="11" r:id="rId18"/>
+    <sheet name="studyDesignEncounters" sheetId="12" r:id="rId19"/>
+    <sheet name="studyDesignElements" sheetId="13" r:id="rId20"/>
+    <sheet name="studyDesignContent" sheetId="17" r:id="rId21"/>
+    <sheet name="configuration" sheetId="10" r:id="rId22"/>
+    <sheet name="usefulInfo" sheetId="26" r:id="rId23"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="729">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="747">
   <si>
     <t>Screening</t>
   </si>
@@ -2244,6 +2245,60 @@
   </si>
   <si>
     <t>includesHealthySubjects</t>
+  </si>
+  <si>
+    <t>siteName</t>
+  </si>
+  <si>
+    <t>siteDescription</t>
+  </si>
+  <si>
+    <t>siteLabel</t>
+  </si>
+  <si>
+    <t>identifierScheme</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>SITE_ORG_1</t>
+  </si>
+  <si>
+    <t>SITE_1</t>
+  </si>
+  <si>
+    <t>Site One</t>
+  </si>
+  <si>
+    <t>Main Site</t>
+  </si>
+  <si>
+    <t>Site Org</t>
+  </si>
+  <si>
+    <t>SITE_2</t>
+  </si>
+  <si>
+    <t>Site Two</t>
+  </si>
+  <si>
+    <t>Secondary Site</t>
+  </si>
+  <si>
+    <t>SITE_ORG_2</t>
+  </si>
+  <si>
+    <t>Clinical Trials Org</t>
+  </si>
+  <si>
+    <t>SITE_3</t>
+  </si>
+  <si>
+    <t>Only Site</t>
+  </si>
+  <si>
+    <t>Only site</t>
   </si>
 </sst>
 </file>
@@ -3001,6 +3056,339 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="35.83203125" style="1" customWidth="1"/>
+    <col min="4" max="9" width="12.33203125" style="1" customWidth="1"/>
+    <col min="10" max="11" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>393</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>590</v>
+      </c>
+      <c r="I2" s="28" t="s">
+        <v>589</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>464</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>592</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>587</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="13"/>
+      <c r="C4" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>554</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="13"/>
+      <c r="C5" s="13" t="s">
+        <v>556</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>547</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>588</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>549</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="13"/>
+      <c r="C6" s="13" t="s">
+        <v>558</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="28" t="s">
+        <v>591</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="13" t="s">
+        <v>559</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="13" t="s">
+        <v>560</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>604</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>542</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>609</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>600</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A0B1F19-81B2-DE4D-B058-6D33A4EF2886}">
   <dimension ref="A1:I7"/>
   <sheetViews>
@@ -3216,7 +3604,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA8389B3-D1BB-1047-BA06-7E793B938DBA}">
   <dimension ref="A1:E6"/>
   <sheetViews>
@@ -3311,7 +3699,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E548DFC1-EB0E-374B-95D2-A04104B745FB}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -3373,7 +3761,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86117B3B-3975-3B4E-8ED4-B6979F031A31}">
   <dimension ref="A1:S3"/>
   <sheetViews>
@@ -3587,7 +3975,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C037A932-CB5B-8D43-956E-5F5C367E07FC}">
   <dimension ref="A1:I4"/>
   <sheetViews>
@@ -3689,7 +4077,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B908C5D6-C6A1-4043-A49A-69C599CFBAE9}">
   <dimension ref="A1:M26"/>
   <sheetViews>
@@ -4131,7 +4519,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBFC82B4-C495-A142-993D-B6A47D77A4C3}">
   <dimension ref="A1:H5"/>
   <sheetViews>
@@ -4258,7 +4646,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D608A778-255D-4443-A7EA-03049F1FC98F}">
   <dimension ref="A1:G5"/>
   <sheetViews>
@@ -4352,7 +4740,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3500D92E-6FB0-8D4D-97D2-7C2457E4D88B}">
   <dimension ref="A1:I7"/>
   <sheetViews>
@@ -4543,131 +4931,6 @@
       </c>
       <c r="I7" s="1" t="s">
         <v>668</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{137D84F3-D0D8-A149-BA12-7DBD407EC782}">
-  <dimension ref="A1:E6"/>
-  <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="9.1640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="24.83203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="15" style="3" customWidth="1"/>
-    <col min="4" max="4" width="23.5" style="3" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" style="3" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
-        <v>393</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>532</v>
-      </c>
-      <c r="D1" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>157</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>158</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>159</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>160</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -4799,6 +5062,131 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{137D84F3-D0D8-A149-BA12-7DBD407EC782}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15" style="3" customWidth="1"/>
+    <col min="4" max="4" width="23.5" style="3" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>393</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>532</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>158</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F40359-1191-3843-B5C3-38D19A754655}">
   <dimension ref="A1:D139"/>
   <sheetViews>
@@ -6057,7 +6445,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1886B59F-3C17-014D-9C61-BEC33F421A82}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -6091,7 +6479,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6CCACBD-9050-2546-A791-CCDEA21B15F7}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -6221,7 +6609,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6355,7 +6743,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B9" sqref="B9:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6591,6 +6979,130 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F32E2E6C-EC56-2C43-9AA4-39E342213E19}">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="17.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="26.5" style="3" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="50" style="3" customWidth="1"/>
+    <col min="7" max="7" width="11.1640625" style="3" customWidth="1"/>
+    <col min="8" max="9" width="17.83203125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>393</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>464</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>732</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>497</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>733</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>729</v>
+      </c>
+      <c r="H1" s="19" t="s">
+        <v>730</v>
+      </c>
+      <c r="I1" s="19" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>734</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>738</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="3">
+        <v>123456789</v>
+      </c>
+      <c r="F2" t="s">
+        <v>610</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>735</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>737</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F3"/>
+      <c r="G3" s="3" t="s">
+        <v>739</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>741</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>742</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="3">
+        <v>234567891</v>
+      </c>
+      <c r="F4" t="s">
+        <v>611</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>744</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>745</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>746</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D7FA707-26D8-0546-9A99-D418F7F4E088}">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -6676,7 +7188,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07E1D5BD-3A57-0140-9167-DAF5A3D4D9EF}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -6767,7 +7279,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED1B92D-F8EC-D24D-81E6-6B85449D22F0}">
   <dimension ref="A1:G5"/>
   <sheetViews>
@@ -6890,11 +7402,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EB40753-8F7D-3941-9F21-F336F33F75CC}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -7017,337 +7529,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
-  <dimension ref="A1:K13"/>
-  <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5" style="3" customWidth="1"/>
-    <col min="3" max="3" width="35.83203125" style="1" customWidth="1"/>
-    <col min="4" max="9" width="12.33203125" style="1" customWidth="1"/>
-    <col min="10" max="11" width="10.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>393</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>544</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>545</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>547</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>588</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>552</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>590</v>
-      </c>
-      <c r="I2" s="28" t="s">
-        <v>589</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>464</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>553</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>552</v>
-      </c>
-      <c r="H3" s="28" t="s">
-        <v>592</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>587</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="13"/>
-      <c r="C4" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>554</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>554</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>554</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>554</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>555</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>554</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
-      <c r="C5" s="13" t="s">
-        <v>556</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>545</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>547</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>548</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>588</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>549</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="13"/>
-      <c r="C6" s="13" t="s">
-        <v>558</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="28" t="s">
-        <v>591</v>
-      </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="13" t="s">
-        <v>559</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="13" t="s">
-        <v>560</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>604</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>542</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>609</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>608</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>600</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>601</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add flexibility for title page and toc
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/full_1.xlsx
+++ b/tests/integration_test_files/full_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EEDB3C-F6D4-274D-9DC1-35AED4A0C25E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3787FE54-9FD9-474E-A6E7-0A55C5F3874C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31500" yWindow="500" windowWidth="44940" windowHeight="26040" firstSheet="9" activeTab="21" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
@@ -2314,9 +2314,6 @@
     <t>Yes</t>
   </si>
   <si>
-    <t>&lt;usdm:ref  template="m11" section="title_page"&gt;</t>
-  </si>
-  <si>
     <t>&lt;usdm:ref  template="m11" section="objective_endpoints"&gt;</t>
   </si>
   <si>
@@ -2324,6 +2321,9 @@
   </si>
   <si>
     <t>&lt;usdm:ref  template="m11" section="exclusion"&gt;</t>
+  </si>
+  <si>
+    <t>&lt;usdm:ref title_page="true"/&gt;&lt;usdm:ref table_of_contents="true"/&gt;&lt;usdm:ref  template="m11" section="title_page"&gt;</t>
   </si>
 </sst>
 </file>
@@ -2547,10 +2547,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -5296,7 +5296,7 @@
   <dimension ref="A1:D139"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5321,7 +5321,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>607</v>
       </c>
@@ -5330,7 +5330,7 @@
         <v>606</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>751</v>
+        <v>754</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5406,7 +5406,7 @@
         <v>458</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5524,7 +5524,7 @@
         <v>215</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5536,7 +5536,7 @@
         <v>216</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -6884,34 +6884,34 @@
       <c r="A3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="36" t="s">
         <v>131</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
@@ -7064,6 +7064,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="B8:E8"/>
@@ -7072,11 +7077,6 @@
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Update readme and full example 1
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/full_1.xlsx
+++ b/tests/integration_test_files/full_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0A4E56-AFB8-F546-A2BC-D0ADC7E044B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8085653-CBFB-554F-A9D7-6871A6A0CC36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19460" firstSheet="10" activeTab="16" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="25120" yWindow="500" windowWidth="33600" windowHeight="19460" activeTab="7" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="755">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="761">
   <si>
     <t>Screening</t>
   </si>
@@ -1906,24 +1906,9 @@
     <t>OE Dictionary</t>
   </si>
   <si>
-    <t>Berber_Dict</t>
-  </si>
-  <si>
-    <t>Dictionary for Berber Example</t>
-  </si>
-  <si>
-    <t>Berber Dictionary</t>
-  </si>
-  <si>
     <t>xxxx</t>
   </si>
   <si>
-    <t>Berber</t>
-  </si>
-  <si>
-    <t>Test for Berber</t>
-  </si>
-  <si>
     <t>Model</t>
   </si>
   <si>
@@ -2324,6 +2309,39 @@
   </si>
   <si>
     <t>The secondary efficacy objective for this study is to evaluate the efficacy of TCZ compared with placebo in combination with SOC for the treatment of severe COVID-19 pneumonia over the age of &lt;usdm:tag name="min_age"/&gt;</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>Example3_Dict</t>
+  </si>
+  <si>
+    <t>Example 3 Dictionary</t>
+  </si>
+  <si>
+    <t>Dictionary for Example</t>
+  </si>
+  <si>
+    <t>value_key</t>
+  </si>
+  <si>
+    <t>Missing Tag</t>
+  </si>
+  <si>
+    <t>Test for missing tag</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>Value Example</t>
+  </si>
+  <si>
+    <t>Test for value dict key</t>
+  </si>
+  <si>
+    <t>If the value is equal to &lt;usdm:tag name="value_key"/&gt;</t>
   </si>
 </sst>
 </file>
@@ -2547,10 +2565,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3594,7 +3612,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>654</v>
+        <v>649</v>
       </c>
       <c r="B7" t="s">
         <v>577</v>
@@ -3657,24 +3675,24 @@
         <v>194</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>733</v>
+        <v>728</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>734</v>
+        <v>729</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>735</v>
+        <v>730</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>742</v>
+        <v>737</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>596</v>
@@ -3685,16 +3703,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>739</v>
+        <v>734</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>130</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>596</v>
@@ -3705,16 +3723,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>737</v>
+        <v>732</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>740</v>
+        <v>735</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>741</v>
+        <v>736</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>744</v>
+        <v>739</v>
       </c>
       <c r="E4" s="4"/>
       <c r="F4" t="s">
@@ -3835,7 +3853,7 @@
         <v>460</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>745</v>
+        <v>740</v>
       </c>
       <c r="E1" s="18" t="s">
         <v>44</v>
@@ -3846,13 +3864,13 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="C2" t="s">
-        <v>655</v>
+        <v>650</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>746</v>
+        <v>741</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>45</v>
@@ -3863,10 +3881,10 @@
         <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>658</v>
+        <v>653</v>
       </c>
       <c r="C3" t="s">
-        <v>656</v>
+        <v>651</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>130</v>
@@ -3926,49 +3944,49 @@
         <v>44</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>659</v>
+        <v>654</v>
       </c>
       <c r="F1" s="18" t="s">
         <v>42</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="H1" s="18" t="s">
+        <v>655</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>656</v>
+      </c>
+      <c r="J1" s="18" t="s">
         <v>660</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="K1" s="18" t="s">
         <v>661</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="L1" s="18" t="s">
+        <v>662</v>
+      </c>
+      <c r="M1" s="18" t="s">
+        <v>657</v>
+      </c>
+      <c r="N1" s="18" t="s">
+        <v>658</v>
+      </c>
+      <c r="O1" s="18" t="s">
+        <v>659</v>
+      </c>
+      <c r="P1" s="18" t="s">
+        <v>663</v>
+      </c>
+      <c r="Q1" s="18" t="s">
+        <v>664</v>
+      </c>
+      <c r="R1" s="18" t="s">
         <v>665</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="S1" s="18" t="s">
         <v>666</v>
-      </c>
-      <c r="L1" s="18" t="s">
-        <v>667</v>
-      </c>
-      <c r="M1" s="18" t="s">
-        <v>662</v>
-      </c>
-      <c r="N1" s="18" t="s">
-        <v>663</v>
-      </c>
-      <c r="O1" s="18" t="s">
-        <v>664</v>
-      </c>
-      <c r="P1" s="18" t="s">
-        <v>668</v>
-      </c>
-      <c r="Q1" s="18" t="s">
-        <v>669</v>
-      </c>
-      <c r="R1" s="18" t="s">
-        <v>670</v>
-      </c>
-      <c r="S1" s="18" t="s">
-        <v>671</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
@@ -3976,58 +3994,58 @@
         <v>64</v>
       </c>
       <c r="B2" t="s">
+        <v>667</v>
+      </c>
+      <c r="C2" t="s">
+        <v>668</v>
+      </c>
+      <c r="D2" t="s">
+        <v>669</v>
+      </c>
+      <c r="E2" t="s">
         <v>672</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F2" s="33" t="s">
+        <v>684</v>
+      </c>
+      <c r="G2" t="s">
+        <v>670</v>
+      </c>
+      <c r="H2" t="s">
         <v>673</v>
       </c>
-      <c r="D2" t="s">
+      <c r="I2" t="s">
+        <v>671</v>
+      </c>
+      <c r="J2" t="s">
         <v>674</v>
       </c>
-      <c r="E2" t="s">
+      <c r="K2" t="s">
+        <v>675</v>
+      </c>
+      <c r="L2" t="s">
+        <v>676</v>
+      </c>
+      <c r="M2" t="s">
+        <v>682</v>
+      </c>
+      <c r="N2" t="s">
         <v>677</v>
       </c>
-      <c r="F2" s="33" t="s">
-        <v>689</v>
-      </c>
-      <c r="G2" t="s">
-        <v>675</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="O2" t="s">
+        <v>683</v>
+      </c>
+      <c r="P2" t="s">
         <v>678</v>
-      </c>
-      <c r="I2" t="s">
-        <v>676</v>
-      </c>
-      <c r="J2" t="s">
-        <v>679</v>
-      </c>
-      <c r="K2" t="s">
-        <v>680</v>
-      </c>
-      <c r="L2" t="s">
-        <v>681</v>
-      </c>
-      <c r="M2" t="s">
-        <v>687</v>
-      </c>
-      <c r="N2" t="s">
-        <v>682</v>
-      </c>
-      <c r="O2" t="s">
-        <v>688</v>
-      </c>
-      <c r="P2" t="s">
-        <v>683</v>
       </c>
       <c r="Q2" t="s">
         <v>130</v>
       </c>
       <c r="R2" t="s">
-        <v>684</v>
+        <v>679</v>
       </c>
       <c r="S2" s="32" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
@@ -4035,58 +4053,58 @@
         <v>66</v>
       </c>
       <c r="B3" t="s">
+        <v>685</v>
+      </c>
+      <c r="C3" t="s">
+        <v>686</v>
+      </c>
+      <c r="D3" t="s">
+        <v>669</v>
+      </c>
+      <c r="E3" t="s">
+        <v>687</v>
+      </c>
+      <c r="F3" s="33" t="s">
+        <v>684</v>
+      </c>
+      <c r="G3" t="s">
+        <v>670</v>
+      </c>
+      <c r="H3" t="s">
+        <v>688</v>
+      </c>
+      <c r="I3" t="s">
+        <v>671</v>
+      </c>
+      <c r="J3" t="s">
+        <v>689</v>
+      </c>
+      <c r="K3" t="s">
         <v>690</v>
       </c>
-      <c r="C3" t="s">
+      <c r="L3" t="s">
         <v>691</v>
       </c>
-      <c r="D3" t="s">
-        <v>674</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="M3" t="s">
+        <v>682</v>
+      </c>
+      <c r="N3" t="s">
+        <v>677</v>
+      </c>
+      <c r="O3" t="s">
+        <v>683</v>
+      </c>
+      <c r="P3" t="s">
         <v>692</v>
-      </c>
-      <c r="F3" s="33" t="s">
-        <v>689</v>
-      </c>
-      <c r="G3" t="s">
-        <v>675</v>
-      </c>
-      <c r="H3" t="s">
-        <v>693</v>
-      </c>
-      <c r="I3" t="s">
-        <v>676</v>
-      </c>
-      <c r="J3" t="s">
-        <v>694</v>
-      </c>
-      <c r="K3" t="s">
-        <v>695</v>
-      </c>
-      <c r="L3" t="s">
-        <v>696</v>
-      </c>
-      <c r="M3" t="s">
-        <v>687</v>
-      </c>
-      <c r="N3" t="s">
-        <v>682</v>
-      </c>
-      <c r="O3" t="s">
-        <v>688</v>
-      </c>
-      <c r="P3" t="s">
-        <v>697</v>
       </c>
       <c r="Q3" t="s">
         <v>130</v>
       </c>
       <c r="R3" t="s">
-        <v>684</v>
+        <v>679</v>
       </c>
       <c r="S3" s="32" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
     </row>
   </sheetData>
@@ -4116,7 +4134,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
-        <v>698</v>
+        <v>693</v>
       </c>
       <c r="B1" s="16" t="s">
         <v>389</v>
@@ -4128,24 +4146,24 @@
         <v>460</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>699</v>
+        <v>694</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>700</v>
+        <v>695</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>711</v>
+        <v>706</v>
       </c>
       <c r="H1" s="16" t="s">
         <v>48</v>
       </c>
       <c r="I1" s="34" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>701</v>
+        <v>696</v>
       </c>
       <c r="B2" t="s">
         <v>503</v>
@@ -4165,13 +4183,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>702</v>
+        <v>697</v>
       </c>
       <c r="B3" t="s">
-        <v>703</v>
+        <v>698</v>
       </c>
       <c r="G3" t="s">
-        <v>712</v>
+        <v>707</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>130</v>
@@ -4179,13 +4197,13 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>702</v>
+        <v>697</v>
       </c>
       <c r="B4" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="G4" t="s">
-        <v>713</v>
+        <v>708</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>130</v>
@@ -4200,7 +4218,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B908C5D6-C6A1-4043-A49A-69C599CFBAE9}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -4300,7 +4318,7 @@
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="12" t="s">
-        <v>754</v>
+        <v>749</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>58</v>
@@ -4899,7 +4917,7 @@
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10" t="s">
-        <v>710</v>
+        <v>705</v>
       </c>
       <c r="G2" s="10"/>
     </row>
@@ -5157,7 +5175,7 @@
         <v>142</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>654</v>
+        <v>649</v>
       </c>
     </row>
   </sheetData>
@@ -5330,7 +5348,7 @@
         <v>604</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>747</v>
+        <v>742</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5406,7 +5424,7 @@
         <v>458</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>748</v>
+        <v>743</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5524,7 +5542,7 @@
         <v>215</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>749</v>
+        <v>744</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -5536,7 +5554,7 @@
         <v>216</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>750</v>
+        <v>745</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -6600,94 +6618,94 @@
   <sheetData>
     <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
-        <v>633</v>
+        <v>628</v>
       </c>
       <c r="B1" s="38"/>
     </row>
     <row r="2" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="30" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="31" t="s">
+        <v>616</v>
+      </c>
+      <c r="B3" s="28" t="s">
         <v>621</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="31" t="s">
+        <v>617</v>
+      </c>
+      <c r="B4" s="28" t="s">
         <v>622</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="31" t="s">
+        <v>618</v>
+      </c>
+      <c r="B5" s="28" t="s">
         <v>623</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="31" t="s">
-        <v>625</v>
+        <v>620</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="31" t="s">
-        <v>624</v>
+        <v>619</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="39" t="s">
-        <v>634</v>
+        <v>629</v>
       </c>
       <c r="B10" s="39"/>
     </row>
     <row r="11" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="30" t="s">
-        <v>638</v>
+        <v>633</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>639</v>
+        <v>634</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="31" t="s">
-        <v>640</v>
+        <v>635</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>635</v>
+        <v>630</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="31" t="s">
+        <v>626</v>
+      </c>
+      <c r="B13" s="28" t="s">
         <v>631</v>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="31" t="s">
+        <v>627</v>
+      </c>
+      <c r="B14" s="28" t="s">
         <v>632</v>
-      </c>
-      <c r="B14" s="28" t="s">
-        <v>637</v>
       </c>
     </row>
   </sheetData>
@@ -6789,53 +6807,53 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>636</v>
+      </c>
+      <c r="B4" t="s">
+        <v>639</v>
+      </c>
+      <c r="C4" t="s">
+        <v>642</v>
+      </c>
+      <c r="D4" t="s">
         <v>641</v>
       </c>
-      <c r="B4" t="s">
-        <v>644</v>
-      </c>
-      <c r="C4" t="s">
-        <v>647</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>646</v>
-      </c>
-      <c r="E4" t="s">
-        <v>651</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
       <c r="B5" t="s">
-        <v>645</v>
+        <v>640</v>
       </c>
       <c r="C5" t="s">
-        <v>648</v>
+        <v>643</v>
       </c>
       <c r="D5" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
       <c r="E5" t="s">
-        <v>652</v>
+        <v>647</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>650</v>
+        <v>645</v>
       </c>
       <c r="B6" t="s">
-        <v>643</v>
+        <v>638</v>
       </c>
       <c r="C6" t="s">
-        <v>649</v>
+        <v>644</v>
       </c>
       <c r="D6" t="s">
         <v>114</v>
       </c>
       <c r="E6" t="s">
-        <v>653</v>
+        <v>648</v>
       </c>
     </row>
   </sheetData>
@@ -6884,34 +6902,34 @@
       <c r="A3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="37" t="s">
         <v>131</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
@@ -6948,10 +6966,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="C9" s="35"/>
       <c r="D9" s="35"/>
@@ -6959,10 +6977,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="B10" s="35" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="C10" s="35"/>
       <c r="D10" s="35"/>
@@ -6970,10 +6988,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
       <c r="C11" s="35"/>
       <c r="D11" s="35"/>
@@ -7064,11 +7082,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="B8:E8"/>
@@ -7077,6 +7090,11 @@
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -7113,30 +7131,30 @@
         <v>42</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="E1" s="16" t="s">
         <v>493</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>719</v>
+        <v>714</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>715</v>
+        <v>710</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>716</v>
+        <v>711</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>717</v>
+        <v>712</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>720</v>
+        <v>715</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>724</v>
+        <v>719</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>113</v>
@@ -7151,33 +7169,33 @@
         <v>602</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>721</v>
+        <v>716</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>723</v>
+        <v>718</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>722</v>
+        <v>717</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F3"/>
       <c r="G3" s="3" t="s">
-        <v>725</v>
+        <v>720</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>727</v>
+        <v>722</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>726</v>
+        <v>721</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>728</v>
+        <v>723</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>729</v>
+        <v>724</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>113</v>
@@ -7192,13 +7210,13 @@
         <v>603</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>730</v>
+        <v>725</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>731</v>
+        <v>726</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>732</v>
+        <v>727</v>
       </c>
     </row>
   </sheetData>
@@ -7386,10 +7404,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED1B92D-F8EC-D24D-81E6-6B85449D22F0}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7400,6 +7418,7 @@
     <col min="4" max="4" width="29.5" customWidth="1"/>
     <col min="5" max="5" width="10.1640625" customWidth="1"/>
     <col min="6" max="6" width="64.83203125" customWidth="1"/>
+    <col min="7" max="7" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -7426,80 +7445,106 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>505</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="4" t="s">
         <v>506</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>507</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="9" t="s">
+        <v>746</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>509</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>511</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="9" t="s">
+        <v>747</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>606</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>606</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>509</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>755</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>756</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>748</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>751</v>
       </c>
-      <c r="G2" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>505</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>509</v>
-      </c>
-      <c r="C3" t="s">
-        <v>510</v>
-      </c>
-      <c r="D3" t="s">
-        <v>511</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>752</v>
-      </c>
-      <c r="G3" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
         <v>606</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>506</v>
-      </c>
-      <c r="C4" t="s">
-        <v>607</v>
-      </c>
-      <c r="D4" t="s">
-        <v>608</v>
-      </c>
-      <c r="F4" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>606</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>509</v>
-      </c>
-      <c r="C5" t="s">
-        <v>619</v>
-      </c>
-      <c r="D5" t="s">
-        <v>620</v>
-      </c>
-      <c r="F5" t="s">
-        <v>753</v>
-      </c>
-      <c r="G5" t="s">
-        <v>615</v>
+      <c r="B6" s="4" t="s">
+        <v>757</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>758</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>759</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>760</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>751</v>
       </c>
     </row>
   </sheetData>
@@ -7509,10 +7554,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EB40753-8F7D-3941-9F21-F336F33F75CC}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7525,7 +7570,7 @@
     <col min="7" max="7" width="31.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="18" t="s">
         <v>389</v>
       </c>
@@ -7547,8 +7592,11 @@
       <c r="G1" s="18" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" s="18" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>498</v>
       </c>
@@ -7568,10 +7616,10 @@
         <v>503</v>
       </c>
       <c r="G2" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
         <v>504</v>
       </c>
@@ -7582,10 +7630,10 @@
         <v>503</v>
       </c>
       <c r="G3" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>612</v>
       </c>
@@ -7605,21 +7653,21 @@
         <v>503</v>
       </c>
       <c r="G4" t="s">
-        <v>711</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>751</v>
+      </c>
+      <c r="B5" t="s">
+        <v>753</v>
+      </c>
+      <c r="C5" t="s">
+        <v>752</v>
+      </c>
+      <c r="D5" t="s">
         <v>615</v>
-      </c>
-      <c r="B5" t="s">
-        <v>616</v>
-      </c>
-      <c r="C5" t="s">
-        <v>617</v>
-      </c>
-      <c r="D5" t="s">
-        <v>618</v>
       </c>
       <c r="E5" t="s">
         <v>546</v>
@@ -7629,6 +7677,14 @@
       </c>
       <c r="G5" t="s">
         <v>460</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>754</v>
+      </c>
+      <c r="H6">
+        <v>1234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update for multiple documents/templates, tests not working
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/full_1.xlsx
+++ b/tests/integration_test_files/full_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E47FB6-ECE8-CE44-B045-1850F66B36C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43961C3E-A09E-DC46-8B5A-C3522785A92E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17280" activeTab="9" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="31560" yWindow="9100" windowWidth="29400" windowHeight="17280" firstSheet="16" activeTab="23" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -34,9 +34,10 @@
     <sheet name="studyDesignProcedures" sheetId="11" r:id="rId19"/>
     <sheet name="studyDesignEncounters" sheetId="12" r:id="rId20"/>
     <sheet name="studyDesignElements" sheetId="13" r:id="rId21"/>
-    <sheet name="studyDesignContent" sheetId="17" r:id="rId22"/>
-    <sheet name="configuration" sheetId="10" r:id="rId23"/>
-    <sheet name="usefulInfo" sheetId="26" r:id="rId24"/>
+    <sheet name="documentContent" sheetId="32" r:id="rId22"/>
+    <sheet name="document" sheetId="17" r:id="rId23"/>
+    <sheet name="configuration" sheetId="10" r:id="rId24"/>
+    <sheet name="usefulInfo" sheetId="26" r:id="rId25"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1015" uniqueCount="759">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="769">
   <si>
     <t>Screening</t>
   </si>
@@ -2336,6 +2337,36 @@
   </si>
   <si>
     <t>Secondary Objective</t>
+  </si>
+  <si>
+    <t>NCI_1</t>
+  </si>
+  <si>
+    <t>NCI_2</t>
+  </si>
+  <si>
+    <t>NCI_3</t>
+  </si>
+  <si>
+    <t>NCI_4</t>
+  </si>
+  <si>
+    <t>NCI_5</t>
+  </si>
+  <si>
+    <t>displaySectionNumber</t>
+  </si>
+  <si>
+    <t>displaySectionTitle</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>Template</t>
+  </si>
+  <si>
+    <t>XXX=document</t>
   </si>
 </sst>
 </file>
@@ -2471,7 +2502,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2559,16 +2590,22 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3093,7 +3130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136502A0-3DDE-CC47-9DA7-EB2F3073B24B}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
@@ -5298,1257 +5335,530 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F40359-1191-3843-B5C3-38D19A754655}">
-  <dimension ref="A1:D139"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5388B46-7AE5-4C42-A1A5-4BAAA12E98C6}">
+  <dimension ref="A1:D100"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24:D25"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="16" style="3" customWidth="1"/>
-    <col min="3" max="3" width="49.83203125" style="9" customWidth="1"/>
-    <col min="4" max="4" width="81.33203125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10" style="3" customWidth="1"/>
+    <col min="2" max="2" width="81.33203125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
-        <v>426</v>
-      </c>
-      <c r="B1" s="21" t="s">
         <v>386</v>
       </c>
-      <c r="C1" s="19" t="s">
-        <v>190</v>
-      </c>
-      <c r="D1" s="19" t="s">
+      <c r="B1" s="19" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
-        <v>602</v>
-      </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="9" t="s">
-        <v>601</v>
-      </c>
-      <c r="D2" s="9" t="s">
+      <c r="A2" s="20" t="s">
+        <v>759</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>735</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="9" t="s">
-        <v>192</v>
+      <c r="A3" s="3" t="s">
+        <v>760</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>736</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
-        <v>323</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>197</v>
+      <c r="A4" s="20" t="s">
+        <v>761</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>737</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
-        <v>324</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>198</v>
+      <c r="A5" s="3" t="s">
+        <v>762</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>738</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
-        <v>325</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
-        <v>326</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
-        <v>327</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
-        <v>328</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
-        <v>329</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
-        <v>454</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>455</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>736</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
-        <v>330</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
-        <v>331</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
-        <v>322</v>
-      </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="9" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
-        <v>332</v>
-      </c>
-      <c r="B15" s="20"/>
-      <c r="C15" s="9" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
-        <v>333</v>
-      </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="9" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
-        <v>334</v>
-      </c>
-      <c r="B17" s="20"/>
-      <c r="C17" s="9" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A18" s="10" t="s">
-        <v>335</v>
-      </c>
-      <c r="B18" s="20"/>
-      <c r="C18" s="9" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
-        <v>409</v>
-      </c>
-      <c r="B19" s="20"/>
-      <c r="C19" s="9" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="10" t="s">
-        <v>410</v>
-      </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="9" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
-        <v>387</v>
-      </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="9" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
-        <v>411</v>
-      </c>
-      <c r="B22" s="20"/>
-      <c r="C22" s="9" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="10" t="s">
-        <v>412</v>
-      </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="9" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
-        <v>413</v>
-      </c>
-      <c r="B24" s="20"/>
-      <c r="C24" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>737</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="10" t="s">
-        <v>414</v>
-      </c>
-      <c r="B25" s="20"/>
-      <c r="C25" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="10" t="s">
-        <v>415</v>
-      </c>
-      <c r="B26" s="20"/>
-      <c r="C26" s="9" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="10" t="s">
-        <v>378</v>
-      </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="9" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="10" t="s">
-        <v>379</v>
-      </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="9" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
-        <v>380</v>
-      </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="9" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A30" s="10" t="s">
-        <v>381</v>
-      </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="9" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="10" t="s">
-        <v>416</v>
-      </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="9" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="10" t="s">
-        <v>388</v>
-      </c>
-      <c r="B32" s="20"/>
-      <c r="C32" s="9" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A33" s="10" t="s">
-        <v>417</v>
-      </c>
-      <c r="B33" s="20"/>
-      <c r="C33" s="9" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="10" t="s">
-        <v>418</v>
-      </c>
-      <c r="B34" s="20"/>
-      <c r="C34" s="9" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="10" t="s">
-        <v>419</v>
-      </c>
-      <c r="B35" s="20"/>
-      <c r="C35" s="9" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="10" t="s">
-        <v>336</v>
-      </c>
-      <c r="B36" s="20"/>
-      <c r="C36" s="9" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A37" s="10" t="s">
-        <v>420</v>
-      </c>
-      <c r="B37" s="20"/>
-      <c r="C37" s="9" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="10" t="s">
-        <v>421</v>
-      </c>
-      <c r="B38" s="20"/>
-      <c r="C38" s="9" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="10" t="s">
-        <v>337</v>
-      </c>
-      <c r="B39" s="20"/>
-      <c r="C39" s="9" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="10" t="s">
-        <v>338</v>
-      </c>
-      <c r="B40" s="20"/>
-      <c r="C40" s="9" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="10" t="s">
-        <v>339</v>
-      </c>
-      <c r="B41" s="20"/>
-      <c r="C41" s="9" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="10" t="s">
-        <v>422</v>
-      </c>
-      <c r="B42" s="20"/>
-      <c r="C42" s="9" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="10" t="s">
-        <v>340</v>
-      </c>
-      <c r="B43" s="20"/>
-      <c r="C43" s="9" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="B44" s="20"/>
-      <c r="C44" s="9" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" s="10" t="s">
-        <v>342</v>
-      </c>
-      <c r="B45" s="20"/>
-      <c r="C45" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="D45" s="9" t="s">
+      <c r="A6" s="20" t="s">
+        <v>763</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="10" t="s">
-        <v>423</v>
-      </c>
-      <c r="B46" s="20"/>
-      <c r="C46" s="9" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="10" t="s">
-        <v>424</v>
-      </c>
-      <c r="B47" s="20"/>
-      <c r="C47" s="9" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="10" t="s">
-        <v>343</v>
-      </c>
-      <c r="B48" s="20"/>
-      <c r="C48" s="9" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" s="10" t="s">
-        <v>344</v>
-      </c>
-      <c r="B49" s="20"/>
-      <c r="C49" s="9" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="10" t="s">
-        <v>345</v>
-      </c>
-      <c r="B50" s="20"/>
-      <c r="C50" s="9" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="10" t="s">
-        <v>346</v>
-      </c>
-      <c r="B51" s="20"/>
-      <c r="C51" s="9" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A52" s="10" t="s">
-        <v>389</v>
-      </c>
-      <c r="B52" s="20"/>
-      <c r="C52" s="9" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="10" t="s">
-        <v>425</v>
-      </c>
-      <c r="B53" s="20"/>
-      <c r="C53" s="9" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A54" s="10" t="s">
-        <v>347</v>
-      </c>
-      <c r="B54" s="20"/>
-      <c r="C54" s="9" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A55" s="10" t="s">
-        <v>348</v>
-      </c>
-      <c r="B55" s="20"/>
-      <c r="C55" s="9" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" s="10" t="s">
-        <v>349</v>
-      </c>
-      <c r="B56" s="20"/>
-      <c r="C56" s="9" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A57" s="10" t="s">
-        <v>427</v>
-      </c>
-      <c r="B57" s="20"/>
-      <c r="C57" s="9" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A58" s="10" t="s">
-        <v>428</v>
-      </c>
-      <c r="B58" s="20"/>
-      <c r="C58" s="9" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" s="10" t="s">
-        <v>429</v>
-      </c>
-      <c r="B59" s="20"/>
-      <c r="C59" s="9" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A60" s="10" t="s">
-        <v>390</v>
-      </c>
-      <c r="B60" s="20"/>
-      <c r="C60" s="9" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A61" s="10" t="s">
-        <v>430</v>
-      </c>
-      <c r="B61" s="20"/>
-      <c r="C61" s="9" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A62" s="10" t="s">
-        <v>431</v>
-      </c>
-      <c r="B62" s="20"/>
-      <c r="C62" s="9" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A63" s="10" t="s">
-        <v>432</v>
-      </c>
-      <c r="B63" s="20"/>
-      <c r="C63" s="9" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A64" s="10" t="s">
-        <v>382</v>
-      </c>
-      <c r="B64" s="20"/>
-      <c r="C64" s="9" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A65" s="10" t="s">
-        <v>350</v>
-      </c>
-      <c r="B65" s="20"/>
-      <c r="C65" s="9" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A66" s="10" t="s">
-        <v>351</v>
-      </c>
-      <c r="B66" s="20"/>
-      <c r="C66" s="9" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A67" s="10" t="s">
-        <v>352</v>
-      </c>
-      <c r="B67" s="20"/>
-      <c r="C67" s="9" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A68" s="10" t="s">
-        <v>353</v>
-      </c>
-      <c r="B68" s="20"/>
-      <c r="C68" s="9" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A69" s="10" t="s">
-        <v>433</v>
-      </c>
-      <c r="B69" s="20"/>
-      <c r="C69" s="9" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A70" s="10" t="s">
-        <v>383</v>
-      </c>
-      <c r="B70" s="20"/>
-      <c r="C70" s="9" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A71" s="10" t="s">
-        <v>354</v>
-      </c>
-      <c r="B71" s="20"/>
-      <c r="C71" s="9" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A72" s="10" t="s">
-        <v>355</v>
-      </c>
-      <c r="B72" s="20"/>
-      <c r="C72" s="9" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A73" s="10" t="s">
-        <v>356</v>
-      </c>
-      <c r="B73" s="20"/>
-      <c r="C73" s="9" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A74" s="10" t="s">
-        <v>357</v>
-      </c>
-      <c r="B74" s="20"/>
-      <c r="C74" s="9" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A75" s="10" t="s">
-        <v>358</v>
-      </c>
-      <c r="B75" s="20"/>
-      <c r="C75" s="9" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A76" s="10" t="s">
-        <v>359</v>
-      </c>
-      <c r="B76" s="20"/>
-      <c r="C76" s="9" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A77" s="10" t="s">
-        <v>360</v>
-      </c>
-      <c r="B77" s="20"/>
-      <c r="C77" s="9" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A78" s="10" t="s">
-        <v>361</v>
-      </c>
-      <c r="B78" s="20"/>
-      <c r="C78" s="9" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A79" s="10" t="s">
-        <v>362</v>
-      </c>
-      <c r="B79" s="20"/>
-      <c r="C79" s="9" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A80" s="10" t="s">
-        <v>434</v>
-      </c>
-      <c r="B80" s="20"/>
-      <c r="C80" s="9" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A81" s="10" t="s">
-        <v>363</v>
-      </c>
-      <c r="B81" s="20"/>
-      <c r="C81" s="9" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A82" s="10" t="s">
-        <v>364</v>
-      </c>
-      <c r="B82" s="20"/>
-      <c r="C82" s="9" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A83" s="10" t="s">
-        <v>435</v>
-      </c>
-      <c r="B83" s="20"/>
-      <c r="C83" s="9" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A84" s="10" t="s">
-        <v>365</v>
-      </c>
-      <c r="B84" s="20"/>
-      <c r="C84" s="9" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A85" s="10" t="s">
-        <v>366</v>
-      </c>
-      <c r="B85" s="20"/>
-      <c r="C85" s="9" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A86" s="10" t="s">
-        <v>367</v>
-      </c>
-      <c r="B86" s="20"/>
-      <c r="C86" s="9" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A87" s="10" t="s">
-        <v>368</v>
-      </c>
-      <c r="B87" s="20"/>
-      <c r="C87" s="9" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A88" s="10" t="s">
-        <v>369</v>
-      </c>
-      <c r="B88" s="20"/>
-      <c r="C88" s="9" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A89" s="10" t="s">
-        <v>436</v>
-      </c>
-      <c r="B89" s="20"/>
-      <c r="C89" s="9" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A90" s="10" t="s">
-        <v>437</v>
-      </c>
-      <c r="B90" s="20"/>
-      <c r="C90" s="9" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A91" s="10" t="s">
-        <v>438</v>
-      </c>
-      <c r="B91" s="20"/>
-      <c r="C91" s="9" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A92" s="10" t="s">
-        <v>430</v>
-      </c>
-      <c r="B92" s="20"/>
-      <c r="C92" s="9" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A93" s="10" t="s">
-        <v>384</v>
-      </c>
-      <c r="B93" s="20"/>
-      <c r="C93" s="9" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A94" s="10" t="s">
-        <v>391</v>
-      </c>
-      <c r="B94" s="20"/>
-      <c r="C94" s="9" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A95" s="10" t="s">
-        <v>439</v>
-      </c>
-      <c r="B95" s="20"/>
-      <c r="C95" s="9" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A96" s="10" t="s">
-        <v>440</v>
-      </c>
-      <c r="B96" s="20"/>
-      <c r="C96" s="9" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A97" s="10" t="s">
-        <v>370</v>
-      </c>
-      <c r="B97" s="20"/>
-      <c r="C97" s="9" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A98" s="10" t="s">
-        <v>371</v>
-      </c>
-      <c r="B98" s="20"/>
-      <c r="C98" s="9" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A99" s="10" t="s">
-        <v>372</v>
-      </c>
-      <c r="B99" s="20"/>
-      <c r="C99" s="9" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A100" s="10" t="s">
-        <v>373</v>
-      </c>
-      <c r="B100" s="20"/>
-      <c r="C100" s="9" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A101" s="10" t="s">
-        <v>374</v>
-      </c>
-      <c r="B101" s="20"/>
-      <c r="C101" s="9" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A102" s="10" t="s">
-        <v>441</v>
-      </c>
-      <c r="B102" s="20"/>
-      <c r="C102" s="9" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A103" s="10" t="s">
-        <v>442</v>
-      </c>
-      <c r="B103" s="20"/>
-      <c r="C103" s="9" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A104" s="10" t="s">
-        <v>443</v>
-      </c>
-      <c r="B104" s="20"/>
-      <c r="C104" s="9" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A105" s="10" t="s">
-        <v>444</v>
-      </c>
-      <c r="B105" s="20"/>
-      <c r="C105" s="9" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A106" s="10" t="s">
-        <v>445</v>
-      </c>
-      <c r="B106" s="20"/>
-      <c r="C106" s="9" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A107" s="10" t="s">
-        <v>446</v>
-      </c>
-      <c r="B107" s="20"/>
-      <c r="C107" s="9" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A108" s="10" t="s">
-        <v>447</v>
-      </c>
-      <c r="B108" s="20"/>
-      <c r="C108" s="9" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A109" s="10" t="s">
-        <v>392</v>
-      </c>
-      <c r="B109" s="20"/>
-      <c r="C109" s="9" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A110" s="10" t="s">
-        <v>448</v>
-      </c>
-      <c r="B110" s="20"/>
-      <c r="C110" s="9" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A111" s="10" t="s">
-        <v>449</v>
-      </c>
-      <c r="B111" s="20"/>
-      <c r="C111" s="9" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A112" s="10" t="s">
-        <v>450</v>
-      </c>
-      <c r="B112" s="20"/>
-      <c r="C112" s="9" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A113" s="10" t="s">
-        <v>451</v>
-      </c>
-      <c r="B113" s="20"/>
-      <c r="C113" s="9" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A114" s="10" t="s">
-        <v>452</v>
-      </c>
-      <c r="B114" s="20"/>
-      <c r="C114" s="9" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A115" s="10" t="s">
-        <v>393</v>
-      </c>
-      <c r="B115" s="20"/>
-      <c r="C115" s="9" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A116" s="10" t="s">
-        <v>408</v>
-      </c>
-      <c r="B116" s="20"/>
-      <c r="C116" s="9" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A117" s="10" t="s">
-        <v>407</v>
-      </c>
-      <c r="B117" s="20"/>
-      <c r="C117" s="9" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A118" s="10" t="s">
-        <v>406</v>
-      </c>
-      <c r="B118" s="20"/>
-      <c r="C118" s="9" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A119" s="10" t="s">
-        <v>394</v>
-      </c>
-      <c r="B119" s="20"/>
-      <c r="C119" s="9" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A120" s="10" t="s">
-        <v>405</v>
-      </c>
-      <c r="B120" s="20"/>
-      <c r="C120" s="9" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A121" s="10" t="s">
-        <v>404</v>
-      </c>
-      <c r="B121" s="20"/>
-      <c r="C121" s="9" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A122" s="10" t="s">
-        <v>403</v>
-      </c>
-      <c r="B122" s="20"/>
-      <c r="C122" s="9" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A123" s="10" t="s">
-        <v>402</v>
-      </c>
-      <c r="B123" s="20"/>
-      <c r="C123" s="9" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A124" s="10" t="s">
-        <v>395</v>
-      </c>
-      <c r="B124" s="20"/>
-      <c r="C124" s="9" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="125" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A125" s="10" t="s">
-        <v>401</v>
-      </c>
-      <c r="B125" s="20"/>
-      <c r="C125" s="9" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A126" s="10" t="s">
-        <v>375</v>
-      </c>
-      <c r="B126" s="20"/>
-      <c r="C126" s="9" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A127" s="10" t="s">
-        <v>376</v>
-      </c>
-      <c r="B127" s="20"/>
-      <c r="C127" s="9" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A128" s="10" t="s">
-        <v>377</v>
-      </c>
-      <c r="B128" s="20"/>
-      <c r="C128" s="9" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A129" s="10" t="s">
-        <v>400</v>
-      </c>
-      <c r="B129" s="20"/>
-      <c r="C129" s="9" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A130" s="10" t="s">
-        <v>399</v>
-      </c>
-      <c r="B130" s="20"/>
-      <c r="C130" s="9" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A131" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="B131" s="20"/>
-      <c r="C131" s="9" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="132" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A132" s="10" t="s">
-        <v>396</v>
-      </c>
-      <c r="B132" s="20"/>
-      <c r="C132" s="9" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="133" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A133" s="10" t="s">
-        <v>397</v>
-      </c>
-      <c r="B133" s="20"/>
-      <c r="C133" s="9" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A134" s="10" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A135" s="10" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A136" s="10" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A137" s="10" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A138" s="10" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A139" s="10" t="s">
-        <v>453</v>
-      </c>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="20"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="20"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="20"/>
+    </row>
+    <row r="10" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="20"/>
+      <c r="C10"/>
+      <c r="D10"/>
+    </row>
+    <row r="11" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="20"/>
+      <c r="C11"/>
+      <c r="D11"/>
+    </row>
+    <row r="12" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="20"/>
+      <c r="C12"/>
+      <c r="D12"/>
+    </row>
+    <row r="13" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="20"/>
+      <c r="C13"/>
+      <c r="D13"/>
+    </row>
+    <row r="14" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="20"/>
+      <c r="C14"/>
+      <c r="D14"/>
+    </row>
+    <row r="15" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="20"/>
+      <c r="C15"/>
+      <c r="D15"/>
+    </row>
+    <row r="16" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="20"/>
+      <c r="C16"/>
+      <c r="D16"/>
+    </row>
+    <row r="17" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="20"/>
+      <c r="C17"/>
+      <c r="D17"/>
+    </row>
+    <row r="18" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="20"/>
+      <c r="C18"/>
+      <c r="D18"/>
+    </row>
+    <row r="19" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="20"/>
+      <c r="C19"/>
+      <c r="D19"/>
+    </row>
+    <row r="20" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+    </row>
+    <row r="21" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="20"/>
+      <c r="C21"/>
+      <c r="D21"/>
+    </row>
+    <row r="22" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="20"/>
+      <c r="C22"/>
+      <c r="D22"/>
+    </row>
+    <row r="23" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="20"/>
+      <c r="C23"/>
+      <c r="D23"/>
+    </row>
+    <row r="24" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="20"/>
+      <c r="C24"/>
+      <c r="D24"/>
+    </row>
+    <row r="25" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="20"/>
+      <c r="C25"/>
+      <c r="D25"/>
+    </row>
+    <row r="26" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="20"/>
+      <c r="C26"/>
+      <c r="D26"/>
+    </row>
+    <row r="27" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="20"/>
+      <c r="C27"/>
+      <c r="D27"/>
+    </row>
+    <row r="28" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="20"/>
+      <c r="C28"/>
+      <c r="D28"/>
+    </row>
+    <row r="29" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="20"/>
+      <c r="C29"/>
+      <c r="D29"/>
+    </row>
+    <row r="30" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="20"/>
+      <c r="C30"/>
+      <c r="D30"/>
+    </row>
+    <row r="31" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="20"/>
+      <c r="C31"/>
+      <c r="D31"/>
+    </row>
+    <row r="32" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="20"/>
+      <c r="C32"/>
+      <c r="D32"/>
+    </row>
+    <row r="33" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="20"/>
+      <c r="C33"/>
+      <c r="D33"/>
+    </row>
+    <row r="34" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="20"/>
+      <c r="C34"/>
+      <c r="D34"/>
+    </row>
+    <row r="35" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="20"/>
+      <c r="C35"/>
+      <c r="D35"/>
+    </row>
+    <row r="36" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="20"/>
+      <c r="C36"/>
+      <c r="D36"/>
+    </row>
+    <row r="37" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="20"/>
+      <c r="C37"/>
+      <c r="D37"/>
+    </row>
+    <row r="38" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="20"/>
+      <c r="C38"/>
+      <c r="D38"/>
+    </row>
+    <row r="39" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="20"/>
+      <c r="C39"/>
+      <c r="D39"/>
+    </row>
+    <row r="40" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="20"/>
+      <c r="C40"/>
+      <c r="D40"/>
+    </row>
+    <row r="41" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="20"/>
+      <c r="C41"/>
+      <c r="D41"/>
+    </row>
+    <row r="42" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="20"/>
+      <c r="C42"/>
+      <c r="D42"/>
+    </row>
+    <row r="43" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="20"/>
+      <c r="C43"/>
+      <c r="D43"/>
+    </row>
+    <row r="44" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="20"/>
+      <c r="C44"/>
+      <c r="D44"/>
+    </row>
+    <row r="45" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="20"/>
+      <c r="C45"/>
+      <c r="D45"/>
+    </row>
+    <row r="46" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="20"/>
+      <c r="C46"/>
+      <c r="D46"/>
+    </row>
+    <row r="47" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="20"/>
+      <c r="C47"/>
+      <c r="D47"/>
+    </row>
+    <row r="48" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="20"/>
+      <c r="C48"/>
+      <c r="D48"/>
+    </row>
+    <row r="49" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="20"/>
+      <c r="C49"/>
+      <c r="D49"/>
+    </row>
+    <row r="50" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="20"/>
+      <c r="C50"/>
+      <c r="D50"/>
+    </row>
+    <row r="51" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="20"/>
+      <c r="C51"/>
+      <c r="D51"/>
+    </row>
+    <row r="52" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="20"/>
+      <c r="C52"/>
+      <c r="D52"/>
+    </row>
+    <row r="53" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="20"/>
+      <c r="C53"/>
+      <c r="D53"/>
+    </row>
+    <row r="54" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="20"/>
+      <c r="C54"/>
+      <c r="D54"/>
+    </row>
+    <row r="55" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="20"/>
+      <c r="C55"/>
+      <c r="D55"/>
+    </row>
+    <row r="56" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="20"/>
+      <c r="C56"/>
+      <c r="D56"/>
+    </row>
+    <row r="57" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="20"/>
+      <c r="C57"/>
+      <c r="D57"/>
+    </row>
+    <row r="58" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="20"/>
+      <c r="C58"/>
+      <c r="D58"/>
+    </row>
+    <row r="59" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="20"/>
+      <c r="C59"/>
+      <c r="D59"/>
+    </row>
+    <row r="60" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="20"/>
+      <c r="C60"/>
+      <c r="D60"/>
+    </row>
+    <row r="61" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="20"/>
+      <c r="C61"/>
+      <c r="D61"/>
+    </row>
+    <row r="62" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="20"/>
+      <c r="C62"/>
+      <c r="D62"/>
+    </row>
+    <row r="63" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="20"/>
+      <c r="C63"/>
+      <c r="D63"/>
+    </row>
+    <row r="64" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="20"/>
+      <c r="C64"/>
+      <c r="D64"/>
+    </row>
+    <row r="65" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="20"/>
+      <c r="C65"/>
+      <c r="D65"/>
+    </row>
+    <row r="66" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="20"/>
+      <c r="C66"/>
+      <c r="D66"/>
+    </row>
+    <row r="67" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="20"/>
+      <c r="C67"/>
+      <c r="D67"/>
+    </row>
+    <row r="68" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="20"/>
+      <c r="C68"/>
+      <c r="D68"/>
+    </row>
+    <row r="69" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="20"/>
+      <c r="C69"/>
+      <c r="D69"/>
+    </row>
+    <row r="70" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="20"/>
+      <c r="C70"/>
+      <c r="D70"/>
+    </row>
+    <row r="71" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="20"/>
+      <c r="C71"/>
+      <c r="D71"/>
+    </row>
+    <row r="72" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="20"/>
+      <c r="C72"/>
+      <c r="D72"/>
+    </row>
+    <row r="73" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="20"/>
+      <c r="C73"/>
+      <c r="D73"/>
+    </row>
+    <row r="74" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="20"/>
+      <c r="C74"/>
+      <c r="D74"/>
+    </row>
+    <row r="75" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="20"/>
+      <c r="C75"/>
+      <c r="D75"/>
+    </row>
+    <row r="76" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="20"/>
+      <c r="C76"/>
+      <c r="D76"/>
+    </row>
+    <row r="77" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="20"/>
+      <c r="C77"/>
+      <c r="D77"/>
+    </row>
+    <row r="78" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="20"/>
+      <c r="C78"/>
+      <c r="D78"/>
+    </row>
+    <row r="79" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="20"/>
+      <c r="C79"/>
+      <c r="D79"/>
+    </row>
+    <row r="80" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="20"/>
+      <c r="C80"/>
+      <c r="D80"/>
+    </row>
+    <row r="81" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="20"/>
+      <c r="C81"/>
+      <c r="D81"/>
+    </row>
+    <row r="82" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="20"/>
+      <c r="C82"/>
+      <c r="D82"/>
+    </row>
+    <row r="83" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="20"/>
+      <c r="C83"/>
+      <c r="D83"/>
+    </row>
+    <row r="84" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="20"/>
+      <c r="C84"/>
+      <c r="D84"/>
+    </row>
+    <row r="85" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="20"/>
+      <c r="C85"/>
+      <c r="D85"/>
+    </row>
+    <row r="86" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="20"/>
+      <c r="C86"/>
+      <c r="D86"/>
+    </row>
+    <row r="87" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="20"/>
+      <c r="C87"/>
+      <c r="D87"/>
+    </row>
+    <row r="88" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="20"/>
+      <c r="C88"/>
+      <c r="D88"/>
+    </row>
+    <row r="89" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="20"/>
+      <c r="C89"/>
+      <c r="D89"/>
+    </row>
+    <row r="90" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="20"/>
+      <c r="C90"/>
+      <c r="D90"/>
+    </row>
+    <row r="91" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="20"/>
+      <c r="C91"/>
+      <c r="D91"/>
+    </row>
+    <row r="92" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="20"/>
+      <c r="C92"/>
+      <c r="D92"/>
+    </row>
+    <row r="93" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="20"/>
+      <c r="C93"/>
+      <c r="D93"/>
+    </row>
+    <row r="94" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="20"/>
+      <c r="C94"/>
+      <c r="D94"/>
+    </row>
+    <row r="95" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="3"/>
+      <c r="C95"/>
+      <c r="D95"/>
+    </row>
+    <row r="96" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="3"/>
+      <c r="C96"/>
+      <c r="D96"/>
+    </row>
+    <row r="97" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="3"/>
+      <c r="C97"/>
+      <c r="D97"/>
+    </row>
+    <row r="98" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="3"/>
+      <c r="C98"/>
+      <c r="D98"/>
+    </row>
+    <row r="99" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="3"/>
+      <c r="C99"/>
+      <c r="D99"/>
+    </row>
+    <row r="100" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="3"/>
+      <c r="C100"/>
+      <c r="D100"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -6557,11 +5867,2070 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F40359-1191-3843-B5C3-38D19A754655}">
+  <dimension ref="A1:F139"/>
+  <sheetViews>
+    <sheetView topLeftCell="A42" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="49.83203125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" style="41" customWidth="1"/>
+    <col min="6" max="6" width="81.33203125" style="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
+        <v>386</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>426</v>
+      </c>
+      <c r="C1" s="40" t="s">
+        <v>764</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="E1" s="40" t="s">
+        <v>765</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="20"/>
+      <c r="B2" s="11" t="s">
+        <v>602</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>477</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>601</v>
+      </c>
+      <c r="E2" s="41" t="s">
+        <v>477</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="20"/>
+      <c r="B3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="E3" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="B4" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="E4" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="B5" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="B6" s="10" t="s">
+        <v>325</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="E6" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="B7" s="10" t="s">
+        <v>326</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="E7" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="B8" s="10" t="s">
+        <v>327</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="E8" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="B9" s="10" t="s">
+        <v>328</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="E9" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="B10" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="B11" s="11" t="s">
+        <v>454</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>455</v>
+      </c>
+      <c r="E11" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="B12" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="E12" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="B13" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="E13" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="20"/>
+      <c r="B14" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="20"/>
+      <c r="B15" s="10" t="s">
+        <v>332</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="E15" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="20"/>
+      <c r="B16" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="E16" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="20"/>
+      <c r="B17" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="E17" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="20"/>
+      <c r="B18" s="10" t="s">
+        <v>335</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="E18" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="20"/>
+      <c r="B19" s="10" t="s">
+        <v>409</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="E19" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="20"/>
+      <c r="B20" s="10" t="s">
+        <v>410</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="E20" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="20"/>
+      <c r="B21" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="E21" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A22" s="20"/>
+      <c r="B22" s="10" t="s">
+        <v>411</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="E22" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A23" s="20"/>
+      <c r="B23" s="10" t="s">
+        <v>412</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="E23" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="20"/>
+      <c r="B24" s="10" t="s">
+        <v>413</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="E24" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="20"/>
+      <c r="B25" s="10" t="s">
+        <v>414</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="E25" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="20"/>
+      <c r="B26" s="10" t="s">
+        <v>415</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="E26" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="20"/>
+      <c r="B27" s="10" t="s">
+        <v>378</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="E27" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A28" s="20"/>
+      <c r="B28" s="10" t="s">
+        <v>379</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="E28" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A29" s="20"/>
+      <c r="B29" s="10" t="s">
+        <v>380</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="E29" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="20"/>
+      <c r="B30" s="10" t="s">
+        <v>381</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="E30" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="20"/>
+      <c r="B31" s="10" t="s">
+        <v>416</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="E31" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="20"/>
+      <c r="B32" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="E32" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="20"/>
+      <c r="B33" s="10" t="s">
+        <v>417</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="E33" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="20"/>
+      <c r="B34" s="10" t="s">
+        <v>418</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="E34" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="20"/>
+      <c r="B35" s="10" t="s">
+        <v>419</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="E35" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="20"/>
+      <c r="B36" s="10" t="s">
+        <v>336</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="E36" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A37" s="20"/>
+      <c r="B37" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="E37" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A38" s="20"/>
+      <c r="B38" s="10" t="s">
+        <v>421</v>
+      </c>
+      <c r="C38" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="E38" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A39" s="20"/>
+      <c r="B39" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="C39" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="E39" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A40" s="20"/>
+      <c r="B40" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="E40" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A41" s="20"/>
+      <c r="B41" s="10" t="s">
+        <v>339</v>
+      </c>
+      <c r="C41" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="E41" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A42" s="20"/>
+      <c r="B42" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="C42" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="E42" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A43" s="20"/>
+      <c r="B43" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="E43" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A44" s="20"/>
+      <c r="B44" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="E44" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A45" s="20"/>
+      <c r="B45" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="E45" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A46" s="20"/>
+      <c r="B46" s="10" t="s">
+        <v>423</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="E46" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A47" s="20"/>
+      <c r="B47" s="10" t="s">
+        <v>424</v>
+      </c>
+      <c r="C47" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="E47" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="17" x14ac:dyDescent="0.2">
+      <c r="A48" s="20"/>
+      <c r="B48" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="E48" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A49" s="20"/>
+      <c r="B49" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="E49" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A50" s="20"/>
+      <c r="B50" s="10" t="s">
+        <v>345</v>
+      </c>
+      <c r="C50" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="E50" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A51" s="20"/>
+      <c r="B51" s="10" t="s">
+        <v>346</v>
+      </c>
+      <c r="C51" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="E51" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A52" s="20"/>
+      <c r="B52" s="10" t="s">
+        <v>389</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="E52" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A53" s="20"/>
+      <c r="B53" s="10" t="s">
+        <v>425</v>
+      </c>
+      <c r="C53" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="E53" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A54" s="20"/>
+      <c r="B54" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="E54" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A55" s="20"/>
+      <c r="B55" s="10" t="s">
+        <v>348</v>
+      </c>
+      <c r="C55" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="E55" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A56" s="20"/>
+      <c r="B56" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="C56" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="E56" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A57" s="20"/>
+      <c r="B57" s="10" t="s">
+        <v>427</v>
+      </c>
+      <c r="C57" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D57" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="E57" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A58" s="20"/>
+      <c r="B58" s="10" t="s">
+        <v>428</v>
+      </c>
+      <c r="C58" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="E58" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A59" s="20"/>
+      <c r="B59" s="10" t="s">
+        <v>429</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="E59" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A60" s="20"/>
+      <c r="B60" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="E60" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A61" s="20"/>
+      <c r="B61" s="10" t="s">
+        <v>430</v>
+      </c>
+      <c r="C61" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="E61" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A62" s="20"/>
+      <c r="B62" s="10" t="s">
+        <v>431</v>
+      </c>
+      <c r="C62" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>249</v>
+      </c>
+      <c r="E62" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A63" s="20"/>
+      <c r="B63" s="10" t="s">
+        <v>432</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="E63" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A64" s="20"/>
+      <c r="B64" s="10" t="s">
+        <v>382</v>
+      </c>
+      <c r="C64" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="E64" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A65" s="20"/>
+      <c r="B65" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="C65" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="E65" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A66" s="20"/>
+      <c r="B66" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="C66" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>253</v>
+      </c>
+      <c r="E66" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A67" s="20"/>
+      <c r="B67" s="10" t="s">
+        <v>352</v>
+      </c>
+      <c r="C67" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="E67" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A68" s="20"/>
+      <c r="B68" s="10" t="s">
+        <v>353</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D68" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="E68" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A69" s="20"/>
+      <c r="B69" s="10" t="s">
+        <v>433</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D69" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="E69" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A70" s="20"/>
+      <c r="B70" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="E70" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A71" s="20"/>
+      <c r="B71" s="10" t="s">
+        <v>354</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="E71" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A72" s="20"/>
+      <c r="B72" s="10" t="s">
+        <v>355</v>
+      </c>
+      <c r="C72" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="E72" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A73" s="20"/>
+      <c r="B73" s="10" t="s">
+        <v>356</v>
+      </c>
+      <c r="C73" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D73" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="E73" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A74" s="20"/>
+      <c r="B74" s="10" t="s">
+        <v>357</v>
+      </c>
+      <c r="C74" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D74" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="E74" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A75" s="20"/>
+      <c r="B75" s="10" t="s">
+        <v>358</v>
+      </c>
+      <c r="C75" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D75" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="E75" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A76" s="20"/>
+      <c r="B76" s="10" t="s">
+        <v>359</v>
+      </c>
+      <c r="C76" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D76" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="E76" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A77" s="20"/>
+      <c r="B77" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="C77" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D77" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="E77" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A78" s="20"/>
+      <c r="B78" s="10" t="s">
+        <v>361</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D78" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="E78" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A79" s="20"/>
+      <c r="B79" s="10" t="s">
+        <v>362</v>
+      </c>
+      <c r="C79" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D79" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="E79" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A80" s="20"/>
+      <c r="B80" s="10" t="s">
+        <v>434</v>
+      </c>
+      <c r="C80" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D80" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="E80" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A81" s="20"/>
+      <c r="B81" s="10" t="s">
+        <v>363</v>
+      </c>
+      <c r="C81" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D81" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="E81" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A82" s="20"/>
+      <c r="B82" s="10" t="s">
+        <v>364</v>
+      </c>
+      <c r="C82" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D82" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="E82" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A83" s="20"/>
+      <c r="B83" s="10" t="s">
+        <v>435</v>
+      </c>
+      <c r="C83" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D83" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="E83" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A84" s="20"/>
+      <c r="B84" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="C84" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D84" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="E84" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A85" s="20"/>
+      <c r="B85" s="10" t="s">
+        <v>366</v>
+      </c>
+      <c r="C85" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D85" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="E85" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A86" s="20"/>
+      <c r="B86" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="C86" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D86" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="E86" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A87" s="20"/>
+      <c r="B87" s="10" t="s">
+        <v>368</v>
+      </c>
+      <c r="C87" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D87" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="E87" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A88" s="20"/>
+      <c r="B88" s="10" t="s">
+        <v>369</v>
+      </c>
+      <c r="C88" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D88" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="E88" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A89" s="20"/>
+      <c r="B89" s="10" t="s">
+        <v>436</v>
+      </c>
+      <c r="C89" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D89" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="E89" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A90" s="20"/>
+      <c r="B90" s="10" t="s">
+        <v>437</v>
+      </c>
+      <c r="C90" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D90" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="E90" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A91" s="20"/>
+      <c r="B91" s="10" t="s">
+        <v>438</v>
+      </c>
+      <c r="C91" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D91" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="E91" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A92" s="20"/>
+      <c r="B92" s="10" t="s">
+        <v>430</v>
+      </c>
+      <c r="C92" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D92" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="E92" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A93" s="20"/>
+      <c r="B93" s="10" t="s">
+        <v>384</v>
+      </c>
+      <c r="C93" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D93" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="E93" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A94" s="20"/>
+      <c r="B94" s="10" t="s">
+        <v>391</v>
+      </c>
+      <c r="C94" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D94" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="E94" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A95" s="20"/>
+      <c r="B95" s="10" t="s">
+        <v>439</v>
+      </c>
+      <c r="C95" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D95" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="E95" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A96" s="20"/>
+      <c r="B96" s="10" t="s">
+        <v>440</v>
+      </c>
+      <c r="C96" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D96" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="E96" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A97" s="20"/>
+      <c r="B97" s="10" t="s">
+        <v>370</v>
+      </c>
+      <c r="C97" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D97" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="E97" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A98" s="20"/>
+      <c r="B98" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D98" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="E98" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A99" s="20"/>
+      <c r="B99" s="10" t="s">
+        <v>372</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D99" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="E99" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A100" s="20"/>
+      <c r="B100" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="C100" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D100" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="E100" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A101" s="20"/>
+      <c r="B101" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="C101" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D101" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="E101" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A102" s="20"/>
+      <c r="B102" s="10" t="s">
+        <v>441</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D102" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="E102" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A103" s="20"/>
+      <c r="B103" s="10" t="s">
+        <v>442</v>
+      </c>
+      <c r="C103" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D103" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="E103" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A104" s="20"/>
+      <c r="B104" s="10" t="s">
+        <v>443</v>
+      </c>
+      <c r="C104" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D104" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="E104" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A105" s="20"/>
+      <c r="B105" s="10" t="s">
+        <v>444</v>
+      </c>
+      <c r="C105" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D105" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E105" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A106" s="20"/>
+      <c r="B106" s="10" t="s">
+        <v>445</v>
+      </c>
+      <c r="C106" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D106" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="E106" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A107" s="20"/>
+      <c r="B107" s="10" t="s">
+        <v>446</v>
+      </c>
+      <c r="C107" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D107" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="E107" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A108" s="20"/>
+      <c r="B108" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="C108" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D108" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="E108" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A109" s="20"/>
+      <c r="B109" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="C109" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D109" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="E109" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A110" s="20"/>
+      <c r="B110" s="10" t="s">
+        <v>448</v>
+      </c>
+      <c r="C110" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D110" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="E110" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A111" s="20"/>
+      <c r="B111" s="10" t="s">
+        <v>449</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D111" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="E111" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A112" s="20"/>
+      <c r="B112" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="C112" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D112" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="E112" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A113" s="20"/>
+      <c r="B113" s="10" t="s">
+        <v>451</v>
+      </c>
+      <c r="C113" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D113" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="E113" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A114" s="20"/>
+      <c r="B114" s="10" t="s">
+        <v>452</v>
+      </c>
+      <c r="C114" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D114" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="E114" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A115" s="20"/>
+      <c r="B115" s="10" t="s">
+        <v>393</v>
+      </c>
+      <c r="C115" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D115" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="E115" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A116" s="20"/>
+      <c r="B116" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="C116" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D116" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="E116" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A117" s="20"/>
+      <c r="B117" s="10" t="s">
+        <v>407</v>
+      </c>
+      <c r="C117" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D117" s="9" t="s">
+        <v>304</v>
+      </c>
+      <c r="E117" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A118" s="20"/>
+      <c r="B118" s="10" t="s">
+        <v>406</v>
+      </c>
+      <c r="C118" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D118" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="E118" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A119" s="20"/>
+      <c r="B119" s="10" t="s">
+        <v>394</v>
+      </c>
+      <c r="C119" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D119" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="E119" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A120" s="20"/>
+      <c r="B120" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="C120" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D120" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="E120" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A121" s="20"/>
+      <c r="B121" s="10" t="s">
+        <v>404</v>
+      </c>
+      <c r="C121" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D121" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="E121" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A122" s="20"/>
+      <c r="B122" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="C122" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D122" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="E122" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A123" s="20"/>
+      <c r="B123" s="10" t="s">
+        <v>402</v>
+      </c>
+      <c r="C123" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D123" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="E123" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A124" s="20"/>
+      <c r="B124" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="C124" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D124" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="E124" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A125" s="20"/>
+      <c r="B125" s="10" t="s">
+        <v>401</v>
+      </c>
+      <c r="C125" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D125" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="E125" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A126" s="20"/>
+      <c r="B126" s="10" t="s">
+        <v>375</v>
+      </c>
+      <c r="C126" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D126" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="E126" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A127" s="20"/>
+      <c r="B127" s="10" t="s">
+        <v>376</v>
+      </c>
+      <c r="C127" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D127" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="E127" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A128" s="20"/>
+      <c r="B128" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="C128" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D128" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="E128" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A129" s="20"/>
+      <c r="B129" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="C129" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D129" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="E129" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A130" s="20"/>
+      <c r="B130" s="10" t="s">
+        <v>399</v>
+      </c>
+      <c r="C130" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D130" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="E130" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A131" s="20"/>
+      <c r="B131" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="C131" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D131" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="E131" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A132" s="20"/>
+      <c r="B132" s="10" t="s">
+        <v>396</v>
+      </c>
+      <c r="C132" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D132" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="E132" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="17" x14ac:dyDescent="0.2">
+      <c r="A133" s="20"/>
+      <c r="B133" s="10" t="s">
+        <v>397</v>
+      </c>
+      <c r="C133" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D133" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="E133" s="41" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B134" s="10" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B135" s="10" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B136" s="10" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B137" s="10" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B138" s="10" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B139" s="10" t="s">
+        <v>453</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1886B59F-3C17-014D-9C61-BEC33F421A82}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6585,12 +7954,20 @@
         <v>103</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="16" t="s">
+        <v>767</v>
+      </c>
+      <c r="B3" t="s">
+        <v>768</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6CCACBD-9050-2546-A791-CCDEA21B15F7}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -6890,34 +8267,34 @@
       <c r="A3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="37" t="s">
         <v>128</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="13" t="s">
@@ -7070,11 +8447,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B7:E7"/>
     <mergeCell ref="B12:E12"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="B8:E8"/>
@@ -7083,6 +8455,11 @@
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Update for CrriterionItems DDF-RA #430
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/full_1.xlsx
+++ b/tests/integration_test_files/full_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CEECB6C-D9D9-E749-BEDD-46731B182F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28AF17EA-D8AD-3845-9037-7A0DCE87F545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51500" yWindow="500" windowWidth="49340" windowHeight="27480" activeTab="5" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="340" yWindow="500" windowWidth="49340" windowHeight="27260" firstSheet="7" activeTab="10" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1456" uniqueCount="778">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1457" uniqueCount="781">
   <si>
     <t>Screening</t>
   </si>
@@ -2396,6 +2396,15 @@
   </si>
   <si>
     <t>trialSubTypes</t>
+  </si>
+  <si>
+    <t>18 .. 70 years</t>
+  </si>
+  <si>
+    <t>@plannedAge/Range/@maxValue/Quantity/@value</t>
+  </si>
+  <si>
+    <t>@plannedAge/Range/@minValue/Quantity/@value</t>
   </si>
 </sst>
 </file>
@@ -3291,8 +3300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EB40753-8F7D-3941-9F21-F336F33F75CC}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3302,7 +3311,7 @@
     <col min="3" max="4" width="18.83203125" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="31.83203125" customWidth="1"/>
+    <col min="7" max="7" width="51.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -3350,8 +3359,8 @@
       <c r="F2" t="s">
         <v>493</v>
       </c>
-      <c r="G2" t="s">
-        <v>692</v>
+      <c r="G2" s="5" t="s">
+        <v>780</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -3364,8 +3373,8 @@
       <c r="F3" t="s">
         <v>493</v>
       </c>
-      <c r="G3" t="s">
-        <v>692</v>
+      <c r="G3" s="5" t="s">
+        <v>779</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -3387,8 +3396,8 @@
       <c r="F4" t="s">
         <v>493</v>
       </c>
-      <c r="G4" t="s">
-        <v>692</v>
+      <c r="G4" s="5" t="s">
+        <v>780</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -4443,7 +4452,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4499,6 +4508,9 @@
       </c>
       <c r="F2">
         <v>120</v>
+      </c>
+      <c r="G2" t="s">
+        <v>778</v>
       </c>
       <c r="H2" t="s">
         <v>42</v>
@@ -5668,7 +5680,7 @@
   <dimension ref="A1:D86"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9017,7 +9029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{679CED36-1B68-6F40-B862-B156999A55CA}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -9265,6 +9277,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
@@ -9276,11 +9293,6 @@
     <mergeCell ref="B5:E5"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Cohort to Indication link, DDF-RA #467
</commit_message>
<xml_diff>
--- a/tests/integration_test_files/full_1.xlsx
+++ b/tests/integration_test_files/full_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveih/Documents/python/usdm/tests/integration_test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28AF17EA-D8AD-3845-9037-7A0DCE87F545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200BFFFF-8FB8-664D-A18A-5DACF9069955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="500" windowWidth="49340" windowHeight="27260" firstSheet="7" activeTab="10" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
+    <workbookView xWindow="340" yWindow="500" windowWidth="49340" windowHeight="27260" firstSheet="7" activeTab="17" xr2:uid="{36865AF5-732C-8F40-95E5-FB8DDE1499F2}"/>
   </bookViews>
   <sheets>
     <sheet name="study" sheetId="2" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1457" uniqueCount="781">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1460" uniqueCount="782">
   <si>
     <t>Screening</t>
   </si>
@@ -2405,6 +2405,9 @@
   </si>
   <si>
     <t>@plannedAge/Range/@minValue/Quantity/@value</t>
+  </si>
+  <si>
+    <t>indications</t>
   </si>
 </sst>
 </file>
@@ -3300,7 +3303,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EB40753-8F7D-3941-9F21-F336F33F75CC}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -4449,10 +4452,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C037A932-CB5B-8D43-956E-5F5C367E07FC}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4467,7 +4470,7 @@
     <col min="9" max="9" width="23.33203125" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>679</v>
       </c>
@@ -4495,8 +4498,11 @@
       <c r="I1" s="32" t="s">
         <v>695</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" s="15" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>682</v>
       </c>
@@ -4519,7 +4525,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>683</v>
       </c>
@@ -4532,8 +4538,11 @@
       <c r="I3" s="6" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>683</v>
       </c>
@@ -4545,6 +4554,9 @@
       </c>
       <c r="I4" s="6" t="s">
         <v>121</v>
+      </c>
+      <c r="J4" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>